<commit_message>
minor update but still missing info
Former-commit-id: 9a14e1035fdf141d1dab4c39ded539853d3a935b
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -1332,10 +1332,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$101</c:f>
+              <c:f>Data!$C$2:$C$401</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="400"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -1635,16 +1635,76 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>43408</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>43410</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>43411</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>43412</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>43413</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>43414</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>43415</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>43417</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>43418</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>43419</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>43420</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>43421</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>43422</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>43423</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>43424</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>43425</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>43427</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>43428</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>43429</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>43430</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>43431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$101</c:f>
+              <c:f>Data!$M$2:$M$401</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="100"/>
+                <c:ptCount val="400"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -1944,6 +2004,39 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>5.25</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>1.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8245,7 +8338,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z121"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="AA40" sqref="AA40"/>
     </sheetView>
   </sheetViews>
@@ -14182,7 +14275,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
@@ -14392,7 +14485,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Partial Update - Needs more info from Laurel
Former-commit-id: 8eeb92ce2a8775c16c803f71fde89e379665b3e5
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aNDREW\Desktop\ice-skating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB6823E-0D0F-4257-8086-80F78E9F2D1E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426E34E9-9C66-4B1A-AA11-7A532A778B52}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="323">
   <si>
     <t>Thursday</t>
   </si>
@@ -1039,6 +1038,33 @@
   </si>
   <si>
     <t>Private, FSI, Public</t>
+  </si>
+  <si>
+    <t>Larry Group lesson and stroking. Worked on sitspin with hockey stick on back. Learned how to do loop patterns and how to switch from BI to FO while in a spin</t>
+  </si>
+  <si>
+    <t>Fixed Entry Edge to Waltz jump. Sit spin getting lower. Getting closer on axel. Ankle pain on both ankles. Worked on jump combos. Worked on walleys and FS4 manuevers</t>
+  </si>
+  <si>
+    <t>Low confidence day. Lesson with visiting lady. Worked on camel spins. Could not do them. Feeling much more in control of sit spin. Able to turn foot out and adjust posture while in the spin.</t>
+  </si>
+  <si>
+    <t>FS5, Stroking, FS3/FS4, Private</t>
+  </si>
+  <si>
+    <t>Worked on split jumps and half loops. Ankles hurt. Glute and lower back hurt. Got skates sharpened last night. Private with Laurel on basics. Went over three turns and mohawks. Sit spins</t>
+  </si>
+  <si>
+    <t>Sprained ankle last night at jump jam, but it doesn't hurt when I skate. Worked on jump combos with Laurel. Skipped lessons this morning because Larry was teaching them and my ankle was hurting. Did basic stroking with Laurel. Noticed Inadequacy holding certain edges. Worked on basics in my private. Learned more about properly executing three turns and learned more about entry edges.</t>
+  </si>
+  <si>
+    <t>Worked on sitspin until glute pain in left leg became too intense. Got confirmation that new skates are ordered.</t>
+  </si>
+  <si>
+    <t>Worked on sit spins with Laurel. One foot spins are getting crazy good.</t>
+  </si>
+  <si>
+    <t>Ober skating with Laurel. Played add-on and getting good with half loops.</t>
   </si>
 </sst>
 </file>
@@ -1432,10 +1458,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$388</c:f>
+              <c:f>Data!$C$2:$C$391</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="387"/>
+                <c:ptCount val="390"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -1843,16 +1869,70 @@
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>43460</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>43461</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>43462</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>43463</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>43464</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>43465</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>43467</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>43468</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>43469</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43470</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43471</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>43472</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43473</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43474</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43475</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>43476</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>43477</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>43478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$388</c:f>
+              <c:f>Data!$M$2:$M$391</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="387"/>
+                <c:ptCount val="390"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2259,6 +2339,24 @@
                   <c:v>6.75</c:v>
                 </c:pt>
                 <c:pt idx="135">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="153">
                   <c:v>2.25</c:v>
                 </c:pt>
               </c:numCache>
@@ -2562,10 +2660,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$388</c:f>
+              <c:f>Data!$C$2:$C$391</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="387"/>
+                <c:ptCount val="390"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -2973,16 +3071,70 @@
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>43460</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>43461</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>43462</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>43463</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>43464</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>43465</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>43467</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>43468</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>43469</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43470</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43471</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>43472</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43473</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43474</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43475</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>43476</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>43477</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>43478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$388</c:f>
+              <c:f>Data!$Q$2:$Q$391</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="387"/>
+                <c:ptCount val="390"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3389,6 +3541,60 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="135">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="153">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -3802,7 +4008,7 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>60.5</c:v>
+                  <c:v>75.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4187,7 +4393,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4476,10 +4682,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$388</c:f>
+              <c:f>Data!$C$2:$C$391</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="387"/>
+                <c:ptCount val="390"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -4887,16 +5093,70 @@
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>43460</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>43461</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>43462</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>43463</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>43464</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>43465</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>43466</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>43467</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>43468</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>43469</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>43470</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>43471</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>43472</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>43473</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>43474</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>43475</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>43476</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>43477</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>43478</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$T$2:$T$388</c:f>
+              <c:f>Data!$T$2:$T$391</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="387"/>
+                <c:ptCount val="390"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -5304,6 +5564,60 @@
                 </c:pt>
                 <c:pt idx="135">
                   <c:v>363.45</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>365.7</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>367.7</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>367.7</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>369.7</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>373.95</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>376.2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>378.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8743,10 +9057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z137"/>
+  <dimension ref="A1:Z155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="H150" sqref="H150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8757,10 +9071,10 @@
     <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="2" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" style="3" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" style="2" customWidth="1"/>
+    <col min="10" max="11" width="11.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.7109375" style="4" customWidth="1"/>
     <col min="14" max="14" width="25.85546875" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
@@ -8928,11 +9242,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M:M)</f>
-        <v>363.45</v>
+        <v>378.45</v>
       </c>
       <c r="V3" s="4">
-        <f>SUM(M19:M387)</f>
-        <v>321.7</v>
+        <f>SUM(M19:M390)</f>
+        <v>336.7</v>
       </c>
       <c r="W3" s="4">
         <f>SUM(M2:M18)</f>
@@ -9744,12 +10058,12 @@
         <v>294</v>
       </c>
       <c r="W19" s="4">
-        <f>SUM(M117:M387)</f>
-        <v>60.5</v>
+        <f>SUM(M117:M390)</f>
+        <v>75.5</v>
       </c>
       <c r="X19">
         <f>COUNTIF(P:P, "Freestyle 4")</f>
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="Y19" s="14">
         <f>C137-C117+1</f>
@@ -9757,7 +10071,7 @@
       </c>
       <c r="Z19" s="14">
         <f>Y19-X19</f>
-        <v>11</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -9963,16 +10277,16 @@
         <v>284</v>
       </c>
       <c r="W23" s="4">
-        <f>SUM(M100:M387)</f>
-        <v>113.5</v>
+        <f>SUM(M100:M390)</f>
+        <v>128.5</v>
       </c>
       <c r="X23">
         <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="Y23" s="14">
         <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="Z23" s="14">
         <f>Y23-X23</f>
@@ -10059,7 +10373,7 @@
       </c>
       <c r="Z25">
         <f>SUM(Z11:Z19)</f>
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -13340,7 +13654,7 @@
         <v>43403</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" ref="C96:C137" si="8">B96</f>
+        <f t="shared" ref="C96:C155" si="8">B96</f>
         <v>43403</v>
       </c>
       <c r="D96" s="3">
@@ -15098,7 +15412,7 @@
         <v>3</v>
       </c>
       <c r="T131" s="4">
-        <f t="shared" ref="T131:T137" si="17">T130+M131</f>
+        <f t="shared" ref="T131:T155" si="17">T130+M131</f>
         <v>344.95</v>
       </c>
     </row>
@@ -15255,7 +15569,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F135" s="2">
-        <f t="shared" ref="F135:F137" si="19">E135-D135</f>
+        <f t="shared" ref="F135:F155" si="19">E135-D135</f>
         <v>0.125</v>
       </c>
       <c r="G135" s="3">
@@ -15408,8 +15722,702 @@
         <v>363.45</v>
       </c>
     </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>0</v>
+      </c>
+      <c r="B138" s="1">
+        <v>43461</v>
+      </c>
+      <c r="C138" s="5">
+        <f t="shared" si="8"/>
+        <v>43461</v>
+      </c>
+      <c r="D138" s="3">
+        <v>0.34375</v>
+      </c>
+      <c r="E138" s="3">
+        <v>0.4375</v>
+      </c>
+      <c r="F138" s="2">
+        <f t="shared" si="19"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M138" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="N138" t="s">
+        <v>316</v>
+      </c>
+      <c r="O138" t="s">
+        <v>317</v>
+      </c>
+      <c r="P138" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q138">
+        <v>8</v>
+      </c>
+      <c r="R138" t="s">
+        <v>284</v>
+      </c>
+      <c r="S138">
+        <v>3</v>
+      </c>
+      <c r="T138" s="4">
+        <f t="shared" si="17"/>
+        <v>365.7</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>1</v>
+      </c>
+      <c r="B139" s="1">
+        <v>43462</v>
+      </c>
+      <c r="C139" s="5">
+        <f t="shared" si="8"/>
+        <v>43462</v>
+      </c>
+      <c r="D139" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E139" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="F139" s="2">
+        <f t="shared" si="19"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G139" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="H139" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I139" s="2">
+        <f>H139-G139</f>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="M139" s="4">
+        <v>2</v>
+      </c>
+      <c r="N139" t="s">
+        <v>318</v>
+      </c>
+      <c r="P139" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q139">
+        <v>8</v>
+      </c>
+      <c r="R139" t="s">
+        <v>284</v>
+      </c>
+      <c r="S139">
+        <v>3</v>
+      </c>
+      <c r="T139" s="4">
+        <f t="shared" si="17"/>
+        <v>367.7</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>2</v>
+      </c>
+      <c r="B140" s="1">
+        <v>43463</v>
+      </c>
+      <c r="C140" s="5">
+        <f t="shared" si="8"/>
+        <v>43463</v>
+      </c>
+      <c r="D140" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="F140" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.52083333333333337</v>
+      </c>
+      <c r="N140" t="s">
+        <v>319</v>
+      </c>
+      <c r="P140" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q140">
+        <v>8</v>
+      </c>
+      <c r="R140" t="s">
+        <v>284</v>
+      </c>
+      <c r="S140">
+        <v>3</v>
+      </c>
+      <c r="T140" s="4">
+        <f t="shared" si="17"/>
+        <v>367.7</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>3</v>
+      </c>
+      <c r="B141" s="1">
+        <v>43464</v>
+      </c>
+      <c r="C141" s="5">
+        <f t="shared" si="8"/>
+        <v>43464</v>
+      </c>
+      <c r="D141" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E141" s="3">
+        <v>0.75</v>
+      </c>
+      <c r="F141" s="2">
+        <f t="shared" si="19"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="M141" s="4">
+        <v>2</v>
+      </c>
+      <c r="N141" t="s">
+        <v>315</v>
+      </c>
+      <c r="P141" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q141">
+        <v>8</v>
+      </c>
+      <c r="R141" t="s">
+        <v>284</v>
+      </c>
+      <c r="S141">
+        <v>3</v>
+      </c>
+      <c r="T141" s="4">
+        <f t="shared" si="17"/>
+        <v>369.7</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>10</v>
+      </c>
+      <c r="B142" s="1">
+        <v>43465</v>
+      </c>
+      <c r="C142" s="5">
+        <f t="shared" si="8"/>
+        <v>43465</v>
+      </c>
+      <c r="D142" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E142" s="3">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="F142" s="2">
+        <f t="shared" si="19"/>
+        <v>0.17708333333333331</v>
+      </c>
+      <c r="M142" s="4">
+        <v>4.25</v>
+      </c>
+      <c r="N142" t="s">
+        <v>314</v>
+      </c>
+      <c r="P142" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q142">
+        <v>8</v>
+      </c>
+      <c r="R142" t="s">
+        <v>284</v>
+      </c>
+      <c r="S142">
+        <v>3</v>
+      </c>
+      <c r="T142" s="4">
+        <f t="shared" si="17"/>
+        <v>373.95</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>69</v>
+      </c>
+      <c r="B143" s="1">
+        <v>43466</v>
+      </c>
+      <c r="C143" s="5">
+        <f t="shared" si="8"/>
+        <v>43466</v>
+      </c>
+      <c r="D143" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E143" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F143" s="2">
+        <f t="shared" si="19"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M143" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="N143" t="s">
+        <v>320</v>
+      </c>
+      <c r="P143" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q143">
+        <v>8</v>
+      </c>
+      <c r="R143" t="s">
+        <v>284</v>
+      </c>
+      <c r="S143">
+        <v>3</v>
+      </c>
+      <c r="T143" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>35</v>
+      </c>
+      <c r="B144" s="1">
+        <v>43467</v>
+      </c>
+      <c r="C144" s="5">
+        <f t="shared" si="8"/>
+        <v>43467</v>
+      </c>
+      <c r="F144" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P144" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q144">
+        <v>8</v>
+      </c>
+      <c r="R144" t="s">
+        <v>284</v>
+      </c>
+      <c r="S144">
+        <v>3</v>
+      </c>
+      <c r="T144" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B145" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C145" s="5">
+        <f t="shared" si="8"/>
+        <v>43468</v>
+      </c>
+      <c r="F145" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P145" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q145">
+        <v>8</v>
+      </c>
+      <c r="R145" t="s">
+        <v>284</v>
+      </c>
+      <c r="S145">
+        <v>3</v>
+      </c>
+      <c r="T145" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>1</v>
+      </c>
+      <c r="B146" s="1">
+        <v>43469</v>
+      </c>
+      <c r="C146" s="5">
+        <f t="shared" si="8"/>
+        <v>43469</v>
+      </c>
+      <c r="F146" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P146" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q146">
+        <v>8</v>
+      </c>
+      <c r="R146" t="s">
+        <v>284</v>
+      </c>
+      <c r="S146">
+        <v>3</v>
+      </c>
+      <c r="T146" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>2</v>
+      </c>
+      <c r="B147" s="1">
+        <v>43470</v>
+      </c>
+      <c r="C147" s="5">
+        <f t="shared" si="8"/>
+        <v>43470</v>
+      </c>
+      <c r="F147" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P147" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q147">
+        <v>8</v>
+      </c>
+      <c r="R147" t="s">
+        <v>284</v>
+      </c>
+      <c r="S147">
+        <v>3</v>
+      </c>
+      <c r="T147" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>3</v>
+      </c>
+      <c r="B148" s="1">
+        <v>43471</v>
+      </c>
+      <c r="C148" s="5">
+        <f t="shared" si="8"/>
+        <v>43471</v>
+      </c>
+      <c r="D148" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E148" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="F148" s="2">
+        <f t="shared" si="19"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G148" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="N148" t="s">
+        <v>321</v>
+      </c>
+      <c r="P148" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q148">
+        <v>8</v>
+      </c>
+      <c r="R148" t="s">
+        <v>284</v>
+      </c>
+      <c r="S148">
+        <v>3</v>
+      </c>
+      <c r="T148" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>10</v>
+      </c>
+      <c r="B149" s="1">
+        <v>43472</v>
+      </c>
+      <c r="C149" s="5">
+        <f t="shared" si="8"/>
+        <v>43472</v>
+      </c>
+      <c r="D149" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F149" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.72916666666666663</v>
+      </c>
+      <c r="P149" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q149">
+        <v>8</v>
+      </c>
+      <c r="R149" t="s">
+        <v>284</v>
+      </c>
+      <c r="S149">
+        <v>3</v>
+      </c>
+      <c r="T149" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>69</v>
+      </c>
+      <c r="B150" s="1">
+        <v>43473</v>
+      </c>
+      <c r="C150" s="5">
+        <f t="shared" si="8"/>
+        <v>43473</v>
+      </c>
+      <c r="F150" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P150" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q150">
+        <v>8</v>
+      </c>
+      <c r="R150" t="s">
+        <v>284</v>
+      </c>
+      <c r="S150">
+        <v>3</v>
+      </c>
+      <c r="T150" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>35</v>
+      </c>
+      <c r="B151" s="1">
+        <v>43474</v>
+      </c>
+      <c r="C151" s="5">
+        <f t="shared" si="8"/>
+        <v>43474</v>
+      </c>
+      <c r="D151" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F151" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.69791666666666663</v>
+      </c>
+      <c r="P151" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q151">
+        <v>8</v>
+      </c>
+      <c r="R151" t="s">
+        <v>284</v>
+      </c>
+      <c r="S151">
+        <v>3</v>
+      </c>
+      <c r="T151" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>0</v>
+      </c>
+      <c r="B152" s="1">
+        <v>43475</v>
+      </c>
+      <c r="C152" s="5">
+        <f t="shared" si="8"/>
+        <v>43475</v>
+      </c>
+      <c r="D152" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F152" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.69791666666666663</v>
+      </c>
+      <c r="P152" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q152">
+        <v>8</v>
+      </c>
+      <c r="R152" t="s">
+        <v>284</v>
+      </c>
+      <c r="S152">
+        <v>3</v>
+      </c>
+      <c r="T152" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>1</v>
+      </c>
+      <c r="B153" s="1">
+        <v>43476</v>
+      </c>
+      <c r="C153" s="5">
+        <f t="shared" si="8"/>
+        <v>43476</v>
+      </c>
+      <c r="D153" s="3">
+        <v>0.78125</v>
+      </c>
+      <c r="F153" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.78125</v>
+      </c>
+      <c r="P153" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q153">
+        <v>8</v>
+      </c>
+      <c r="R153" t="s">
+        <v>284</v>
+      </c>
+      <c r="S153">
+        <v>3</v>
+      </c>
+      <c r="T153" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>2</v>
+      </c>
+      <c r="B154" s="1">
+        <v>43477</v>
+      </c>
+      <c r="C154" s="5">
+        <f t="shared" si="8"/>
+        <v>43477</v>
+      </c>
+      <c r="D154" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F154" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.73958333333333337</v>
+      </c>
+      <c r="P154" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q154">
+        <v>8</v>
+      </c>
+      <c r="R154" t="s">
+        <v>284</v>
+      </c>
+      <c r="S154">
+        <v>3</v>
+      </c>
+      <c r="T154" s="4">
+        <f t="shared" si="17"/>
+        <v>376.2</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>3</v>
+      </c>
+      <c r="B155" s="1">
+        <v>43478</v>
+      </c>
+      <c r="C155" s="5">
+        <f t="shared" si="8"/>
+        <v>43478</v>
+      </c>
+      <c r="D155" s="3">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E155" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F155" s="2">
+        <f t="shared" si="19"/>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M155" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="N155" t="s">
+        <v>322</v>
+      </c>
+      <c r="P155" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q155">
+        <v>8</v>
+      </c>
+      <c r="R155" t="s">
+        <v>284</v>
+      </c>
+      <c r="S155">
+        <v>3</v>
+      </c>
+      <c r="T155" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A138:T528 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T531">
     <cfRule type="expression" dxfId="17" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>

</xml_diff>

<commit_message>
SORT OF UPDATED TO 2/8
NEED LAUREL

Former-commit-id: a33c09c4345d56b2597fb1777db24419fc186738
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B312D251-2B42-41CD-8120-CD126F99EBEA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A51F9B88-EED4-420B-8ED3-9C5BD14DFE5D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="897" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="929" uniqueCount="333">
   <si>
     <t>Thursday</t>
   </si>
@@ -1103,6 +1102,21 @@
       </rPr>
       <t>):</t>
     </r>
+  </si>
+  <si>
+    <t>Morning Pairs with Laurel. Worked on couples Spotlight. Blister pain</t>
+  </si>
+  <si>
+    <t>Early Bird</t>
+  </si>
+  <si>
+    <t>FS4 class with Devon. FS5 class with devon. Landed 'chicken' axels. Went to show Laurel and landed my first axel. Fully rotated and checked exit.</t>
+  </si>
+  <si>
+    <t>Stroking, FS3/FS4, FS5</t>
+  </si>
+  <si>
+    <t>Axel Lesson with Devon. Greatest Showman Practice.</t>
   </si>
 </sst>
 </file>
@@ -1992,6 +2006,33 @@
                 <c:pt idx="163">
                   <c:v>43495</c:v>
                 </c:pt>
+                <c:pt idx="164">
+                  <c:v>43496</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>43498</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>43499</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>43500</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>43501</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>43502</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>43503</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>43504</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3224,6 +3265,33 @@
                 <c:pt idx="163">
                   <c:v>43495</c:v>
                 </c:pt>
+                <c:pt idx="164">
+                  <c:v>43496</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>43498</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>43499</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>43500</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>43501</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>43502</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>43503</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>43504</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -3723,6 +3791,33 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="163">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="172">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -4521,7 +4616,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5306,6 +5401,33 @@
                 <c:pt idx="163">
                   <c:v>43495</c:v>
                 </c:pt>
+                <c:pt idx="164">
+                  <c:v>43496</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>43497</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>43498</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>43499</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>43500</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>43501</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>43502</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>43503</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>43504</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -5805,6 +5927,33 @@
                   <c:v>378.45</c:v>
                 </c:pt>
                 <c:pt idx="163">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>378.45</c:v>
+                </c:pt>
+                <c:pt idx="172">
                   <c:v>378.45</c:v>
                 </c:pt>
               </c:numCache>
@@ -9245,10 +9394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z165"/>
+  <dimension ref="A1:Z174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A140" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="J172" sqref="J172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10254,7 +10403,7 @@
       </c>
       <c r="X19">
         <f>COUNTIF(P:P, "Freestyle 4")</f>
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="Y19" s="14">
         <f>C137-C117+1</f>
@@ -10262,7 +10411,7 @@
       </c>
       <c r="Z19" s="14">
         <f>Y19-X19</f>
-        <v>-17</v>
+        <v>-26</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -10473,11 +10622,11 @@
       </c>
       <c r="X23">
         <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="Y23" s="14">
         <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="Z23" s="14">
         <f>Y23-X23</f>
@@ -10564,7 +10713,7 @@
       </c>
       <c r="Z25">
         <f>SUM(Z11:Z19)</f>
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
@@ -13845,7 +13994,7 @@
         <v>43403</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" ref="C96:C165" si="8">B96</f>
+        <f t="shared" ref="C96:C168" si="8">B96</f>
         <v>43403</v>
       </c>
       <c r="D96" s="3">
@@ -15603,7 +15752,7 @@
         <v>3</v>
       </c>
       <c r="T131" s="4">
-        <f t="shared" ref="T131:T165" si="17">T130+M131</f>
+        <f t="shared" ref="T131:T174" si="17">T130+M131</f>
         <v>344.95</v>
       </c>
     </row>
@@ -16945,6 +17094,15 @@
         <f t="shared" si="8"/>
         <v>43495</v>
       </c>
+      <c r="D165" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="N165" t="s">
+        <v>330</v>
+      </c>
+      <c r="O165" t="s">
+        <v>331</v>
+      </c>
       <c r="P165" s="20" t="s">
         <v>119</v>
       </c>
@@ -16958,6 +17116,300 @@
         <v>3</v>
       </c>
       <c r="T165" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>0</v>
+      </c>
+      <c r="B166" s="1">
+        <v>43496</v>
+      </c>
+      <c r="C166" s="5">
+        <f t="shared" si="8"/>
+        <v>43496</v>
+      </c>
+      <c r="D166" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="P166" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q166">
+        <v>8</v>
+      </c>
+      <c r="R166" t="s">
+        <v>282</v>
+      </c>
+      <c r="S166">
+        <v>3</v>
+      </c>
+      <c r="T166" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>1</v>
+      </c>
+      <c r="B167" s="1">
+        <v>43497</v>
+      </c>
+      <c r="C167" s="5">
+        <f t="shared" si="8"/>
+        <v>43497</v>
+      </c>
+      <c r="D167" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="G167" s="3">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="N167" t="s">
+        <v>332</v>
+      </c>
+      <c r="P167" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q167">
+        <v>8</v>
+      </c>
+      <c r="R167" t="s">
+        <v>282</v>
+      </c>
+      <c r="S167">
+        <v>3</v>
+      </c>
+      <c r="T167" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>2</v>
+      </c>
+      <c r="B168" s="1">
+        <v>43498</v>
+      </c>
+      <c r="C168" s="5">
+        <f t="shared" si="8"/>
+        <v>43498</v>
+      </c>
+      <c r="D168" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="P168" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q168">
+        <v>8</v>
+      </c>
+      <c r="R168" t="s">
+        <v>282</v>
+      </c>
+      <c r="S168">
+        <v>3</v>
+      </c>
+      <c r="T168" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>3</v>
+      </c>
+      <c r="B169" s="1">
+        <v>43499</v>
+      </c>
+      <c r="C169" s="5">
+        <f t="shared" ref="C169:C174" si="20">B169</f>
+        <v>43499</v>
+      </c>
+      <c r="D169" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="E169" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="P169" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q169">
+        <v>8</v>
+      </c>
+      <c r="R169" t="s">
+        <v>282</v>
+      </c>
+      <c r="S169">
+        <v>3</v>
+      </c>
+      <c r="T169" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>10</v>
+      </c>
+      <c r="B170" s="1">
+        <v>43500</v>
+      </c>
+      <c r="C170" s="5">
+        <f t="shared" si="20"/>
+        <v>43500</v>
+      </c>
+      <c r="P170" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q170">
+        <v>8</v>
+      </c>
+      <c r="R170" t="s">
+        <v>282</v>
+      </c>
+      <c r="S170">
+        <v>3</v>
+      </c>
+      <c r="T170" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>67</v>
+      </c>
+      <c r="B171" s="1">
+        <v>43501</v>
+      </c>
+      <c r="C171" s="5">
+        <f t="shared" si="20"/>
+        <v>43501</v>
+      </c>
+      <c r="D171" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="P171" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q171">
+        <v>8</v>
+      </c>
+      <c r="R171" t="s">
+        <v>282</v>
+      </c>
+      <c r="S171">
+        <v>3</v>
+      </c>
+      <c r="T171" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>35</v>
+      </c>
+      <c r="B172" s="1">
+        <v>43502</v>
+      </c>
+      <c r="C172" s="5">
+        <f t="shared" si="20"/>
+        <v>43502</v>
+      </c>
+      <c r="D172" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="P172" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q172">
+        <v>8</v>
+      </c>
+      <c r="R172" t="s">
+        <v>282</v>
+      </c>
+      <c r="S172">
+        <v>3</v>
+      </c>
+      <c r="T172" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>0</v>
+      </c>
+      <c r="B173" s="1">
+        <v>43503</v>
+      </c>
+      <c r="C173" s="5">
+        <f t="shared" si="20"/>
+        <v>43503</v>
+      </c>
+      <c r="D173" s="3">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="P173" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q173">
+        <v>8</v>
+      </c>
+      <c r="R173" t="s">
+        <v>282</v>
+      </c>
+      <c r="S173">
+        <v>3</v>
+      </c>
+      <c r="T173" s="4">
+        <f t="shared" si="17"/>
+        <v>378.45</v>
+      </c>
+    </row>
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>1</v>
+      </c>
+      <c r="B174" s="1">
+        <v>43504</v>
+      </c>
+      <c r="C174" s="5">
+        <f t="shared" si="20"/>
+        <v>43504</v>
+      </c>
+      <c r="D174" s="3">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="E174" s="3">
+        <v>0.34375</v>
+      </c>
+      <c r="N174" t="s">
+        <v>328</v>
+      </c>
+      <c r="O174" t="s">
+        <v>329</v>
+      </c>
+      <c r="P174" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q174">
+        <v>8</v>
+      </c>
+      <c r="R174" t="s">
+        <v>282</v>
+      </c>
+      <c r="S174">
+        <v>3</v>
+      </c>
+      <c r="T174" s="4">
         <f t="shared" si="17"/>
         <v>378.45</v>
       </c>
@@ -17231,7 +17683,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated to 2/25 with missing info
Former-commit-id: c4d0948c48d8e5e8d43f78a52f0ea32aa745c1bd
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Desktop\repositories\ice-skating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4014BAF-510A-4B19-8079-06B16EF6DCD2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AD4D52-6F6F-4F5F-B36C-B394BD961420}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -19,17 +19,23 @@
     <sheet name="Skater Evaluation" sheetId="3" r:id="rId4"/>
     <sheet name="Test Requirements" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="352">
   <si>
     <t>Thursday</t>
   </si>
@@ -896,12 +902,6 @@
   </si>
   <si>
     <t>Currier, Private, Stroking</t>
-  </si>
-  <si>
-    <t>FS 1</t>
-  </si>
-  <si>
-    <t>FS 2</t>
   </si>
   <si>
     <t>FS 3</t>
@@ -1157,6 +1157,24 @@
   </si>
   <si>
     <t>Breakin in the New ones</t>
+  </si>
+  <si>
+    <t>Greatest Showman / Pairs Competition</t>
+  </si>
+  <si>
+    <t>Footwork Competition</t>
+  </si>
+  <si>
+    <t>FS Bronze Competition</t>
+  </si>
+  <si>
+    <t>Worked On FS4 Manuevers, Pairs with Laurel</t>
+  </si>
+  <si>
+    <t>Worked On FS4 Manuevers, High Confidence</t>
+  </si>
+  <si>
+    <t>FS 1 / FS 2</t>
   </si>
 </sst>
 </file>
@@ -1290,12 +1308,12 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -1550,10 +1568,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$390</c:f>
+              <c:f>Data!$C$2:$C$387</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="389"/>
+                <c:ptCount val="386"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -2072,16 +2090,55 @@
                 </c:pt>
                 <c:pt idx="172">
                   <c:v>43505</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>43506</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>43507</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>43508</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>43511</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>43512</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>43513</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>43514</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>43515</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>43516</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>43517</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>43518</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>43520</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>43521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$390</c:f>
+              <c:f>Data!$M$2:$M$387</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="389"/>
+                <c:ptCount val="386"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2567,6 +2624,21 @@
                 </c:pt>
                 <c:pt idx="172">
                   <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2869,10 +2941,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$390</c:f>
+              <c:f>Data!$C$2:$C$387</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="389"/>
+                <c:ptCount val="386"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -3391,16 +3463,55 @@
                 </c:pt>
                 <c:pt idx="172">
                   <c:v>43505</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>43506</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>43507</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>43508</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>43511</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>43512</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>43513</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>43514</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>43515</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>43516</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>43517</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>43518</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>43520</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>43521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$390</c:f>
+              <c:f>Data!$Q$2:$Q$387</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="389"/>
+                <c:ptCount val="386"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -3918,6 +4029,45 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="172">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="185">
                   <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
@@ -4267,9 +4417,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$V$11:$V$19</c:f>
+              <c:f>Data!$V$11:$V$18</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Pre Alpha</c:v>
                 </c:pt>
@@ -4286,15 +4436,12 @@
                   <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FS 1</c:v>
+                  <c:v>FS 1 / FS 2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>FS 2</c:v>
+                  <c:v>FS 3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FS 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>FS 4</c:v>
                 </c:pt>
               </c:strCache>
@@ -4302,10 +4449,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$11:$W$19</c:f>
+              <c:f>Data!$W$11:$W$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>7.75</c:v>
                 </c:pt>
@@ -4322,16 +4469,13 @@
                   <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>137.25</c:v>
+                  <c:v>137.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>119.75</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4652,9 +4796,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$V$11:$V$19</c:f>
+              <c:f>Data!$V$11:$V$18</c:f>
               <c:strCache>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>Pre Alpha</c:v>
                 </c:pt>
@@ -4671,15 +4815,12 @@
                   <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FS 1</c:v>
+                  <c:v>FS 1 / FS 2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>FS 2</c:v>
+                  <c:v>FS 3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FS 3</c:v>
-                </c:pt>
-                <c:pt idx="8">
                   <c:v>FS 4</c:v>
                 </c:pt>
               </c:strCache>
@@ -4687,10 +4828,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$11:$X$19</c:f>
+              <c:f>Data!$X$11:$X$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4710,13 +4851,10 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>58</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5005,10 +5143,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$390</c:f>
+              <c:f>Data!$C$2:$C$387</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="389"/>
+                <c:ptCount val="386"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -5527,16 +5665,55 @@
                 </c:pt>
                 <c:pt idx="172">
                   <c:v>43505</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>43506</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>43507</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>43508</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>43511</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>43512</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>43513</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>43514</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>43515</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>43516</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>43517</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>43518</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>43520</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>43521</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$T$2:$T$390</c:f>
+              <c:f>Data!$T$2:$T$387</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="389"/>
+                <c:ptCount val="386"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -6055,6 +6232,45 @@
                 </c:pt>
                 <c:pt idx="172">
                   <c:v>422.7</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>422.7</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>422.7</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>422.7</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>422.95</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>423.2</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>423.7</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>423.7</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>423.7</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>423.7</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>423.7</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>427.95</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>429.95</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>429.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9494,10 +9710,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z174"/>
+  <dimension ref="A1:Z187"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="W23" sqref="W23"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9634,13 +9850,13 @@
         <v>4</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -9682,11 +9898,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M:M)</f>
-        <v>422.7</v>
+        <v>429.95</v>
       </c>
       <c r="V3" s="4">
-        <f>SUM(M156:M400)</f>
-        <v>42.5</v>
+        <f>SUM(M156:M397)</f>
+        <v>49.75</v>
       </c>
       <c r="W3" s="4">
         <f>SUM(M19:M155)</f>
@@ -10310,11 +10526,11 @@
         <v>32</v>
       </c>
       <c r="V16" t="s">
-        <v>289</v>
+        <v>351</v>
       </c>
       <c r="W16" s="4">
-        <f>SUM(M43:M95)</f>
-        <v>137.25</v>
+        <f>SUM(M43:M96)</f>
+        <v>137.75</v>
       </c>
       <c r="X16">
         <f>COUNTIF(P:P, "Freestyle 1")</f>
@@ -10381,21 +10597,23 @@
         <v>38.25</v>
       </c>
       <c r="V17" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="W17" s="4">
-        <f>SUM(M96)</f>
-        <v>0.5</v>
+        <f>SUM(M97:M116)</f>
+        <v>61</v>
       </c>
       <c r="X17">
-        <f>COUNTIF(P:P, "Freestyle 2")</f>
-        <v>1</v>
-      </c>
-      <c r="Y17">
-        <v>1</v>
-      </c>
-      <c r="Z17">
-        <v>0</v>
+        <f>COUNTIF(P:P, "Freestyle 3")</f>
+        <v>20</v>
+      </c>
+      <c r="Y17" s="14">
+        <f>C116-C97+1</f>
+        <v>25</v>
+      </c>
+      <c r="Z17" s="14">
+        <f>Y17-X17</f>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
@@ -10439,23 +10657,23 @@
         <v>41.75</v>
       </c>
       <c r="V18" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="W18" s="4">
-        <f>SUM(M97:M116)</f>
-        <v>61</v>
+        <f>SUM(M117:M386)</f>
+        <v>127</v>
       </c>
       <c r="X18">
-        <f>COUNTIF(P:P, "Freestyle 3")</f>
-        <v>20</v>
+        <f>COUNTIF(P:P, "Freestyle 4")</f>
+        <v>71</v>
       </c>
       <c r="Y18" s="14">
-        <f>C116-C97+1</f>
-        <v>25</v>
+        <f>C137-C117+1</f>
+        <v>32</v>
       </c>
       <c r="Z18" s="14">
         <f>Y18-X18</f>
-        <v>5</v>
+        <v>-39</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -10498,25 +10716,6 @@
         <f t="shared" si="2"/>
         <v>42.75</v>
       </c>
-      <c r="V19" t="s">
-        <v>292</v>
-      </c>
-      <c r="W19" s="4">
-        <f>SUM(M117:M389)</f>
-        <v>119.75</v>
-      </c>
-      <c r="X19">
-        <f>COUNTIF(P:P, "Freestyle 4")</f>
-        <v>58</v>
-      </c>
-      <c r="Y19" s="14">
-        <f>C137-C117+1</f>
-        <v>32</v>
-      </c>
-      <c r="Z19" s="14">
-        <f>Y19-X19</f>
-        <v>-26</v>
-      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -10555,6 +10754,25 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
+      <c r="V20" t="s">
+        <v>254</v>
+      </c>
+      <c r="W20" s="4">
+        <f>SUM(M50:M92)</f>
+        <v>114.25</v>
+      </c>
+      <c r="X20">
+        <f>COUNTIF(R:R, "Dance 1")</f>
+        <v>43</v>
+      </c>
+      <c r="Y20" s="14">
+        <f>C92-C50+1</f>
+        <v>50</v>
+      </c>
+      <c r="Z20" s="14">
+        <f>Y20-X20</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -10594,23 +10812,23 @@
         <v>47.25</v>
       </c>
       <c r="V21" t="s">
-        <v>254</v>
+        <v>280</v>
       </c>
       <c r="W21" s="4">
-        <f>SUM(M50:M92)</f>
-        <v>114.25</v>
+        <f>SUM(M93:M100)</f>
+        <v>19</v>
       </c>
       <c r="X21">
-        <f>COUNTIF(R:R, "Dance 1")</f>
-        <v>43</v>
+        <f>COUNTIF(R:R, "Dance 2") - 1</f>
+        <v>7</v>
       </c>
       <c r="Y21" s="14">
-        <f>C92-C50+1</f>
-        <v>50</v>
+        <f>C100 - C92</f>
+        <v>7</v>
       </c>
       <c r="Z21" s="14">
         <f>Y21-X21</f>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -10651,23 +10869,23 @@
         <v>51.25</v>
       </c>
       <c r="V22" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="W22" s="4">
-        <f>SUM(M93:M100)</f>
-        <v>19</v>
+        <f>SUM(M100:M386)</f>
+        <v>180</v>
       </c>
       <c r="X22">
-        <f>COUNTIF(R:R, "Dance 2") - 1</f>
-        <v>7</v>
+        <f>COUNTIF(R:R, "Dance 3")</f>
+        <v>87</v>
       </c>
       <c r="Y22" s="14">
-        <f>C100 - C92</f>
-        <v>7</v>
+        <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
+        <v>114</v>
       </c>
       <c r="Z22" s="14">
         <f>Y22-X22</f>
-        <v>0</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -10717,24 +10935,8 @@
         <f t="shared" si="2"/>
         <v>58.5</v>
       </c>
-      <c r="V23" t="s">
-        <v>282</v>
-      </c>
-      <c r="W23" s="4">
-        <f>SUM(M100:M389)</f>
-        <v>172.75</v>
-      </c>
-      <c r="X23">
-        <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>74</v>
-      </c>
-      <c r="Y23" s="14">
-        <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>98</v>
-      </c>
-      <c r="Z23" s="14">
-        <f>Y23-X23</f>
-        <v>24</v>
+      <c r="Z23" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -10774,8 +10976,9 @@
         <f t="shared" si="2"/>
         <v>59.5</v>
       </c>
-      <c r="Z24" s="7" t="s">
-        <v>198</v>
+      <c r="Z24">
+        <f>SUM(Z11:Z18)</f>
+        <v>-12</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -10815,10 +11018,6 @@
         <f t="shared" si="2"/>
         <v>60.5</v>
       </c>
-      <c r="Z25">
-        <f>SUM(Z11:Z19)</f>
-        <v>1</v>
-      </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -14797,10 +14996,10 @@
         <v>2.5</v>
       </c>
       <c r="N110" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O110" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="P110" s="20" t="s">
         <v>113</v>
@@ -14864,10 +15063,10 @@
         <v>6.75</v>
       </c>
       <c r="N111" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="O111" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P111" s="20" t="s">
         <v>113</v>
@@ -14955,7 +15154,7 @@
         <v>1</v>
       </c>
       <c r="N113" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="O113" t="s">
         <v>284</v>
@@ -15049,7 +15248,7 @@
         <v>1</v>
       </c>
       <c r="N115" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O115" t="s">
         <v>68</v>
@@ -15257,7 +15456,7 @@
         <v>1</v>
       </c>
       <c r="N119" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O119" t="s">
         <v>284</v>
@@ -15348,7 +15547,7 @@
         <v>4</v>
       </c>
       <c r="O121" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="P121" s="20" t="s">
         <v>119</v>
@@ -15404,7 +15603,7 @@
         <v>4.25</v>
       </c>
       <c r="O122" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P122" s="20" t="s">
         <v>119</v>
@@ -15448,10 +15647,10 @@
         <v>3.5</v>
       </c>
       <c r="N123" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="O123" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="P123" s="20" t="s">
         <v>119</v>
@@ -15495,10 +15694,10 @@
         <v>1.75</v>
       </c>
       <c r="N124" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O124" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P124" s="20" t="s">
         <v>119</v>
@@ -15542,10 +15741,10 @@
         <v>1.75</v>
       </c>
       <c r="N125" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O125" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P125" s="20" t="s">
         <v>119</v>
@@ -15589,10 +15788,10 @@
         <v>1.75</v>
       </c>
       <c r="N126" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O126" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P126" s="20" t="s">
         <v>119</v>
@@ -15646,10 +15845,10 @@
         <v>3.5</v>
       </c>
       <c r="N127" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O127" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P127" s="20" t="s">
         <v>119</v>
@@ -15703,10 +15902,10 @@
         <v>3.5</v>
       </c>
       <c r="N128" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="O128" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P128" s="20" t="s">
         <v>119</v>
@@ -15838,10 +16037,10 @@
         <v>7.75</v>
       </c>
       <c r="N131" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O131" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P131" s="20" t="s">
         <v>119</v>
@@ -15856,7 +16055,7 @@
         <v>3</v>
       </c>
       <c r="T131" s="4">
-        <f t="shared" ref="T131:T174" si="17">T130+M131</f>
+        <f t="shared" ref="T131:T187" si="17">T130+M131</f>
         <v>344.95</v>
       </c>
     </row>
@@ -15929,7 +16128,7 @@
         <v>2</v>
       </c>
       <c r="N133" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O133" t="s">
         <v>17</v>
@@ -16013,7 +16212,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F135" s="2">
-        <f t="shared" ref="F135:F174" si="19">E135-D135</f>
+        <f t="shared" ref="F135:F187" si="19">E135-D135</f>
         <v>0.125</v>
       </c>
       <c r="G135" s="3">
@@ -16030,10 +16229,10 @@
         <v>5</v>
       </c>
       <c r="N135" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O135" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="P135" s="20" t="s">
         <v>119</v>
@@ -16087,10 +16286,10 @@
         <v>6.75</v>
       </c>
       <c r="N136" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="O136" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="P136" s="20" t="s">
         <v>119</v>
@@ -16144,7 +16343,7 @@
         <v>2.25</v>
       </c>
       <c r="N137" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O137" t="s">
         <v>21</v>
@@ -16191,10 +16390,10 @@
         <v>2.25</v>
       </c>
       <c r="N138" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O138" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P138" s="20" t="s">
         <v>119</v>
@@ -16248,7 +16447,7 @@
         <v>2</v>
       </c>
       <c r="N139" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="P139" s="20" t="s">
         <v>119</v>
@@ -16292,7 +16491,7 @@
         <v>1.75</v>
       </c>
       <c r="N140" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P140" s="20" t="s">
         <v>119</v>
@@ -16336,7 +16535,7 @@
         <v>2</v>
       </c>
       <c r="N141" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P141" s="20" t="s">
         <v>119</v>
@@ -16380,7 +16579,7 @@
         <v>4.25</v>
       </c>
       <c r="N142" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P142" s="20" t="s">
         <v>119</v>
@@ -16424,7 +16623,7 @@
         <v>2.25</v>
       </c>
       <c r="N143" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P143" s="20" t="s">
         <v>119</v>
@@ -16596,7 +16795,7 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="N148" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="P148" s="20" t="s">
         <v>119</v>
@@ -16847,7 +17046,7 @@
         <v>2.25</v>
       </c>
       <c r="N155" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P155" s="20" t="s">
         <v>119</v>
@@ -16891,7 +17090,7 @@
         <v>5.75</v>
       </c>
       <c r="N156" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="P156" s="20" t="s">
         <v>119</v>
@@ -16935,7 +17134,7 @@
         <v>3.5</v>
       </c>
       <c r="N157" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="P157" s="20" t="s">
         <v>119</v>
@@ -16979,7 +17178,7 @@
         <v>0.75</v>
       </c>
       <c r="N158" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="P158" s="20" t="s">
         <v>119</v>
@@ -17023,7 +17222,7 @@
         <v>0.5</v>
       </c>
       <c r="N159" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P159" s="20" t="s">
         <v>119</v>
@@ -17067,7 +17266,7 @@
         <v>3.5</v>
       </c>
       <c r="N160" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="P160" s="20" t="s">
         <v>119</v>
@@ -17111,7 +17310,7 @@
         <v>2</v>
       </c>
       <c r="N161" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="P161" s="20" t="s">
         <v>119</v>
@@ -17155,7 +17354,7 @@
         <v>0.5</v>
       </c>
       <c r="N162" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="P162" s="20" t="s">
         <v>119</v>
@@ -17199,7 +17398,7 @@
         <v>1.25</v>
       </c>
       <c r="N163" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="P163" s="20" t="s">
         <v>119</v>
@@ -17243,10 +17442,10 @@
         <v>1</v>
       </c>
       <c r="N164" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="O164" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="P164" s="20" t="s">
         <v>119</v>
@@ -17290,10 +17489,10 @@
         <v>2.75</v>
       </c>
       <c r="N165" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="O165" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="P165" s="20" t="s">
         <v>119</v>
@@ -17337,7 +17536,7 @@
         <v>1</v>
       </c>
       <c r="N166" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P166" s="20" t="s">
         <v>119</v>
@@ -17391,7 +17590,7 @@
         <v>1.75</v>
       </c>
       <c r="N167" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="P167" s="20" t="s">
         <v>119</v>
@@ -17445,7 +17644,7 @@
         <v>4.5</v>
       </c>
       <c r="N168" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="P168" s="20" t="s">
         <v>119</v>
@@ -17472,7 +17671,7 @@
         <v>43499</v>
       </c>
       <c r="C169" s="5">
-        <f t="shared" ref="C169:C174" si="20">B169</f>
+        <f t="shared" ref="C169:C187" si="20">B169</f>
         <v>43499</v>
       </c>
       <c r="D169" s="3">
@@ -17489,7 +17688,7 @@
         <v>2.25</v>
       </c>
       <c r="N169" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O169" t="s">
         <v>17</v>
@@ -17536,7 +17735,7 @@
         <v>1</v>
       </c>
       <c r="N170" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O170" t="s">
         <v>68</v>
@@ -17593,10 +17792,10 @@
         <v>2.25</v>
       </c>
       <c r="N171" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="O171" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P171" s="20" t="s">
         <v>119</v>
@@ -17640,7 +17839,7 @@
         <v>1.5</v>
       </c>
       <c r="N172" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="O172" t="s">
         <v>266</v>
@@ -17697,10 +17896,10 @@
         <v>1.75</v>
       </c>
       <c r="N173" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O173" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="P173" s="20" t="s">
         <v>119</v>
@@ -17744,10 +17943,10 @@
         <v>5</v>
       </c>
       <c r="N174" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O174" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="P174" s="20" t="s">
         <v>119</v>
@@ -17766,8 +17965,508 @@
         <v>422.7</v>
       </c>
     </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>3</v>
+      </c>
+      <c r="B175" s="1">
+        <v>43506</v>
+      </c>
+      <c r="C175" s="5">
+        <f t="shared" si="20"/>
+        <v>43506</v>
+      </c>
+      <c r="D175" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="F175" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.375</v>
+      </c>
+      <c r="P175" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q175">
+        <v>8</v>
+      </c>
+      <c r="R175" t="s">
+        <v>282</v>
+      </c>
+      <c r="S175">
+        <v>3</v>
+      </c>
+      <c r="T175" s="4">
+        <f t="shared" si="17"/>
+        <v>422.7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>10</v>
+      </c>
+      <c r="B176" s="1">
+        <v>43507</v>
+      </c>
+      <c r="C176" s="5">
+        <f t="shared" si="20"/>
+        <v>43507</v>
+      </c>
+      <c r="D176" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F176" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.69791666666666663</v>
+      </c>
+      <c r="P176" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q176">
+        <v>8</v>
+      </c>
+      <c r="R176" t="s">
+        <v>282</v>
+      </c>
+      <c r="S176">
+        <v>3</v>
+      </c>
+      <c r="T176" s="4">
+        <f t="shared" si="17"/>
+        <v>422.7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>67</v>
+      </c>
+      <c r="B177" s="1">
+        <v>43508</v>
+      </c>
+      <c r="C177" s="5">
+        <f t="shared" si="20"/>
+        <v>43508</v>
+      </c>
+      <c r="D177" s="3">
+        <v>0.68402777777777779</v>
+      </c>
+      <c r="F177" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.68402777777777779</v>
+      </c>
+      <c r="P177" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q177">
+        <v>8</v>
+      </c>
+      <c r="R177" t="s">
+        <v>282</v>
+      </c>
+      <c r="S177">
+        <v>3</v>
+      </c>
+      <c r="T177" s="4">
+        <f t="shared" si="17"/>
+        <v>422.7</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>1</v>
+      </c>
+      <c r="B178" s="1">
+        <v>43511</v>
+      </c>
+      <c r="C178" s="5">
+        <f t="shared" si="20"/>
+        <v>43511</v>
+      </c>
+      <c r="D178" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E178" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="F178" s="2">
+        <f t="shared" si="19"/>
+        <v>1.041666666666663E-2</v>
+      </c>
+      <c r="M178" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="N178" t="s">
+        <v>348</v>
+      </c>
+      <c r="P178" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q178">
+        <v>8</v>
+      </c>
+      <c r="R178" t="s">
+        <v>282</v>
+      </c>
+      <c r="S178">
+        <v>3</v>
+      </c>
+      <c r="T178" s="4">
+        <f t="shared" si="17"/>
+        <v>422.95</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>2</v>
+      </c>
+      <c r="B179" s="1">
+        <v>43512</v>
+      </c>
+      <c r="C179" s="5">
+        <f t="shared" si="20"/>
+        <v>43512</v>
+      </c>
+      <c r="D179" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E179" s="3">
+        <v>0.40625</v>
+      </c>
+      <c r="F179" s="2">
+        <f t="shared" si="19"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="M179" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="N179" t="s">
+        <v>347</v>
+      </c>
+      <c r="P179" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q179">
+        <v>8</v>
+      </c>
+      <c r="R179" t="s">
+        <v>282</v>
+      </c>
+      <c r="S179">
+        <v>3</v>
+      </c>
+      <c r="T179" s="4">
+        <f t="shared" si="17"/>
+        <v>423.2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" s="1">
+        <v>43513</v>
+      </c>
+      <c r="C180" s="5">
+        <f t="shared" si="20"/>
+        <v>43513</v>
+      </c>
+      <c r="D180" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E180" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="F180" s="2">
+        <f t="shared" si="19"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="M180" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N180" t="s">
+        <v>346</v>
+      </c>
+      <c r="P180" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q180">
+        <v>8</v>
+      </c>
+      <c r="R180" t="s">
+        <v>282</v>
+      </c>
+      <c r="S180">
+        <v>3</v>
+      </c>
+      <c r="T180" s="4">
+        <f t="shared" si="17"/>
+        <v>423.7</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>10</v>
+      </c>
+      <c r="B181" s="1">
+        <v>43514</v>
+      </c>
+      <c r="C181" s="5">
+        <f t="shared" si="20"/>
+        <v>43514</v>
+      </c>
+      <c r="F181" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P181" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q181">
+        <v>8</v>
+      </c>
+      <c r="R181" t="s">
+        <v>282</v>
+      </c>
+      <c r="S181">
+        <v>3</v>
+      </c>
+      <c r="T181" s="4">
+        <f t="shared" si="17"/>
+        <v>423.7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>67</v>
+      </c>
+      <c r="B182" s="1">
+        <v>43515</v>
+      </c>
+      <c r="C182" s="5">
+        <f t="shared" si="20"/>
+        <v>43515</v>
+      </c>
+      <c r="D182" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F182" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.69791666666666663</v>
+      </c>
+      <c r="P182" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q182">
+        <v>8</v>
+      </c>
+      <c r="R182" t="s">
+        <v>282</v>
+      </c>
+      <c r="S182">
+        <v>3</v>
+      </c>
+      <c r="T182" s="4">
+        <f t="shared" si="17"/>
+        <v>423.7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>35</v>
+      </c>
+      <c r="B183" s="1">
+        <v>43516</v>
+      </c>
+      <c r="C183" s="5">
+        <f t="shared" si="20"/>
+        <v>43516</v>
+      </c>
+      <c r="D183" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F183" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.73958333333333337</v>
+      </c>
+      <c r="P183" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q183">
+        <v>8</v>
+      </c>
+      <c r="R183" t="s">
+        <v>282</v>
+      </c>
+      <c r="S183">
+        <v>3</v>
+      </c>
+      <c r="T183" s="4">
+        <f t="shared" si="17"/>
+        <v>423.7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>0</v>
+      </c>
+      <c r="B184" s="1">
+        <v>43517</v>
+      </c>
+      <c r="C184" s="5">
+        <f t="shared" si="20"/>
+        <v>43517</v>
+      </c>
+      <c r="D184" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="F184" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.69791666666666663</v>
+      </c>
+      <c r="P184" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q184">
+        <v>8</v>
+      </c>
+      <c r="R184" t="s">
+        <v>282</v>
+      </c>
+      <c r="S184">
+        <v>3</v>
+      </c>
+      <c r="T184" s="4">
+        <f t="shared" si="17"/>
+        <v>423.7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>1</v>
+      </c>
+      <c r="B185" s="1">
+        <v>43518</v>
+      </c>
+      <c r="C185" s="5">
+        <f t="shared" si="20"/>
+        <v>43518</v>
+      </c>
+      <c r="D185" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E185" s="3">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="F185" s="2">
+        <f t="shared" si="19"/>
+        <v>0.17708333333333326</v>
+      </c>
+      <c r="M185" s="4">
+        <v>4.25</v>
+      </c>
+      <c r="N185" t="s">
+        <v>349</v>
+      </c>
+      <c r="O185" t="s">
+        <v>17</v>
+      </c>
+      <c r="P185" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q185">
+        <v>8</v>
+      </c>
+      <c r="R185" t="s">
+        <v>282</v>
+      </c>
+      <c r="S185">
+        <v>3</v>
+      </c>
+      <c r="T185" s="4">
+        <f t="shared" si="17"/>
+        <v>427.95</v>
+      </c>
+    </row>
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" s="1">
+        <v>43520</v>
+      </c>
+      <c r="C186" s="5">
+        <f t="shared" si="20"/>
+        <v>43520</v>
+      </c>
+      <c r="D186" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="E186" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F186" s="2">
+        <f t="shared" si="19"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="M186" s="4">
+        <v>2</v>
+      </c>
+      <c r="N186" t="s">
+        <v>350</v>
+      </c>
+      <c r="O186" t="s">
+        <v>17</v>
+      </c>
+      <c r="P186" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q186">
+        <v>8</v>
+      </c>
+      <c r="R186" t="s">
+        <v>282</v>
+      </c>
+      <c r="S186">
+        <v>3</v>
+      </c>
+      <c r="T186" s="4">
+        <f t="shared" si="17"/>
+        <v>429.95</v>
+      </c>
+    </row>
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>10</v>
+      </c>
+      <c r="B187" s="1">
+        <v>43521</v>
+      </c>
+      <c r="C187" s="5">
+        <f t="shared" si="20"/>
+        <v>43521</v>
+      </c>
+      <c r="F187" s="2">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="P187" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q187">
+        <v>8</v>
+      </c>
+      <c r="R187" t="s">
+        <v>282</v>
+      </c>
+      <c r="S187">
+        <v>3</v>
+      </c>
+      <c r="T187" s="4">
+        <f t="shared" si="17"/>
+        <v>429.95</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T530">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T527">
     <cfRule type="expression" dxfId="17" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
@@ -18023,7 +18722,7 @@
         <v>209</v>
       </c>
       <c r="I5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
   </sheetData>
@@ -18035,7 +18734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
ENTIRELY CAUGHT UP TO 3/5/19
Former-commit-id: b363fe8fa87fd61cd74e6a1133e25ae8ebaddb2d
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aNDREW\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AD4D52-6F6F-4F5F-B36C-B394BD961420}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8007C56-5160-4004-8553-BA8B4A4C38E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="8640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="356">
   <si>
     <t>Thursday</t>
   </si>
@@ -1175,6 +1175,18 @@
   </si>
   <si>
     <t>FS 1 / FS 2</t>
+  </si>
+  <si>
+    <t>Pain on blisters couldn't skate</t>
+  </si>
+  <si>
+    <t>Passed FS4, got tour from greg, worked on Camels and footwork</t>
+  </si>
+  <si>
+    <t>Program Drills</t>
+  </si>
+  <si>
+    <t>FS5</t>
   </si>
 </sst>
 </file>
@@ -1568,10 +1580,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$387</c:f>
+              <c:f>Data!$C$2:$C$382</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="386"/>
+                <c:ptCount val="381"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -1999,146 +2011,152 @@
                   <c:v>43466</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>43467</c:v>
+                  <c:v>43468</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>43468</c:v>
+                  <c:v>43471</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>43469</c:v>
+                  <c:v>43472</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>43470</c:v>
+                  <c:v>43474</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>43471</c:v>
+                  <c:v>43475</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>43472</c:v>
+                  <c:v>43476</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>43473</c:v>
+                  <c:v>43477</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>43474</c:v>
+                  <c:v>43478</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>43475</c:v>
+                  <c:v>43484</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>43476</c:v>
+                  <c:v>43485</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>43477</c:v>
+                  <c:v>43487</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>43478</c:v>
+                  <c:v>43489</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>43484</c:v>
+                  <c:v>43490</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>43485</c:v>
+                  <c:v>43491</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>43487</c:v>
+                  <c:v>43492</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>43489</c:v>
+                  <c:v>43493</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>43490</c:v>
+                  <c:v>43494</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>43491</c:v>
+                  <c:v>43495</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>43492</c:v>
+                  <c:v>43496</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>43493</c:v>
+                  <c:v>43497</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>43494</c:v>
+                  <c:v>43498</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>43495</c:v>
+                  <c:v>43499</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>43496</c:v>
+                  <c:v>43501</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>43497</c:v>
+                  <c:v>43502</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>43498</c:v>
+                  <c:v>43503</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>43499</c:v>
+                  <c:v>43504</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>43501</c:v>
+                  <c:v>43505</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>43502</c:v>
+                  <c:v>43506</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>43503</c:v>
+                  <c:v>43507</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>43504</c:v>
+                  <c:v>43508</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>43505</c:v>
+                  <c:v>43511</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>43506</c:v>
+                  <c:v>43512</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>43507</c:v>
+                  <c:v>43513</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>43508</c:v>
+                  <c:v>43515</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>43511</c:v>
+                  <c:v>43516</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>43512</c:v>
+                  <c:v>43517</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>43513</c:v>
+                  <c:v>43518</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>43514</c:v>
+                  <c:v>43520</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>43515</c:v>
+                  <c:v>43521</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>43516</c:v>
+                  <c:v>43522</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>43517</c:v>
+                  <c:v>43523</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>43518</c:v>
+                  <c:v>43524</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>43520</c:v>
+                  <c:v>43525</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>43521</c:v>
+                  <c:v>43526</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>43527</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>43528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$387</c:f>
+              <c:f>Data!$M$2:$M$382</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="386"/>
+                <c:ptCount val="381"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2565,80 +2583,143 @@
                 <c:pt idx="141">
                   <c:v>2.25</c:v>
                 </c:pt>
+                <c:pt idx="142">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>5.75</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>0.75</c:v>
+                </c:pt>
                 <c:pt idx="153">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="163">
                   <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="154">
-                  <c:v>5.75</c:v>
-                </c:pt>
-                <c:pt idx="155">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="156">
-                  <c:v>0.75</c:v>
-                </c:pt>
-                <c:pt idx="157">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="158">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="159">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="160">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="161">
-                  <c:v>1.25</c:v>
-                </c:pt>
-                <c:pt idx="162">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="163">
-                  <c:v>2.75</c:v>
                 </c:pt>
                 <c:pt idx="164">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="165">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="167">
                   <c:v>1.75</c:v>
                 </c:pt>
-                <c:pt idx="166">
-                  <c:v>4.5</c:v>
-                </c:pt>
-                <c:pt idx="167">
+                <c:pt idx="168">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>4.25</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="185">
                   <c:v>2.25</c:v>
                 </c:pt>
-                <c:pt idx="168">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="169">
-                  <c:v>2.25</c:v>
-                </c:pt>
-                <c:pt idx="170">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="171">
+                <c:pt idx="186">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="187">
                   <c:v>1.75</c:v>
-                </c:pt>
-                <c:pt idx="172">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="176">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="177">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="178">
-                  <c:v>0.5</c:v>
-                </c:pt>
-                <c:pt idx="183">
-                  <c:v>4.25</c:v>
-                </c:pt>
-                <c:pt idx="184">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2941,10 +3022,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$387</c:f>
+              <c:f>Data!$C$2:$C$382</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="386"/>
+                <c:ptCount val="381"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -3372,146 +3453,152 @@
                   <c:v>43466</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>43467</c:v>
+                  <c:v>43468</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>43468</c:v>
+                  <c:v>43471</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>43469</c:v>
+                  <c:v>43472</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>43470</c:v>
+                  <c:v>43474</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>43471</c:v>
+                  <c:v>43475</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>43472</c:v>
+                  <c:v>43476</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>43473</c:v>
+                  <c:v>43477</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>43474</c:v>
+                  <c:v>43478</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>43475</c:v>
+                  <c:v>43484</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>43476</c:v>
+                  <c:v>43485</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>43477</c:v>
+                  <c:v>43487</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>43478</c:v>
+                  <c:v>43489</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>43484</c:v>
+                  <c:v>43490</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>43485</c:v>
+                  <c:v>43491</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>43487</c:v>
+                  <c:v>43492</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>43489</c:v>
+                  <c:v>43493</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>43490</c:v>
+                  <c:v>43494</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>43491</c:v>
+                  <c:v>43495</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>43492</c:v>
+                  <c:v>43496</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>43493</c:v>
+                  <c:v>43497</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>43494</c:v>
+                  <c:v>43498</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>43495</c:v>
+                  <c:v>43499</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>43496</c:v>
+                  <c:v>43501</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>43497</c:v>
+                  <c:v>43502</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>43498</c:v>
+                  <c:v>43503</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>43499</c:v>
+                  <c:v>43504</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>43501</c:v>
+                  <c:v>43505</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>43502</c:v>
+                  <c:v>43506</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>43503</c:v>
+                  <c:v>43507</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>43504</c:v>
+                  <c:v>43508</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>43505</c:v>
+                  <c:v>43511</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>43506</c:v>
+                  <c:v>43512</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>43507</c:v>
+                  <c:v>43513</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>43508</c:v>
+                  <c:v>43515</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>43511</c:v>
+                  <c:v>43516</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>43512</c:v>
+                  <c:v>43517</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>43513</c:v>
+                  <c:v>43518</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>43514</c:v>
+                  <c:v>43520</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>43515</c:v>
+                  <c:v>43521</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>43516</c:v>
+                  <c:v>43522</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>43517</c:v>
+                  <c:v>43523</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>43518</c:v>
+                  <c:v>43524</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>43520</c:v>
+                  <c:v>43525</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>43521</c:v>
+                  <c:v>43526</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>43527</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>43528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$387</c:f>
+              <c:f>Data!$Q$2:$Q$382</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="386"/>
+                <c:ptCount val="381"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4056,19 +4143,25 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4417,9 +4510,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$V$11:$V$18</c:f>
+              <c:f>Data!$V$11:$V$19</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Pre Alpha</c:v>
                 </c:pt>
@@ -4443,16 +4536,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>FS 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FS5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$W$11:$W$18</c:f>
+              <c:f>Data!$W$11:$W$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>7.75</c:v>
                 </c:pt>
@@ -4475,7 +4571,10 @@
                   <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>127</c:v>
+                  <c:v>150.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4796,9 +4895,9 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$V$11:$V$18</c:f>
+              <c:f>Data!$V$11:$V$19</c:f>
               <c:strCache>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>Pre Alpha</c:v>
                 </c:pt>
@@ -4822,16 +4921,19 @@
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>FS 4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>FS5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$X$11:$X$18</c:f>
+              <c:f>Data!$X$11:$X$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>3</c:v>
                 </c:pt>
@@ -4854,7 +4956,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>71</c:v>
+                  <c:v>66</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5143,10 +5245,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$387</c:f>
+              <c:f>Data!$C$2:$C$382</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="386"/>
+                <c:ptCount val="381"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -5574,146 +5676,152 @@
                   <c:v>43466</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>43467</c:v>
+                  <c:v>43468</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>43468</c:v>
+                  <c:v>43471</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>43469</c:v>
+                  <c:v>43472</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>43470</c:v>
+                  <c:v>43474</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>43471</c:v>
+                  <c:v>43475</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>43472</c:v>
+                  <c:v>43476</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>43473</c:v>
+                  <c:v>43477</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>43474</c:v>
+                  <c:v>43478</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>43475</c:v>
+                  <c:v>43484</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>43476</c:v>
+                  <c:v>43485</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>43477</c:v>
+                  <c:v>43487</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>43478</c:v>
+                  <c:v>43489</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>43484</c:v>
+                  <c:v>43490</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>43485</c:v>
+                  <c:v>43491</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>43487</c:v>
+                  <c:v>43492</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>43489</c:v>
+                  <c:v>43493</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>43490</c:v>
+                  <c:v>43494</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>43491</c:v>
+                  <c:v>43495</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>43492</c:v>
+                  <c:v>43496</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>43493</c:v>
+                  <c:v>43497</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>43494</c:v>
+                  <c:v>43498</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>43495</c:v>
+                  <c:v>43499</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>43496</c:v>
+                  <c:v>43501</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>43497</c:v>
+                  <c:v>43502</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>43498</c:v>
+                  <c:v>43503</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>43499</c:v>
+                  <c:v>43504</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>43501</c:v>
+                  <c:v>43505</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>43502</c:v>
+                  <c:v>43506</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>43503</c:v>
+                  <c:v>43507</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>43504</c:v>
+                  <c:v>43508</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>43505</c:v>
+                  <c:v>43511</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>43506</c:v>
+                  <c:v>43512</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>43507</c:v>
+                  <c:v>43513</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>43508</c:v>
+                  <c:v>43515</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>43511</c:v>
+                  <c:v>43516</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>43512</c:v>
+                  <c:v>43517</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>43513</c:v>
+                  <c:v>43518</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>43514</c:v>
+                  <c:v>43520</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>43515</c:v>
+                  <c:v>43521</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>43516</c:v>
+                  <c:v>43522</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>43517</c:v>
+                  <c:v>43523</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>43518</c:v>
+                  <c:v>43524</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>43520</c:v>
+                  <c:v>43525</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>43521</c:v>
+                  <c:v>43526</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>43527</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>43528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$T$2:$T$387</c:f>
+              <c:f>Data!$T$2:$T$382</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="386"/>
+                <c:ptCount val="381"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -6141,136 +6249,142 @@
                   <c:v>377.95</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>377.95</c:v>
+                  <c:v>379.45</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>377.95</c:v>
+                  <c:v>381.95</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>377.95</c:v>
+                  <c:v>384.2</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>377.95</c:v>
+                  <c:v>387.2</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>377.95</c:v>
+                  <c:v>388.2</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>377.95</c:v>
+                  <c:v>389.95</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>377.95</c:v>
+                  <c:v>392.7</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>377.95</c:v>
+                  <c:v>394.95</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>377.95</c:v>
+                  <c:v>400.7</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>377.95</c:v>
+                  <c:v>404.2</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>377.95</c:v>
+                  <c:v>404.95</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>380.2</c:v>
+                  <c:v>405.45</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>385.95</c:v>
+                  <c:v>408.95</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>389.45</c:v>
+                  <c:v>410.95</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>390.2</c:v>
+                  <c:v>411.45</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>390.7</c:v>
+                  <c:v>412.7</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>394.2</c:v>
+                  <c:v>413.7</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>396.2</c:v>
+                  <c:v>416.45</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>396.7</c:v>
+                  <c:v>417.45</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>397.95</c:v>
+                  <c:v>419.2</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>398.95</c:v>
+                  <c:v>423.7</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>401.7</c:v>
+                  <c:v>425.95</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>402.7</c:v>
+                  <c:v>426.95</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>404.45</c:v>
+                  <c:v>429.2</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>408.95</c:v>
+                  <c:v>430.7</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>411.2</c:v>
+                  <c:v>432.45</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>412.2</c:v>
+                  <c:v>437.45</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>414.45</c:v>
+                  <c:v>439.2</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>415.95</c:v>
+                  <c:v>440.2</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>417.7</c:v>
+                  <c:v>441.45</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>422.7</c:v>
+                  <c:v>441.7</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>422.7</c:v>
+                  <c:v>441.95</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>422.7</c:v>
+                  <c:v>442.45</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>422.7</c:v>
+                  <c:v>443.45</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>422.95</c:v>
+                  <c:v>445.45</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>423.2</c:v>
+                  <c:v>446.45</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>423.7</c:v>
+                  <c:v>450.7</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>423.7</c:v>
+                  <c:v>452.7</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>423.7</c:v>
+                  <c:v>453.7</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>423.7</c:v>
+                  <c:v>454.95</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>423.7</c:v>
+                  <c:v>455.45</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>427.95</c:v>
+                  <c:v>458.95</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>429.95</c:v>
+                  <c:v>460.45</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>429.95</c:v>
+                  <c:v>462.7</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>463.95</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>465.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9710,10 +9824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z187"/>
+  <dimension ref="A1:Z189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="V3" sqref="V3"/>
+    <sheetView topLeftCell="M1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9898,15 +10012,15 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M:M)</f>
-        <v>429.95</v>
+        <v>465.7</v>
       </c>
       <c r="V3" s="4">
-        <f>SUM(M156:M397)</f>
-        <v>49.75</v>
+        <f>SUM(M152:M392)</f>
+        <v>70.75</v>
       </c>
       <c r="W3" s="4">
-        <f>SUM(M19:M155)</f>
-        <v>338.45</v>
+        <f>SUM(M19:M151)</f>
+        <v>353.2</v>
       </c>
       <c r="X3" s="4">
         <f>SUM(M2:M18)</f>
@@ -10660,12 +10774,12 @@
         <v>290</v>
       </c>
       <c r="W18" s="4">
-        <f>SUM(M117:M386)</f>
-        <v>127</v>
+        <f>SUM(M117:M182)</f>
+        <v>150.75</v>
       </c>
       <c r="X18">
         <f>COUNTIF(P:P, "Freestyle 4")</f>
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="Y18" s="14">
         <f>C137-C117+1</f>
@@ -10673,7 +10787,7 @@
       </c>
       <c r="Z18" s="14">
         <f>Y18-X18</f>
-        <v>-39</v>
+        <v>-34</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
@@ -10716,6 +10830,13 @@
         <f t="shared" si="2"/>
         <v>42.75</v>
       </c>
+      <c r="V19" t="s">
+        <v>355</v>
+      </c>
+      <c r="W19" s="4">
+        <f>SUM(M183:M400)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -10754,25 +10875,6 @@
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="V20" t="s">
-        <v>254</v>
-      </c>
-      <c r="W20" s="4">
-        <f>SUM(M50:M92)</f>
-        <v>114.25</v>
-      </c>
-      <c r="X20">
-        <f>COUNTIF(R:R, "Dance 1")</f>
-        <v>43</v>
-      </c>
-      <c r="Y20" s="14">
-        <f>C92-C50+1</f>
-        <v>50</v>
-      </c>
-      <c r="Z20" s="14">
-        <f>Y20-X20</f>
-        <v>7</v>
-      </c>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -10812,23 +10914,23 @@
         <v>47.25</v>
       </c>
       <c r="V21" t="s">
-        <v>280</v>
+        <v>254</v>
       </c>
       <c r="W21" s="4">
-        <f>SUM(M93:M100)</f>
-        <v>19</v>
+        <f>SUM(M50:M92)</f>
+        <v>114.25</v>
       </c>
       <c r="X21">
-        <f>COUNTIF(R:R, "Dance 2") - 1</f>
-        <v>7</v>
+        <f>COUNTIF(R:R, "Dance 1")</f>
+        <v>43</v>
       </c>
       <c r="Y21" s="14">
-        <f>C100 - C92</f>
-        <v>7</v>
+        <f>C92-C50+1</f>
+        <v>50</v>
       </c>
       <c r="Z21" s="14">
         <f>Y21-X21</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
@@ -10869,23 +10971,23 @@
         <v>51.25</v>
       </c>
       <c r="V22" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="W22" s="4">
-        <f>SUM(M100:M386)</f>
-        <v>180</v>
+        <f>SUM(M93:M100)</f>
+        <v>19</v>
       </c>
       <c r="X22">
-        <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>87</v>
+        <f>COUNTIF(R:R, "Dance 2") - 1</f>
+        <v>7</v>
       </c>
       <c r="Y22" s="14">
-        <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>114</v>
+        <f>C100 - C92</f>
+        <v>7</v>
       </c>
       <c r="Z22" s="14">
         <f>Y22-X22</f>
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
@@ -10935,8 +11037,24 @@
         <f t="shared" si="2"/>
         <v>58.5</v>
       </c>
-      <c r="Z23" s="7" t="s">
-        <v>198</v>
+      <c r="V23" t="s">
+        <v>282</v>
+      </c>
+      <c r="W23" s="4">
+        <f>SUM(M100:M381)</f>
+        <v>215.75</v>
+      </c>
+      <c r="X23">
+        <f>COUNTIF(R:R, "Dance 3")</f>
+        <v>89</v>
+      </c>
+      <c r="Y23" s="14">
+        <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
+        <v>121</v>
+      </c>
+      <c r="Z23" s="14">
+        <f>Y23-X23</f>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -10976,9 +11094,8 @@
         <f t="shared" si="2"/>
         <v>59.5</v>
       </c>
-      <c r="Z24">
-        <f>SUM(Z11:Z18)</f>
-        <v>-12</v>
+      <c r="Z24" s="7" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
@@ -11018,6 +11135,10 @@
         <f t="shared" si="2"/>
         <v>60.5</v>
       </c>
+      <c r="Z25">
+        <f>SUM(Z11:Z18)</f>
+        <v>-7</v>
+      </c>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -14297,7 +14418,7 @@
         <v>43403</v>
       </c>
       <c r="C96" s="5">
-        <f t="shared" ref="C96:C168" si="8">B96</f>
+        <f t="shared" ref="C96:C164" si="8">B96</f>
         <v>43403</v>
       </c>
       <c r="D96" s="3">
@@ -16055,7 +16176,7 @@
         <v>3</v>
       </c>
       <c r="T131" s="4">
-        <f t="shared" ref="T131:T187" si="17">T130+M131</f>
+        <f t="shared" ref="T131:T189" si="17">T130+M131</f>
         <v>344.95</v>
       </c>
     </row>
@@ -16212,7 +16333,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F135" s="2">
-        <f t="shared" ref="F135:F187" si="19">E135-D135</f>
+        <f t="shared" ref="F135:F189" si="19">E135-D135</f>
         <v>0.125</v>
       </c>
       <c r="G135" s="3">
@@ -16644,18 +16765,27 @@
     </row>
     <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="B144" s="1">
-        <v>43467</v>
+        <v>43468</v>
       </c>
       <c r="C144" s="5">
         <f t="shared" si="8"/>
-        <v>43467</v>
+        <v>43468</v>
+      </c>
+      <c r="D144" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="E144" s="3">
+        <v>0.89583333333333337</v>
       </c>
       <c r="F144" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M144" s="4">
+        <v>1.5</v>
       </c>
       <c r="P144" s="20" t="s">
         <v>119</v>
@@ -16671,23 +16801,45 @@
       </c>
       <c r="T144" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>379.45</v>
       </c>
     </row>
     <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B145" s="1">
-        <v>43468</v>
+        <v>43471</v>
       </c>
       <c r="C145" s="5">
         <f t="shared" si="8"/>
-        <v>43468</v>
+        <v>43471</v>
+      </c>
+      <c r="D145" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="E145" s="3">
+        <v>0.46875</v>
       </c>
       <c r="F145" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G145" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="H145" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="I145" s="2">
+        <f>H145-G145</f>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M145" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="N145" t="s">
+        <v>317</v>
       </c>
       <c r="P145" s="20" t="s">
         <v>119</v>
@@ -16703,23 +16855,32 @@
       </c>
       <c r="T145" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>381.95</v>
       </c>
     </row>
     <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B146" s="1">
-        <v>43469</v>
+        <v>43472</v>
       </c>
       <c r="C146" s="5">
         <f t="shared" si="8"/>
-        <v>43469</v>
+        <v>43472</v>
+      </c>
+      <c r="D146" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="E146" s="3">
+        <v>0.82291666666666663</v>
       </c>
       <c r="F146" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M146" s="4">
+        <v>2.25</v>
       </c>
       <c r="P146" s="20" t="s">
         <v>119</v>
@@ -16735,23 +16896,32 @@
       </c>
       <c r="T146" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>384.2</v>
       </c>
     </row>
     <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B147" s="1">
-        <v>43470</v>
+        <v>43474</v>
       </c>
       <c r="C147" s="5">
         <f t="shared" si="8"/>
-        <v>43470</v>
+        <v>43474</v>
+      </c>
+      <c r="D147" s="3">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E147" s="3">
+        <v>0.82291666666666663</v>
       </c>
       <c r="F147" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.125</v>
+      </c>
+      <c r="M147" s="4">
+        <v>3</v>
       </c>
       <c r="P147" s="20" t="s">
         <v>119</v>
@@ -16767,35 +16937,32 @@
       </c>
       <c r="T147" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>387.2</v>
       </c>
     </row>
     <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B148" s="1">
-        <v>43471</v>
+        <v>43475</v>
       </c>
       <c r="C148" s="5">
         <f t="shared" si="8"/>
-        <v>43471</v>
+        <v>43475</v>
       </c>
       <c r="D148" s="3">
-        <v>0.42708333333333331</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E148" s="3">
-        <v>0.46875</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F148" s="2">
         <f t="shared" si="19"/>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="G148" s="3">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="N148" t="s">
-        <v>317</v>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="M148" s="4">
+        <v>1</v>
       </c>
       <c r="P148" s="20" t="s">
         <v>119</v>
@@ -16811,26 +16978,32 @@
       </c>
       <c r="T148" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>388.2</v>
       </c>
     </row>
     <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B149" s="1">
-        <v>43472</v>
+        <v>43476</v>
       </c>
       <c r="C149" s="5">
         <f t="shared" si="8"/>
-        <v>43472</v>
+        <v>43476</v>
       </c>
       <c r="D149" s="3">
-        <v>0.72916666666666663</v>
+        <v>0.78125</v>
+      </c>
+      <c r="E149" s="3">
+        <v>0.85416666666666663</v>
       </c>
       <c r="F149" s="2">
         <f t="shared" si="19"/>
-        <v>-0.72916666666666663</v>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="M149" s="4">
+        <v>1.75</v>
       </c>
       <c r="P149" s="20" t="s">
         <v>119</v>
@@ -16846,23 +17019,32 @@
       </c>
       <c r="T149" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>389.95</v>
       </c>
     </row>
     <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B150" s="1">
-        <v>43473</v>
+        <v>43477</v>
       </c>
       <c r="C150" s="5">
         <f t="shared" si="8"/>
-        <v>43473</v>
+        <v>43477</v>
+      </c>
+      <c r="D150" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E150" s="3">
+        <v>0.85416666666666663</v>
       </c>
       <c r="F150" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>0.11458333333333326</v>
+      </c>
+      <c r="M150" s="4">
+        <v>2.75</v>
       </c>
       <c r="P150" s="20" t="s">
         <v>119</v>
@@ -16878,26 +17060,35 @@
       </c>
       <c r="T150" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>392.7</v>
       </c>
     </row>
     <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B151" s="1">
-        <v>43474</v>
+        <v>43478</v>
       </c>
       <c r="C151" s="5">
         <f t="shared" si="8"/>
-        <v>43474</v>
+        <v>43478</v>
       </c>
       <c r="D151" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="E151" s="3">
+        <v>0.64583333333333337</v>
       </c>
       <c r="F151" s="2">
         <f t="shared" si="19"/>
-        <v>-0.69791666666666663</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M151" s="4">
+        <v>2.25</v>
+      </c>
+      <c r="N151" t="s">
+        <v>318</v>
       </c>
       <c r="P151" s="20" t="s">
         <v>119</v>
@@ -16913,26 +17104,35 @@
       </c>
       <c r="T151" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>394.95</v>
       </c>
     </row>
     <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B152" s="1">
-        <v>43475</v>
+        <v>43484</v>
       </c>
       <c r="C152" s="5">
         <f t="shared" si="8"/>
-        <v>43475</v>
+        <v>43484</v>
       </c>
       <c r="D152" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.46875</v>
+      </c>
+      <c r="E152" s="3">
+        <v>0.70833333333333337</v>
       </c>
       <c r="F152" s="2">
         <f t="shared" si="19"/>
-        <v>-0.69791666666666663</v>
+        <v>0.23958333333333337</v>
+      </c>
+      <c r="M152" s="4">
+        <v>5.75</v>
+      </c>
+      <c r="N152" t="s">
+        <v>344</v>
       </c>
       <c r="P152" s="20" t="s">
         <v>119</v>
@@ -16948,26 +17148,35 @@
       </c>
       <c r="T152" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>400.7</v>
       </c>
     </row>
     <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B153" s="1">
-        <v>43476</v>
+        <v>43485</v>
       </c>
       <c r="C153" s="5">
         <f t="shared" si="8"/>
-        <v>43476</v>
+        <v>43485</v>
       </c>
       <c r="D153" s="3">
-        <v>0.78125</v>
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="E153" s="3">
+        <v>0.6875</v>
       </c>
       <c r="F153" s="2">
         <f t="shared" si="19"/>
-        <v>-0.78125</v>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="M153" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="N153" t="s">
+        <v>345</v>
       </c>
       <c r="P153" s="20" t="s">
         <v>119</v>
@@ -16983,26 +17192,35 @@
       </c>
       <c r="T153" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>404.2</v>
       </c>
     </row>
     <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>2</v>
+        <v>67</v>
       </c>
       <c r="B154" s="1">
-        <v>43477</v>
+        <v>43487</v>
       </c>
       <c r="C154" s="5">
         <f t="shared" si="8"/>
-        <v>43477</v>
+        <v>43487</v>
       </c>
       <c r="D154" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E154" s="3">
         <v>0.73958333333333337</v>
       </c>
       <c r="F154" s="2">
         <f t="shared" si="19"/>
-        <v>-0.73958333333333337</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M154" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="N154" t="s">
+        <v>343</v>
       </c>
       <c r="P154" s="20" t="s">
         <v>119</v>
@@ -17018,35 +17236,35 @@
       </c>
       <c r="T154" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
+        <v>404.95</v>
       </c>
     </row>
     <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B155" s="1">
-        <v>43478</v>
+        <v>43489</v>
       </c>
       <c r="C155" s="5">
         <f t="shared" si="8"/>
-        <v>43478</v>
+        <v>43489</v>
       </c>
       <c r="D155" s="3">
-        <v>0.55208333333333337</v>
+        <v>0.71875</v>
       </c>
       <c r="E155" s="3">
-        <v>0.64583333333333337</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F155" s="2">
         <f t="shared" si="19"/>
-        <v>9.375E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="M155" s="4">
-        <v>2.25</v>
+        <v>0.5</v>
       </c>
       <c r="N155" t="s">
-        <v>318</v>
+        <v>342</v>
       </c>
       <c r="P155" s="20" t="s">
         <v>119</v>
@@ -17062,35 +17280,35 @@
       </c>
       <c r="T155" s="4">
         <f t="shared" si="17"/>
-        <v>380.2</v>
+        <v>405.45</v>
       </c>
     </row>
     <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B156" s="1">
-        <v>43484</v>
+        <v>43490</v>
       </c>
       <c r="C156" s="5">
         <f t="shared" si="8"/>
-        <v>43484</v>
+        <v>43490</v>
       </c>
       <c r="D156" s="3">
-        <v>0.46875</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E156" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.85416666666666663</v>
       </c>
       <c r="F156" s="2">
         <f t="shared" si="19"/>
-        <v>0.23958333333333337</v>
+        <v>0.14583333333333326</v>
       </c>
       <c r="M156" s="4">
-        <v>5.75</v>
+        <v>3.5</v>
       </c>
       <c r="N156" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="P156" s="20" t="s">
         <v>119</v>
@@ -17106,35 +17324,35 @@
       </c>
       <c r="T156" s="4">
         <f t="shared" si="17"/>
-        <v>385.95</v>
+        <v>408.95</v>
       </c>
     </row>
     <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B157" s="1">
-        <v>43485</v>
+        <v>43491</v>
       </c>
       <c r="C157" s="5">
         <f t="shared" si="8"/>
-        <v>43485</v>
+        <v>43491</v>
       </c>
       <c r="D157" s="3">
-        <v>0.54166666666666663</v>
+        <v>0.65625</v>
       </c>
       <c r="E157" s="3">
-        <v>0.6875</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F157" s="2">
         <f t="shared" si="19"/>
-        <v>0.14583333333333337</v>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="M157" s="4">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="N157" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="P157" s="20" t="s">
         <v>119</v>
@@ -17150,35 +17368,35 @@
       </c>
       <c r="T157" s="4">
         <f t="shared" si="17"/>
-        <v>389.45</v>
+        <v>410.95</v>
       </c>
     </row>
     <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>67</v>
+        <v>3</v>
       </c>
       <c r="B158" s="1">
-        <v>43487</v>
+        <v>43492</v>
       </c>
       <c r="C158" s="5">
         <f t="shared" si="8"/>
-        <v>43487</v>
+        <v>43492</v>
       </c>
       <c r="D158" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.66666666666666663</v>
       </c>
       <c r="E158" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.6875</v>
       </c>
       <c r="F158" s="2">
         <f t="shared" si="19"/>
-        <v>3.125E-2</v>
+        <v>2.083333333333337E-2</v>
       </c>
       <c r="M158" s="4">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="N158" t="s">
-        <v>343</v>
+        <v>320</v>
       </c>
       <c r="P158" s="20" t="s">
         <v>119</v>
@@ -17194,35 +17412,35 @@
       </c>
       <c r="T158" s="4">
         <f t="shared" si="17"/>
-        <v>390.2</v>
+        <v>411.45</v>
       </c>
     </row>
     <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B159" s="1">
-        <v>43489</v>
+        <v>43493</v>
       </c>
       <c r="C159" s="5">
         <f t="shared" si="8"/>
-        <v>43489</v>
+        <v>43493</v>
       </c>
       <c r="D159" s="3">
-        <v>0.71875</v>
+        <v>0.77083333333333337</v>
       </c>
       <c r="E159" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="F159" s="2">
         <f t="shared" si="19"/>
-        <v>2.083333333333337E-2</v>
+        <v>5.2083333333333259E-2</v>
       </c>
       <c r="M159" s="4">
-        <v>0.5</v>
+        <v>1.25</v>
       </c>
       <c r="N159" t="s">
-        <v>342</v>
+        <v>321</v>
       </c>
       <c r="P159" s="20" t="s">
         <v>119</v>
@@ -17238,35 +17456,38 @@
       </c>
       <c r="T159" s="4">
         <f t="shared" si="17"/>
-        <v>390.7</v>
+        <v>412.7</v>
       </c>
     </row>
     <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="B160" s="1">
-        <v>43490</v>
+        <v>43494</v>
       </c>
       <c r="C160" s="5">
         <f t="shared" si="8"/>
-        <v>43490</v>
+        <v>43494</v>
       </c>
       <c r="D160" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="E160" s="3">
-        <v>0.85416666666666663</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="F160" s="2">
         <f t="shared" si="19"/>
-        <v>0.14583333333333326</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="M160" s="4">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="N160" t="s">
-        <v>341</v>
+        <v>319</v>
+      </c>
+      <c r="O160" t="s">
+        <v>322</v>
       </c>
       <c r="P160" s="20" t="s">
         <v>119</v>
@@ -17282,35 +17503,38 @@
       </c>
       <c r="T160" s="4">
         <f t="shared" si="17"/>
-        <v>394.2</v>
+        <v>413.7</v>
       </c>
     </row>
     <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="B161" s="1">
-        <v>43491</v>
+        <v>43495</v>
       </c>
       <c r="C161" s="5">
         <f t="shared" si="8"/>
-        <v>43491</v>
+        <v>43495</v>
       </c>
       <c r="D161" s="3">
-        <v>0.65625</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E161" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="F161" s="2">
         <f t="shared" si="19"/>
-        <v>8.333333333333337E-2</v>
+        <v>0.11458333333333326</v>
       </c>
       <c r="M161" s="4">
-        <v>2</v>
+        <v>2.75</v>
       </c>
       <c r="N161" t="s">
-        <v>340</v>
+        <v>339</v>
+      </c>
+      <c r="O161" t="s">
+        <v>326</v>
       </c>
       <c r="P161" s="20" t="s">
         <v>119</v>
@@ -17326,35 +17550,35 @@
       </c>
       <c r="T161" s="4">
         <f t="shared" si="17"/>
-        <v>396.2</v>
+        <v>416.45</v>
       </c>
     </row>
     <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B162" s="1">
-        <v>43492</v>
+        <v>43496</v>
       </c>
       <c r="C162" s="5">
         <f t="shared" si="8"/>
-        <v>43492</v>
+        <v>43496</v>
       </c>
       <c r="D162" s="3">
-        <v>0.66666666666666663</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E162" s="3">
-        <v>0.6875</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F162" s="2">
         <f t="shared" si="19"/>
-        <v>2.083333333333337E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="M162" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N162" t="s">
-        <v>320</v>
+        <v>337</v>
       </c>
       <c r="P162" s="20" t="s">
         <v>119</v>
@@ -17370,35 +17594,45 @@
       </c>
       <c r="T162" s="4">
         <f t="shared" si="17"/>
-        <v>396.7</v>
+        <v>417.45</v>
       </c>
     </row>
     <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B163" s="1">
-        <v>43493</v>
+        <v>43497</v>
       </c>
       <c r="C163" s="5">
         <f t="shared" si="8"/>
-        <v>43493</v>
+        <v>43497</v>
       </c>
       <c r="D163" s="3">
-        <v>0.77083333333333337</v>
+        <v>0.59375</v>
       </c>
       <c r="E163" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.61458333333333337</v>
       </c>
       <c r="F163" s="2">
         <f t="shared" si="19"/>
-        <v>5.2083333333333259E-2</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="G163" s="3">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="H163" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="I163" s="2">
+        <f>H163-G163</f>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="M163" s="4">
-        <v>1.25</v>
+        <v>1.75</v>
       </c>
       <c r="N163" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="P163" s="20" t="s">
         <v>119</v>
@@ -17414,38 +17648,45 @@
       </c>
       <c r="T163" s="4">
         <f t="shared" si="17"/>
-        <v>397.95</v>
+        <v>419.2</v>
       </c>
     </row>
     <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B164" s="1">
-        <v>43494</v>
+        <v>43498</v>
       </c>
       <c r="C164" s="5">
         <f t="shared" si="8"/>
-        <v>43494</v>
+        <v>43498</v>
       </c>
       <c r="D164" s="3">
-        <v>0.63541666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="E164" s="3">
-        <v>0.67708333333333337</v>
+        <v>0.47916666666666669</v>
       </c>
       <c r="F164" s="2">
         <f t="shared" si="19"/>
-        <v>4.1666666666666741E-2</v>
+        <v>0.10416666666666669</v>
+      </c>
+      <c r="G164" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="H164" s="3">
+        <v>0.90625</v>
+      </c>
+      <c r="I164" s="2">
+        <f>H164-G164</f>
+        <v>8.333333333333337E-2</v>
       </c>
       <c r="M164" s="4">
-        <v>1</v>
+        <v>4.5</v>
       </c>
       <c r="N164" t="s">
-        <v>319</v>
-      </c>
-      <c r="O164" t="s">
-        <v>322</v>
+        <v>338</v>
       </c>
       <c r="P164" s="20" t="s">
         <v>119</v>
@@ -17461,38 +17702,38 @@
       </c>
       <c r="T164" s="4">
         <f t="shared" si="17"/>
-        <v>398.95</v>
+        <v>423.7</v>
       </c>
     </row>
     <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B165" s="1">
-        <v>43495</v>
+        <v>43499</v>
       </c>
       <c r="C165" s="5">
-        <f t="shared" si="8"/>
-        <v>43495</v>
+        <f t="shared" ref="C165:C189" si="20">B165</f>
+        <v>43499</v>
       </c>
       <c r="D165" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.59375</v>
       </c>
       <c r="E165" s="3">
-        <v>0.82291666666666663</v>
+        <v>0.6875</v>
       </c>
       <c r="F165" s="2">
         <f t="shared" si="19"/>
-        <v>0.11458333333333326</v>
+        <v>9.375E-2</v>
       </c>
       <c r="M165" s="4">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="N165" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="O165" t="s">
-        <v>326</v>
+        <v>17</v>
       </c>
       <c r="P165" s="20" t="s">
         <v>119</v>
@@ -17508,19 +17749,19 @@
       </c>
       <c r="T165" s="4">
         <f t="shared" si="17"/>
-        <v>401.7</v>
+        <v>425.95</v>
       </c>
     </row>
     <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="B166" s="1">
-        <v>43496</v>
+        <v>43501</v>
       </c>
       <c r="C166" s="5">
-        <f t="shared" si="8"/>
-        <v>43496</v>
+        <f t="shared" si="20"/>
+        <v>43501</v>
       </c>
       <c r="D166" s="3">
         <v>0.69791666666666663</v>
@@ -17536,7 +17777,10 @@
         <v>1</v>
       </c>
       <c r="N166" t="s">
-        <v>337</v>
+        <v>335</v>
+      </c>
+      <c r="O166" t="s">
+        <v>68</v>
       </c>
       <c r="P166" s="20" t="s">
         <v>119</v>
@@ -17552,45 +17796,48 @@
       </c>
       <c r="T166" s="4">
         <f t="shared" si="17"/>
-        <v>402.7</v>
+        <v>426.95</v>
       </c>
     </row>
     <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B167" s="1">
-        <v>43497</v>
+        <v>43502</v>
       </c>
       <c r="C167" s="5">
-        <f t="shared" si="8"/>
-        <v>43497</v>
+        <f t="shared" si="20"/>
+        <v>43502</v>
       </c>
       <c r="D167" s="3">
-        <v>0.59375</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="E167" s="3">
-        <v>0.61458333333333337</v>
+        <v>0.63541666666666663</v>
       </c>
       <c r="F167" s="2">
         <f t="shared" si="19"/>
-        <v>2.083333333333337E-2</v>
+        <v>5.2083333333333259E-2</v>
       </c>
       <c r="G167" s="3">
-        <v>0.76041666666666663</v>
+        <v>0.78125</v>
       </c>
       <c r="H167" s="3">
-        <v>0.8125</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="I167" s="2">
         <f>H167-G167</f>
-        <v>5.208333333333337E-2</v>
+        <v>4.166666666666663E-2</v>
       </c>
       <c r="M167" s="4">
-        <v>1.75</v>
+        <v>2.25</v>
       </c>
       <c r="N167" t="s">
-        <v>327</v>
+        <v>333</v>
+      </c>
+      <c r="O167" t="s">
+        <v>334</v>
       </c>
       <c r="P167" s="20" t="s">
         <v>119</v>
@@ -17606,45 +17853,38 @@
       </c>
       <c r="T167" s="4">
         <f t="shared" si="17"/>
-        <v>404.45</v>
+        <v>429.2</v>
       </c>
     </row>
     <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B168" s="1">
-        <v>43498</v>
+        <v>43503</v>
       </c>
       <c r="C168" s="5">
-        <f t="shared" si="8"/>
-        <v>43498</v>
+        <f t="shared" si="20"/>
+        <v>43503</v>
       </c>
       <c r="D168" s="3">
-        <v>0.375</v>
+        <v>0.67708333333333337</v>
       </c>
       <c r="E168" s="3">
-        <v>0.47916666666666669</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F168" s="2">
         <f t="shared" si="19"/>
-        <v>0.10416666666666669</v>
-      </c>
-      <c r="G168" s="3">
-        <v>0.82291666666666663</v>
-      </c>
-      <c r="H168" s="3">
-        <v>0.90625</v>
-      </c>
-      <c r="I168" s="2">
-        <f>H168-G168</f>
-        <v>8.333333333333337E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M168" s="4">
-        <v>4.5</v>
+        <v>1.5</v>
       </c>
       <c r="N168" t="s">
-        <v>338</v>
+        <v>332</v>
+      </c>
+      <c r="O168" t="s">
+        <v>266</v>
       </c>
       <c r="P168" s="20" t="s">
         <v>119</v>
@@ -17660,38 +17900,48 @@
       </c>
       <c r="T168" s="4">
         <f t="shared" si="17"/>
-        <v>408.95</v>
+        <v>430.7</v>
       </c>
     </row>
     <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B169" s="1">
-        <v>43499</v>
+        <v>43504</v>
       </c>
       <c r="C169" s="5">
-        <f t="shared" ref="C169:C187" si="20">B169</f>
-        <v>43499</v>
+        <f t="shared" si="20"/>
+        <v>43504</v>
       </c>
       <c r="D169" s="3">
-        <v>0.59375</v>
+        <v>0.30208333333333331</v>
       </c>
       <c r="E169" s="3">
-        <v>0.6875</v>
+        <v>0.34375</v>
       </c>
       <c r="F169" s="2">
         <f t="shared" si="19"/>
-        <v>9.375E-2</v>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="G169" s="3">
+        <v>0.77430555555555547</v>
+      </c>
+      <c r="H169" s="3">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="I169" s="2">
+        <f>H169-G169</f>
+        <v>3.125E-2</v>
       </c>
       <c r="M169" s="4">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="N169" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="O169" t="s">
-        <v>17</v>
+        <v>331</v>
       </c>
       <c r="P169" s="20" t="s">
         <v>119</v>
@@ -17707,38 +17957,38 @@
       </c>
       <c r="T169" s="4">
         <f t="shared" si="17"/>
-        <v>411.2</v>
+        <v>432.45</v>
       </c>
     </row>
     <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>67</v>
+        <v>2</v>
       </c>
       <c r="B170" s="1">
-        <v>43501</v>
+        <v>43505</v>
       </c>
       <c r="C170" s="5">
         <f t="shared" si="20"/>
-        <v>43501</v>
+        <v>43505</v>
       </c>
       <c r="D170" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.375</v>
       </c>
       <c r="E170" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.58333333333333337</v>
       </c>
       <c r="F170" s="2">
         <f t="shared" si="19"/>
-        <v>4.1666666666666741E-2</v>
+        <v>0.20833333333333337</v>
       </c>
       <c r="M170" s="4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N170" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="O170" t="s">
-        <v>68</v>
+        <v>329</v>
       </c>
       <c r="P170" s="20" t="s">
         <v>119</v>
@@ -17754,48 +18004,35 @@
       </c>
       <c r="T170" s="4">
         <f t="shared" si="17"/>
-        <v>412.2</v>
+        <v>437.45</v>
       </c>
     </row>
     <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>35</v>
+        <v>3</v>
       </c>
       <c r="B171" s="1">
-        <v>43502</v>
+        <v>43506</v>
       </c>
       <c r="C171" s="5">
         <f t="shared" si="20"/>
-        <v>43502</v>
+        <v>43506</v>
       </c>
       <c r="D171" s="3">
-        <v>0.58333333333333337</v>
+        <v>0.375</v>
       </c>
       <c r="E171" s="3">
-        <v>0.63541666666666663</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="F171" s="2">
         <f t="shared" si="19"/>
-        <v>5.2083333333333259E-2</v>
-      </c>
-      <c r="G171" s="3">
-        <v>0.78125</v>
-      </c>
-      <c r="H171" s="3">
-        <v>0.82291666666666663</v>
-      </c>
-      <c r="I171" s="2">
-        <f>H171-G171</f>
-        <v>4.166666666666663E-2</v>
+        <v>7.2916666666666685E-2</v>
       </c>
       <c r="M171" s="4">
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="N171" t="s">
-        <v>333</v>
-      </c>
-      <c r="O171" t="s">
-        <v>334</v>
+        <v>354</v>
       </c>
       <c r="P171" s="20" t="s">
         <v>119</v>
@@ -17811,38 +18048,35 @@
       </c>
       <c r="T171" s="4">
         <f t="shared" si="17"/>
-        <v>414.45</v>
+        <v>439.2</v>
       </c>
     </row>
     <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B172" s="1">
-        <v>43503</v>
+        <v>43507</v>
       </c>
       <c r="C172" s="5">
         <f t="shared" si="20"/>
-        <v>43503</v>
+        <v>43507</v>
       </c>
       <c r="D172" s="3">
-        <v>0.67708333333333337</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E172" s="3">
         <v>0.73958333333333337</v>
       </c>
       <c r="F172" s="2">
         <f t="shared" si="19"/>
-        <v>6.25E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="M172" s="4">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="N172" t="s">
-        <v>332</v>
-      </c>
-      <c r="O172" t="s">
-        <v>266</v>
+        <v>354</v>
       </c>
       <c r="P172" s="20" t="s">
         <v>119</v>
@@ -17858,48 +18092,35 @@
       </c>
       <c r="T172" s="4">
         <f t="shared" si="17"/>
-        <v>415.95</v>
+        <v>440.2</v>
       </c>
     </row>
     <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>1</v>
+        <v>67</v>
       </c>
       <c r="B173" s="1">
-        <v>43504</v>
+        <v>43508</v>
       </c>
       <c r="C173" s="5">
         <f t="shared" si="20"/>
-        <v>43504</v>
+        <v>43508</v>
       </c>
       <c r="D173" s="3">
-        <v>0.30208333333333331</v>
+        <v>0.6875</v>
       </c>
       <c r="E173" s="3">
-        <v>0.34375</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F173" s="2">
         <f t="shared" si="19"/>
-        <v>4.1666666666666685E-2</v>
-      </c>
-      <c r="G173" s="3">
-        <v>0.77430555555555547</v>
-      </c>
-      <c r="H173" s="3">
-        <v>0.80555555555555547</v>
-      </c>
-      <c r="I173" s="2">
-        <f>H173-G173</f>
-        <v>3.125E-2</v>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="M173" s="4">
-        <v>1.75</v>
+        <v>1.25</v>
       </c>
       <c r="N173" t="s">
-        <v>330</v>
-      </c>
-      <c r="O173" t="s">
-        <v>331</v>
+        <v>354</v>
       </c>
       <c r="P173" s="20" t="s">
         <v>119</v>
@@ -17915,38 +18136,35 @@
       </c>
       <c r="T173" s="4">
         <f t="shared" si="17"/>
-        <v>417.7</v>
+        <v>441.45</v>
       </c>
     </row>
     <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B174" s="1">
-        <v>43505</v>
+        <v>43511</v>
       </c>
       <c r="C174" s="5">
         <f t="shared" si="20"/>
-        <v>43505</v>
+        <v>43511</v>
       </c>
       <c r="D174" s="3">
-        <v>0.375</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E174" s="3">
-        <v>0.58333333333333337</v>
+        <v>0.71875</v>
       </c>
       <c r="F174" s="2">
         <f t="shared" si="19"/>
-        <v>0.20833333333333337</v>
+        <v>1.041666666666663E-2</v>
       </c>
       <c r="M174" s="4">
-        <v>5</v>
+        <v>0.25</v>
       </c>
       <c r="N174" t="s">
-        <v>328</v>
-      </c>
-      <c r="O174" t="s">
-        <v>329</v>
+        <v>348</v>
       </c>
       <c r="P174" s="20" t="s">
         <v>119</v>
@@ -17962,26 +18180,35 @@
       </c>
       <c r="T174" s="4">
         <f t="shared" si="17"/>
-        <v>422.7</v>
+        <v>441.7</v>
       </c>
     </row>
     <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B175" s="1">
-        <v>43506</v>
+        <v>43512</v>
       </c>
       <c r="C175" s="5">
         <f t="shared" si="20"/>
-        <v>43506</v>
+        <v>43512</v>
       </c>
       <c r="D175" s="3">
-        <v>0.375</v>
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="E175" s="3">
+        <v>0.40625</v>
       </c>
       <c r="F175" s="2">
         <f t="shared" si="19"/>
-        <v>-0.375</v>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="M175" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="N175" t="s">
+        <v>347</v>
       </c>
       <c r="P175" s="20" t="s">
         <v>119</v>
@@ -17997,26 +18224,35 @@
       </c>
       <c r="T175" s="4">
         <f t="shared" si="17"/>
-        <v>422.7</v>
+        <v>441.95</v>
       </c>
     </row>
     <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B176" s="1">
-        <v>43507</v>
+        <v>43513</v>
       </c>
       <c r="C176" s="5">
         <f t="shared" si="20"/>
-        <v>43507</v>
+        <v>43513</v>
       </c>
       <c r="D176" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="E176" s="3">
+        <v>0.60416666666666663</v>
       </c>
       <c r="F176" s="2">
         <f t="shared" si="19"/>
-        <v>-0.69791666666666663</v>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="M176" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N176" t="s">
+        <v>346</v>
       </c>
       <c r="P176" s="20" t="s">
         <v>119</v>
@@ -18032,7 +18268,7 @@
       </c>
       <c r="T176" s="4">
         <f t="shared" si="17"/>
-        <v>422.7</v>
+        <v>442.45</v>
       </c>
     </row>
     <row r="177" spans="1:20" x14ac:dyDescent="0.25">
@@ -18040,18 +18276,24 @@
         <v>67</v>
       </c>
       <c r="B177" s="1">
-        <v>43508</v>
+        <v>43515</v>
       </c>
       <c r="C177" s="5">
         <f t="shared" si="20"/>
-        <v>43508</v>
+        <v>43515</v>
       </c>
       <c r="D177" s="3">
-        <v>0.68402777777777779</v>
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="E177" s="3">
+        <v>0.73958333333333337</v>
       </c>
       <c r="F177" s="2">
         <f t="shared" si="19"/>
-        <v>-0.68402777777777779</v>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="M177" s="4">
+        <v>1</v>
       </c>
       <c r="P177" s="20" t="s">
         <v>119</v>
@@ -18067,35 +18309,32 @@
       </c>
       <c r="T177" s="4">
         <f t="shared" si="17"/>
-        <v>422.7</v>
+        <v>443.45</v>
       </c>
     </row>
     <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B178" s="1">
-        <v>43511</v>
+        <v>43516</v>
       </c>
       <c r="C178" s="5">
         <f t="shared" si="20"/>
-        <v>43511</v>
+        <v>43516</v>
       </c>
       <c r="D178" s="3">
-        <v>0.70833333333333337</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="E178" s="3">
-        <v>0.71875</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="F178" s="2">
         <f t="shared" si="19"/>
-        <v>1.041666666666663E-2</v>
+        <v>8.3333333333333259E-2</v>
       </c>
       <c r="M178" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="N178" t="s">
-        <v>348</v>
+        <v>2</v>
       </c>
       <c r="P178" s="20" t="s">
         <v>119</v>
@@ -18111,35 +18350,32 @@
       </c>
       <c r="T178" s="4">
         <f t="shared" si="17"/>
-        <v>422.95</v>
+        <v>445.45</v>
       </c>
     </row>
     <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B179" s="1">
-        <v>43512</v>
+        <v>43517</v>
       </c>
       <c r="C179" s="5">
         <f t="shared" si="20"/>
-        <v>43512</v>
+        <v>43517</v>
       </c>
       <c r="D179" s="3">
-        <v>0.39583333333333331</v>
+        <v>0.69791666666666663</v>
       </c>
       <c r="E179" s="3">
-        <v>0.40625</v>
+        <v>0.73958333333333337</v>
       </c>
       <c r="F179" s="2">
         <f t="shared" si="19"/>
-        <v>1.0416666666666685E-2</v>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="M179" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="N179" t="s">
-        <v>347</v>
+        <v>1</v>
       </c>
       <c r="P179" s="20" t="s">
         <v>119</v>
@@ -18155,35 +18391,38 @@
       </c>
       <c r="T179" s="4">
         <f t="shared" si="17"/>
-        <v>423.2</v>
+        <v>446.45</v>
       </c>
     </row>
     <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B180" s="1">
-        <v>43513</v>
+        <v>43518</v>
       </c>
       <c r="C180" s="5">
         <f t="shared" si="20"/>
-        <v>43513</v>
+        <v>43518</v>
       </c>
       <c r="D180" s="3">
-        <v>0.58333333333333337</v>
+        <v>0.70833333333333337</v>
       </c>
       <c r="E180" s="3">
-        <v>0.60416666666666663</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="F180" s="2">
         <f t="shared" si="19"/>
-        <v>2.0833333333333259E-2</v>
+        <v>0.17708333333333326</v>
       </c>
       <c r="M180" s="4">
-        <v>0.5</v>
+        <v>4.25</v>
       </c>
       <c r="N180" t="s">
-        <v>346</v>
+        <v>349</v>
+      </c>
+      <c r="O180" t="s">
+        <v>17</v>
       </c>
       <c r="P180" s="20" t="s">
         <v>119</v>
@@ -18199,23 +18438,38 @@
       </c>
       <c r="T180" s="4">
         <f t="shared" si="17"/>
-        <v>423.7</v>
+        <v>450.7</v>
       </c>
     </row>
     <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B181" s="1">
-        <v>43514</v>
+        <v>43520</v>
       </c>
       <c r="C181" s="5">
         <f t="shared" si="20"/>
-        <v>43514</v>
+        <v>43520</v>
+      </c>
+      <c r="D181" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="E181" s="3">
+        <v>0.64583333333333337</v>
       </c>
       <c r="F181" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="M181" s="4">
+        <v>2</v>
+      </c>
+      <c r="N181" t="s">
+        <v>350</v>
+      </c>
+      <c r="O181" t="s">
+        <v>17</v>
       </c>
       <c r="P181" s="20" t="s">
         <v>119</v>
@@ -18231,26 +18485,32 @@
       </c>
       <c r="T181" s="4">
         <f t="shared" si="17"/>
-        <v>423.7</v>
+        <v>452.7</v>
       </c>
     </row>
     <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>67</v>
+        <v>10</v>
       </c>
       <c r="B182" s="1">
-        <v>43515</v>
+        <v>43521</v>
       </c>
       <c r="C182" s="5">
         <f t="shared" si="20"/>
-        <v>43515</v>
+        <v>43521</v>
       </c>
       <c r="D182" s="3">
         <v>0.69791666666666663</v>
       </c>
+      <c r="E182" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F182" s="2">
         <f t="shared" si="19"/>
-        <v>-0.69791666666666663</v>
+        <v>4.1666666666666741E-2</v>
+      </c>
+      <c r="M182" s="4">
+        <v>1</v>
       </c>
       <c r="P182" s="20" t="s">
         <v>119</v>
@@ -18266,32 +18526,51 @@
       </c>
       <c r="T182" s="4">
         <f t="shared" si="17"/>
-        <v>423.7</v>
+        <v>453.7</v>
       </c>
     </row>
     <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B183" s="1">
-        <v>43516</v>
+        <v>43522</v>
       </c>
       <c r="C183" s="5">
         <f t="shared" si="20"/>
-        <v>43516</v>
+        <v>43522</v>
       </c>
       <c r="D183" s="3">
-        <v>0.73958333333333337</v>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E183" s="3">
+        <v>0.6875</v>
       </c>
       <c r="F183" s="2">
         <f t="shared" si="19"/>
-        <v>-0.73958333333333337</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="G183" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="H183" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="I183" s="2">
+        <f>H183-G183</f>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M183" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="N183" t="s">
+        <v>353</v>
       </c>
       <c r="P183" s="20" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q183">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R183" t="s">
         <v>282</v>
@@ -18301,32 +18580,41 @@
       </c>
       <c r="T183" s="4">
         <f t="shared" si="17"/>
-        <v>423.7</v>
+        <v>454.95</v>
       </c>
     </row>
     <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B184" s="1">
-        <v>43517</v>
+        <v>43523</v>
       </c>
       <c r="C184" s="5">
         <f t="shared" si="20"/>
-        <v>43517</v>
+        <v>43523</v>
       </c>
       <c r="D184" s="3">
-        <v>0.69791666666666663</v>
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E184" s="3">
+        <v>0.72916666666666663</v>
       </c>
       <c r="F184" s="2">
         <f t="shared" si="19"/>
-        <v>-0.69791666666666663</v>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="M184" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N184" t="s">
+        <v>352</v>
       </c>
       <c r="P184" s="20" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q184">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R184" t="s">
         <v>282</v>
@@ -18336,44 +18624,48 @@
       </c>
       <c r="T184" s="4">
         <f t="shared" si="17"/>
-        <v>423.7</v>
+        <v>455.45</v>
       </c>
     </row>
     <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B185" s="1">
-        <v>43518</v>
+        <v>43524</v>
       </c>
       <c r="C185" s="5">
         <f t="shared" si="20"/>
-        <v>43518</v>
+        <v>43524</v>
       </c>
       <c r="D185" s="3">
         <v>0.70833333333333337</v>
       </c>
       <c r="E185" s="3">
-        <v>0.88541666666666663</v>
+        <v>0.8125</v>
       </c>
       <c r="F185" s="2">
         <f t="shared" si="19"/>
-        <v>0.17708333333333326</v>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="G185" s="3">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="H185" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="I185" s="2">
+        <f>H185-G185</f>
+        <v>4.1666666666666741E-2</v>
       </c>
       <c r="M185" s="4">
-        <v>4.25</v>
-      </c>
-      <c r="N185" t="s">
-        <v>349</v>
-      </c>
-      <c r="O185" t="s">
-        <v>17</v>
+        <v>3.5</v>
       </c>
       <c r="P185" s="20" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q185">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R185" t="s">
         <v>282</v>
@@ -18383,44 +18675,38 @@
       </c>
       <c r="T185" s="4">
         <f t="shared" si="17"/>
-        <v>427.95</v>
+        <v>458.95</v>
       </c>
     </row>
     <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B186" s="1">
-        <v>43520</v>
+        <v>43525</v>
       </c>
       <c r="C186" s="5">
         <f t="shared" si="20"/>
-        <v>43520</v>
+        <v>43525</v>
       </c>
       <c r="D186" s="3">
-        <v>0.5625</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="E186" s="3">
-        <v>0.64583333333333337</v>
+        <v>0.88541666666666663</v>
       </c>
       <c r="F186" s="2">
         <f t="shared" si="19"/>
-        <v>8.333333333333337E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M186" s="4">
-        <v>2</v>
-      </c>
-      <c r="N186" t="s">
-        <v>350</v>
-      </c>
-      <c r="O186" t="s">
-        <v>17</v>
+        <v>1.5</v>
       </c>
       <c r="P186" s="20" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q186">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R186" t="s">
         <v>282</v>
@@ -18430,29 +18716,38 @@
       </c>
       <c r="T186" s="4">
         <f t="shared" si="17"/>
-        <v>429.95</v>
+        <v>460.45</v>
       </c>
     </row>
     <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B187" s="1">
-        <v>43521</v>
+        <v>43526</v>
       </c>
       <c r="C187" s="5">
         <f t="shared" si="20"/>
-        <v>43521</v>
+        <v>43526</v>
+      </c>
+      <c r="D187" s="3">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E187" s="3">
+        <v>0.61458333333333337</v>
       </c>
       <c r="F187" s="2">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M187" s="4">
+        <v>2.25</v>
       </c>
       <c r="P187" s="20" t="s">
-        <v>119</v>
+        <v>125</v>
       </c>
       <c r="Q187">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R187" t="s">
         <v>282</v>
@@ -18462,11 +18757,103 @@
       </c>
       <c r="T187" s="4">
         <f t="shared" si="17"/>
-        <v>429.95</v>
+        <v>462.7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" s="1">
+        <v>43527</v>
+      </c>
+      <c r="C188" s="5">
+        <f t="shared" si="20"/>
+        <v>43527</v>
+      </c>
+      <c r="D188" s="3">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E188" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="F188" s="2">
+        <f t="shared" si="19"/>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="M188" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="P188" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q188">
+        <v>9</v>
+      </c>
+      <c r="R188" t="s">
+        <v>282</v>
+      </c>
+      <c r="S188">
+        <v>3</v>
+      </c>
+      <c r="T188" s="4">
+        <f t="shared" si="17"/>
+        <v>463.95</v>
+      </c>
+    </row>
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>10</v>
+      </c>
+      <c r="B189" s="1">
+        <v>43528</v>
+      </c>
+      <c r="C189" s="5">
+        <f t="shared" si="20"/>
+        <v>43528</v>
+      </c>
+      <c r="D189" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E189" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F189" s="2">
+        <f t="shared" si="19"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="G189" s="3">
+        <v>0.78125</v>
+      </c>
+      <c r="H189" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="I189" s="2">
+        <f>H189-G189</f>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="M189" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="P189" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q189">
+        <v>9</v>
+      </c>
+      <c r="R189" t="s">
+        <v>282</v>
+      </c>
+      <c r="S189">
+        <v>3</v>
+      </c>
+      <c r="T189" s="4">
+        <f t="shared" si="17"/>
+        <v>465.7</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T527">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T522">
     <cfRule type="expression" dxfId="17" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
@@ -18734,8 +19121,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Partial Update to 3/12
Remove stray files, including videos.
Need to update equations regarding break days.

Former-commit-id: 8de5d2a2da6bb0f69e85abfa86d4c3d28522e90f
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aNDREW\Desktop\ice-skating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8007C56-5160-4004-8553-BA8B4A4C38E4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CCC7BC0-EE78-4F6B-8196-A2058DB1676D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="8640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="38040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="358">
   <si>
     <t>Thursday</t>
   </si>
@@ -1187,6 +1187,12 @@
   </si>
   <si>
     <t>FS5</t>
+  </si>
+  <si>
+    <t>Landed Axel again!</t>
+  </si>
+  <si>
+    <t>Devon's FS5/FS6. Did interpretive and worked on spins and waltz loop</t>
   </si>
 </sst>
 </file>
@@ -1580,10 +1586,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$382</c:f>
+              <c:f>Data!$C$2:$C$379</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="381"/>
+                <c:ptCount val="378"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -2147,16 +2153,31 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>43528</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>43531</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>43532</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>43533</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>43534</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>43536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$382</c:f>
+              <c:f>Data!$M$2:$M$379</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="381"/>
+                <c:ptCount val="378"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2245,7 +2266,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.45</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>4</c:v>
@@ -2720,6 +2741,9 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3022,10 +3046,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$382</c:f>
+              <c:f>Data!$C$2:$C$379</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="381"/>
+                <c:ptCount val="378"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -3589,16 +3613,31 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>43528</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>43531</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>43532</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>43533</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>43534</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>43536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$382</c:f>
+              <c:f>Data!$Q$2:$Q$379</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="381"/>
+                <c:ptCount val="378"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4161,6 +4200,21 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="187">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="192">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -4559,7 +4613,7 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>38.200000000000003</c:v>
+                  <c:v>38.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>27.75</c:v>
@@ -4574,7 +4628,7 @@
                   <c:v>150.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4958,6 +5012,9 @@
                 <c:pt idx="7">
                   <c:v>66</c:v>
                 </c:pt>
+                <c:pt idx="8">
+                  <c:v>12</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5245,10 +5302,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$382</c:f>
+              <c:f>Data!$C$2:$C$379</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="381"/>
+                <c:ptCount val="378"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -5812,16 +5869,31 @@
                 </c:pt>
                 <c:pt idx="187">
                   <c:v>43528</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>43531</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>43532</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>43533</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>43534</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>43536</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$T$2:$T$382</c:f>
+              <c:f>Data!$T$2:$T$379</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="381"/>
+                <c:ptCount val="378"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -5910,481 +5982,496 @@
                   <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>72.45</c:v>
+                  <c:v>72.75</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>76.45</c:v>
+                  <c:v>76.75</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>78.2</c:v>
+                  <c:v>78.5</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>85.7</c:v>
+                  <c:v>86</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>88.7</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>89.7</c:v>
+                  <c:v>90</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>92.7</c:v>
+                  <c:v>93</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>95.2</c:v>
+                  <c:v>95.5</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>97.45</c:v>
+                  <c:v>97.75</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>99.95</c:v>
+                  <c:v>100.25</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>100.95</c:v>
+                  <c:v>101.25</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>104.2</c:v>
+                  <c:v>104.5</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>106.45</c:v>
+                  <c:v>106.75</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>114.2</c:v>
+                  <c:v>114.5</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>116.95</c:v>
+                  <c:v>117.25</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>117.7</c:v>
+                  <c:v>118</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>118.2</c:v>
+                  <c:v>118.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>121.95</c:v>
+                  <c:v>122.25</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>124.7</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>131.94999999999999</c:v>
+                  <c:v>132.25</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>135.44999999999999</c:v>
+                  <c:v>135.75</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>137.69999999999999</c:v>
+                  <c:v>138</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>138.44999999999999</c:v>
+                  <c:v>138.75</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>140.94999999999999</c:v>
+                  <c:v>141.25</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>144.69999999999999</c:v>
+                  <c:v>145</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>147.94999999999999</c:v>
+                  <c:v>148.25</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>150.44999999999999</c:v>
+                  <c:v>150.75</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>150.44999999999999</c:v>
+                  <c:v>150.75</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>150.94999999999999</c:v>
+                  <c:v>151.25</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>151.94999999999999</c:v>
+                  <c:v>152.25</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>153.69999999999999</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>159.69999999999999</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>163.19999999999999</c:v>
+                  <c:v>163.5</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>165.45</c:v>
+                  <c:v>165.75</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>166.2</c:v>
+                  <c:v>166.5</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>167.2</c:v>
+                  <c:v>167.5</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>167.95</c:v>
+                  <c:v>168.25</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>169.95</c:v>
+                  <c:v>170.25</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>173.95</c:v>
+                  <c:v>174.25</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>176.95</c:v>
+                  <c:v>177.25</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>178.7</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>181.7</c:v>
+                  <c:v>182</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>184.45</c:v>
+                  <c:v>184.75</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>184.7</c:v>
+                  <c:v>185</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>188.2</c:v>
+                  <c:v>188.5</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>190.95</c:v>
+                  <c:v>191.25</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>192.95</c:v>
+                  <c:v>193.25</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>196.45</c:v>
+                  <c:v>196.75</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>200.2</c:v>
+                  <c:v>200.5</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>204.45</c:v>
+                  <c:v>204.75</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>208.2</c:v>
+                  <c:v>208.5</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>210.95</c:v>
+                  <c:v>211.25</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>212.95</c:v>
+                  <c:v>213.25</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>217.7</c:v>
+                  <c:v>218</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>220.45</c:v>
+                  <c:v>220.75</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>224.7</c:v>
+                  <c:v>225</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>228.2</c:v>
+                  <c:v>228.5</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>230.2</c:v>
+                  <c:v>230.5</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>230.95</c:v>
+                  <c:v>231.25</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>233.2</c:v>
+                  <c:v>233.5</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>235.2</c:v>
+                  <c:v>235.5</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>238.95</c:v>
+                  <c:v>239.25</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>239.95</c:v>
+                  <c:v>240.25</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>240.95</c:v>
+                  <c:v>241.25</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>241.45</c:v>
+                  <c:v>241.75</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>241.95</c:v>
+                  <c:v>242.25</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>244.95</c:v>
+                  <c:v>245.25</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>248.95</c:v>
+                  <c:v>249.25</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>249.95</c:v>
+                  <c:v>250.25</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>257.95</c:v>
+                  <c:v>258.25</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>261.45</c:v>
+                  <c:v>261.75</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>262.2</c:v>
+                  <c:v>262.5</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>265.2</c:v>
+                  <c:v>265.5</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>269.7</c:v>
+                  <c:v>270</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>273.2</c:v>
+                  <c:v>273.5</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>278.45</c:v>
+                  <c:v>278.75</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>279.7</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>280.95</c:v>
+                  <c:v>281.25</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>283.95</c:v>
+                  <c:v>284.25</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>286.45</c:v>
+                  <c:v>286.75</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>293.2</c:v>
+                  <c:v>293.5</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>295.45</c:v>
+                  <c:v>295.75</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>296.45</c:v>
+                  <c:v>296.75</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>298.45</c:v>
+                  <c:v>298.75</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>299.45</c:v>
+                  <c:v>299.75</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>302.95</c:v>
+                  <c:v>303.25</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>304.2</c:v>
+                  <c:v>304.5</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>305.7</c:v>
+                  <c:v>306</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>306.7</c:v>
+                  <c:v>307</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>308.2</c:v>
+                  <c:v>308.5</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>312.2</c:v>
+                  <c:v>312.5</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>316.45</c:v>
+                  <c:v>316.75</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>319.95</c:v>
+                  <c:v>320.25</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>321.7</c:v>
+                  <c:v>322</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>323.45</c:v>
+                  <c:v>323.75</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>325.2</c:v>
+                  <c:v>325.5</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>328.7</c:v>
+                  <c:v>329</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>332.2</c:v>
+                  <c:v>332.5</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>335.45</c:v>
+                  <c:v>335.75</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>337.2</c:v>
+                  <c:v>337.5</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>344.95</c:v>
+                  <c:v>345.25</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>345.7</c:v>
+                  <c:v>346</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>347.7</c:v>
+                  <c:v>348</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>349.45</c:v>
+                  <c:v>349.75</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>354.45</c:v>
+                  <c:v>354.75</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>361.2</c:v>
+                  <c:v>361.5</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>363.45</c:v>
+                  <c:v>363.75</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>365.7</c:v>
+                  <c:v>366</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>367.7</c:v>
+                  <c:v>368</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>369.45</c:v>
+                  <c:v>369.75</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>371.45</c:v>
+                  <c:v>371.75</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>375.7</c:v>
+                  <c:v>376</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>377.95</c:v>
+                  <c:v>378.25</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>379.45</c:v>
+                  <c:v>379.75</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>381.95</c:v>
+                  <c:v>382.25</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>384.2</c:v>
+                  <c:v>384.5</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>387.2</c:v>
+                  <c:v>387.5</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>388.2</c:v>
+                  <c:v>388.5</c:v>
                 </c:pt>
                 <c:pt idx="147">
-                  <c:v>389.95</c:v>
+                  <c:v>390.25</c:v>
                 </c:pt>
                 <c:pt idx="148">
-                  <c:v>392.7</c:v>
+                  <c:v>393</c:v>
                 </c:pt>
                 <c:pt idx="149">
-                  <c:v>394.95</c:v>
+                  <c:v>395.25</c:v>
                 </c:pt>
                 <c:pt idx="150">
-                  <c:v>400.7</c:v>
+                  <c:v>401</c:v>
                 </c:pt>
                 <c:pt idx="151">
-                  <c:v>404.2</c:v>
+                  <c:v>404.5</c:v>
                 </c:pt>
                 <c:pt idx="152">
-                  <c:v>404.95</c:v>
+                  <c:v>405.25</c:v>
                 </c:pt>
                 <c:pt idx="153">
-                  <c:v>405.45</c:v>
+                  <c:v>405.75</c:v>
                 </c:pt>
                 <c:pt idx="154">
-                  <c:v>408.95</c:v>
+                  <c:v>409.25</c:v>
                 </c:pt>
                 <c:pt idx="155">
-                  <c:v>410.95</c:v>
+                  <c:v>411.25</c:v>
                 </c:pt>
                 <c:pt idx="156">
-                  <c:v>411.45</c:v>
+                  <c:v>411.75</c:v>
                 </c:pt>
                 <c:pt idx="157">
-                  <c:v>412.7</c:v>
+                  <c:v>413</c:v>
                 </c:pt>
                 <c:pt idx="158">
-                  <c:v>413.7</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="159">
-                  <c:v>416.45</c:v>
+                  <c:v>416.75</c:v>
                 </c:pt>
                 <c:pt idx="160">
-                  <c:v>417.45</c:v>
+                  <c:v>417.75</c:v>
                 </c:pt>
                 <c:pt idx="161">
-                  <c:v>419.2</c:v>
+                  <c:v>419.5</c:v>
                 </c:pt>
                 <c:pt idx="162">
-                  <c:v>423.7</c:v>
+                  <c:v>424</c:v>
                 </c:pt>
                 <c:pt idx="163">
-                  <c:v>425.95</c:v>
+                  <c:v>426.25</c:v>
                 </c:pt>
                 <c:pt idx="164">
-                  <c:v>426.95</c:v>
+                  <c:v>427.25</c:v>
                 </c:pt>
                 <c:pt idx="165">
-                  <c:v>429.2</c:v>
+                  <c:v>429.5</c:v>
                 </c:pt>
                 <c:pt idx="166">
-                  <c:v>430.7</c:v>
+                  <c:v>431</c:v>
                 </c:pt>
                 <c:pt idx="167">
-                  <c:v>432.45</c:v>
+                  <c:v>432.75</c:v>
                 </c:pt>
                 <c:pt idx="168">
-                  <c:v>437.45</c:v>
+                  <c:v>437.75</c:v>
                 </c:pt>
                 <c:pt idx="169">
-                  <c:v>439.2</c:v>
+                  <c:v>439.5</c:v>
                 </c:pt>
                 <c:pt idx="170">
-                  <c:v>440.2</c:v>
+                  <c:v>440.5</c:v>
                 </c:pt>
                 <c:pt idx="171">
-                  <c:v>441.45</c:v>
+                  <c:v>441.75</c:v>
                 </c:pt>
                 <c:pt idx="172">
-                  <c:v>441.7</c:v>
+                  <c:v>442</c:v>
                 </c:pt>
                 <c:pt idx="173">
-                  <c:v>441.95</c:v>
+                  <c:v>442.25</c:v>
                 </c:pt>
                 <c:pt idx="174">
-                  <c:v>442.45</c:v>
+                  <c:v>442.75</c:v>
                 </c:pt>
                 <c:pt idx="175">
-                  <c:v>443.45</c:v>
+                  <c:v>443.75</c:v>
                 </c:pt>
                 <c:pt idx="176">
-                  <c:v>445.45</c:v>
+                  <c:v>445.75</c:v>
                 </c:pt>
                 <c:pt idx="177">
-                  <c:v>446.45</c:v>
+                  <c:v>446.75</c:v>
                 </c:pt>
                 <c:pt idx="178">
-                  <c:v>450.7</c:v>
+                  <c:v>451</c:v>
                 </c:pt>
                 <c:pt idx="179">
-                  <c:v>452.7</c:v>
+                  <c:v>453</c:v>
                 </c:pt>
                 <c:pt idx="180">
-                  <c:v>453.7</c:v>
+                  <c:v>454</c:v>
                 </c:pt>
                 <c:pt idx="181">
-                  <c:v>454.95</c:v>
+                  <c:v>455.25</c:v>
                 </c:pt>
                 <c:pt idx="182">
-                  <c:v>455.45</c:v>
+                  <c:v>455.75</c:v>
                 </c:pt>
                 <c:pt idx="183">
-                  <c:v>458.95</c:v>
+                  <c:v>459.25</c:v>
                 </c:pt>
                 <c:pt idx="184">
-                  <c:v>460.45</c:v>
+                  <c:v>460.75</c:v>
                 </c:pt>
                 <c:pt idx="185">
-                  <c:v>462.7</c:v>
+                  <c:v>463</c:v>
                 </c:pt>
                 <c:pt idx="186">
-                  <c:v>463.95</c:v>
+                  <c:v>464.25</c:v>
                 </c:pt>
                 <c:pt idx="187">
-                  <c:v>465.7</c:v>
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>466</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>468</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>468</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9824,41 +9911,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z189"/>
+  <dimension ref="A1:Z194"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="G127" sqref="G127"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="5" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="11.7109375" style="3" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" style="2" customWidth="1"/>
-    <col min="10" max="11" width="11.7109375" style="3" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7265625" style="5" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="11.7265625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="11.7265625" style="2" customWidth="1"/>
+    <col min="10" max="11" width="11.7265625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="11.7265625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.7265625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="25.81640625" customWidth="1"/>
     <col min="15" max="15" width="21" customWidth="1"/>
     <col min="16" max="16" width="11" style="20" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" customWidth="1"/>
-    <col min="18" max="18" width="10.85546875" customWidth="1"/>
-    <col min="19" max="19" width="16.140625" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" customWidth="1"/>
-    <col min="22" max="22" width="20.42578125" customWidth="1"/>
-    <col min="23" max="23" width="24.85546875" customWidth="1"/>
-    <col min="24" max="24" width="16.5703125" customWidth="1"/>
+    <col min="17" max="17" width="9.453125" customWidth="1"/>
+    <col min="18" max="18" width="10.81640625" customWidth="1"/>
+    <col min="19" max="19" width="16.1796875" customWidth="1"/>
+    <col min="20" max="20" width="13.1796875" customWidth="1"/>
+    <col min="21" max="21" width="10.453125" customWidth="1"/>
+    <col min="22" max="22" width="20.453125" customWidth="1"/>
+    <col min="23" max="23" width="24.81640625" customWidth="1"/>
+    <col min="24" max="24" width="16.54296875" customWidth="1"/>
     <col min="25" max="25" width="13" customWidth="1"/>
-    <col min="26" max="27" width="16.7109375" customWidth="1"/>
+    <col min="26" max="27" width="16.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -9920,7 +10007,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -9973,7 +10060,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -10012,22 +10099,22 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M:M)</f>
-        <v>465.7</v>
+        <v>468</v>
       </c>
       <c r="V3" s="4">
-        <f>SUM(M152:M392)</f>
-        <v>70.75</v>
+        <f>SUM(M152:M389)</f>
+        <v>72.75</v>
       </c>
       <c r="W3" s="4">
         <f>SUM(M19:M151)</f>
-        <v>353.2</v>
+        <v>353.5</v>
       </c>
       <c r="X3" s="4">
         <f>SUM(M2:M18)</f>
         <v>41.75</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -10068,7 +10155,7 @@
         <v>7.75</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -10106,7 +10193,7 @@
         <v>11.25</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -10144,7 +10231,7 @@
         <v>13.25</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -10182,7 +10269,7 @@
         <v>14.25</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -10220,7 +10307,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -10258,7 +10345,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -10314,7 +10401,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -10371,7 +10458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -10428,7 +10515,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -10485,7 +10572,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -10530,7 +10617,7 @@
       </c>
       <c r="W14" s="4">
         <f>SUM(M18:M32)</f>
-        <v>38.200000000000003</v>
+        <v>38.5</v>
       </c>
       <c r="X14">
         <f>COUNTIF(P:P, "Gamma")</f>
@@ -10545,7 +10632,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -10602,7 +10689,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>1</v>
       </c>
@@ -10659,7 +10746,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -10730,7 +10817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -10782,15 +10869,15 @@
         <v>66</v>
       </c>
       <c r="Y18" s="14">
-        <f>C137-C117+1</f>
-        <v>32</v>
+        <f>C182-C117+1</f>
+        <v>93</v>
       </c>
       <c r="Z18" s="14">
         <f>Y18-X18</f>
-        <v>-34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -10834,11 +10921,15 @@
         <v>355</v>
       </c>
       <c r="W19" s="4">
-        <f>SUM(M183:M400)</f>
+        <f>SUM(M183:M397)</f>
+        <v>14</v>
+      </c>
+      <c r="X19">
+        <f>COUNTIF(P:P, "Freestyle 5")</f>
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -10876,7 +10967,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -10933,7 +11024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>1</v>
       </c>
@@ -10990,7 +11081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -11041,23 +11132,23 @@
         <v>282</v>
       </c>
       <c r="W23" s="4">
-        <f>SUM(M100:M381)</f>
-        <v>215.75</v>
+        <f>SUM(M100:M378)</f>
+        <v>217.75</v>
       </c>
       <c r="X23">
         <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="Y23" s="14">
         <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>121</v>
+        <v>129</v>
       </c>
       <c r="Z23" s="14">
         <f>Y23-X23</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>3</v>
       </c>
@@ -11098,7 +11189,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -11136,11 +11227,11 @@
         <v>60.5</v>
       </c>
       <c r="Z25">
-        <f>SUM(Z11:Z18)</f>
-        <v>-7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+        <f>SUM(Z11:Z19)</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -11178,7 +11269,7 @@
         <v>61.75</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -11219,7 +11310,7 @@
         <v>63.75</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -11270,7 +11361,7 @@
         <v>67.5</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>3</v>
       </c>
@@ -11311,7 +11402,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -11349,7 +11440,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -11371,7 +11462,7 @@
         <v>3.125E-2</v>
       </c>
       <c r="M31" s="4">
-        <v>0.45</v>
+        <v>0.75</v>
       </c>
       <c r="N31" t="s">
         <v>69</v>
@@ -11387,10 +11478,10 @@
       </c>
       <c r="T31" s="4">
         <f t="shared" si="2"/>
-        <v>72.45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
+        <v>72.75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -11428,10 +11519,10 @@
       </c>
       <c r="T32" s="4">
         <f t="shared" si="2"/>
-        <v>76.45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <v>76.75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -11476,10 +11567,10 @@
       </c>
       <c r="T33" s="4">
         <f t="shared" si="2"/>
-        <v>78.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <v>78.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -11524,10 +11615,10 @@
       </c>
       <c r="T34" s="4">
         <f t="shared" si="2"/>
-        <v>85.7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>3</v>
       </c>
@@ -11562,10 +11653,10 @@
       </c>
       <c r="T35" s="4">
         <f t="shared" ref="T35:T66" si="5">T34+M35</f>
-        <v>88.7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -11603,10 +11694,10 @@
       </c>
       <c r="T36" s="4">
         <f t="shared" si="5"/>
-        <v>89.7</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -11644,10 +11735,10 @@
       </c>
       <c r="T37" s="4">
         <f t="shared" si="5"/>
-        <v>92.7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>1</v>
       </c>
@@ -11682,10 +11773,10 @@
       </c>
       <c r="T38" s="4">
         <f t="shared" si="5"/>
-        <v>95.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>95.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -11723,10 +11814,10 @@
       </c>
       <c r="T39" s="4">
         <f t="shared" si="5"/>
-        <v>97.45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <v>97.75</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -11764,10 +11855,10 @@
       </c>
       <c r="T40" s="4">
         <f t="shared" si="5"/>
-        <v>99.95</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>100.25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>67</v>
       </c>
@@ -11802,10 +11893,10 @@
       </c>
       <c r="T41" s="4">
         <f t="shared" si="5"/>
-        <v>100.95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>101.25</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -11853,10 +11944,10 @@
       </c>
       <c r="T42" s="4">
         <f t="shared" si="5"/>
-        <v>104.2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <v>104.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>1</v>
       </c>
@@ -11894,10 +11985,10 @@
       </c>
       <c r="T43" s="4">
         <f t="shared" si="5"/>
-        <v>106.45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <v>106.75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -11955,10 +12046,10 @@
       </c>
       <c r="T44" s="4">
         <f t="shared" si="5"/>
-        <v>114.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+        <v>114.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -12006,10 +12097,10 @@
       </c>
       <c r="T45" s="4">
         <f t="shared" si="5"/>
-        <v>116.95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>117.25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>67</v>
       </c>
@@ -12047,10 +12138,10 @@
       </c>
       <c r="T46" s="4">
         <f t="shared" si="5"/>
-        <v>117.7</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>35</v>
       </c>
@@ -12088,10 +12179,10 @@
       </c>
       <c r="T47" s="4">
         <f t="shared" si="5"/>
-        <v>118.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+        <v>118.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -12129,10 +12220,10 @@
       </c>
       <c r="T48" s="4">
         <f t="shared" si="5"/>
-        <v>121.95</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+        <v>122.25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -12170,10 +12261,10 @@
       </c>
       <c r="T49" s="4">
         <f t="shared" si="5"/>
-        <v>124.7</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -12217,10 +12308,10 @@
       </c>
       <c r="T50" s="4">
         <f t="shared" si="5"/>
-        <v>131.94999999999999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+        <v>132.25</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>3</v>
       </c>
@@ -12264,10 +12355,10 @@
       </c>
       <c r="T51" s="4">
         <f t="shared" si="5"/>
-        <v>135.44999999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+        <v>135.75</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>10</v>
       </c>
@@ -12311,10 +12402,10 @@
       </c>
       <c r="T52" s="4">
         <f t="shared" si="5"/>
-        <v>137.69999999999999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>67</v>
       </c>
@@ -12358,10 +12449,10 @@
       </c>
       <c r="T53" s="4">
         <f t="shared" si="5"/>
-        <v>138.44999999999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+        <v>138.75</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>35</v>
       </c>
@@ -12405,10 +12496,10 @@
       </c>
       <c r="T54" s="4">
         <f t="shared" si="5"/>
-        <v>140.94999999999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+        <v>141.25</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -12452,10 +12543,10 @@
       </c>
       <c r="T55" s="4">
         <f t="shared" si="5"/>
-        <v>144.69999999999999</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>1</v>
       </c>
@@ -12499,10 +12590,10 @@
       </c>
       <c r="T56" s="4">
         <f t="shared" si="5"/>
-        <v>147.94999999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+        <v>148.25</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -12546,10 +12637,10 @@
       </c>
       <c r="T57" s="4">
         <f t="shared" si="5"/>
-        <v>150.44999999999999</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+        <v>150.75</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -12593,10 +12684,10 @@
       </c>
       <c r="T58" s="4">
         <f t="shared" si="5"/>
-        <v>150.44999999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+        <v>150.75</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>67</v>
       </c>
@@ -12640,10 +12731,10 @@
       </c>
       <c r="T59" s="4">
         <f t="shared" si="5"/>
-        <v>150.94999999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>151.25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -12681,10 +12772,10 @@
       </c>
       <c r="T60" s="4">
         <f t="shared" si="5"/>
-        <v>151.94999999999999</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+        <v>152.25</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>1</v>
       </c>
@@ -12728,10 +12819,10 @@
       </c>
       <c r="T61" s="4">
         <f t="shared" si="5"/>
-        <v>153.69999999999999</v>
-      </c>
-    </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -12785,10 +12876,10 @@
       </c>
       <c r="T62" s="4">
         <f t="shared" si="5"/>
-        <v>159.69999999999999</v>
-      </c>
-    </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>3</v>
       </c>
@@ -12832,10 +12923,10 @@
       </c>
       <c r="T63" s="4">
         <f t="shared" si="5"/>
-        <v>163.19999999999999</v>
-      </c>
-    </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+        <v>163.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>10</v>
       </c>
@@ -12879,10 +12970,10 @@
       </c>
       <c r="T64" s="4">
         <f t="shared" si="5"/>
-        <v>165.45</v>
-      </c>
-    </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+        <v>165.75</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>67</v>
       </c>
@@ -12926,10 +13017,10 @@
       </c>
       <c r="T65" s="4">
         <f t="shared" si="5"/>
-        <v>166.2</v>
-      </c>
-    </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+        <v>166.5</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -12973,10 +13064,10 @@
       </c>
       <c r="T66" s="4">
         <f t="shared" si="5"/>
-        <v>167.2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+        <v>167.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>1</v>
       </c>
@@ -13020,10 +13111,10 @@
       </c>
       <c r="T67" s="4">
         <f t="shared" ref="T67:T130" si="7">T66+M67</f>
-        <v>167.95</v>
-      </c>
-    </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+        <v>168.25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -13067,10 +13158,10 @@
       </c>
       <c r="T68" s="4">
         <f t="shared" si="7"/>
-        <v>169.95</v>
-      </c>
-    </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+        <v>170.25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>3</v>
       </c>
@@ -13114,10 +13205,10 @@
       </c>
       <c r="T69" s="4">
         <f t="shared" si="7"/>
-        <v>173.95</v>
-      </c>
-    </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+        <v>174.25</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>10</v>
       </c>
@@ -13161,10 +13252,10 @@
       </c>
       <c r="T70" s="4">
         <f t="shared" si="7"/>
-        <v>176.95</v>
-      </c>
-    </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+        <v>177.25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>67</v>
       </c>
@@ -13208,10 +13299,10 @@
       </c>
       <c r="T71" s="4">
         <f t="shared" si="7"/>
-        <v>178.7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>35</v>
       </c>
@@ -13255,10 +13346,10 @@
       </c>
       <c r="T72" s="4">
         <f t="shared" si="7"/>
-        <v>181.7</v>
-      </c>
-    </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -13312,10 +13403,10 @@
       </c>
       <c r="T73" s="4">
         <f t="shared" si="7"/>
-        <v>184.45</v>
-      </c>
-    </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+        <v>184.75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -13359,10 +13450,10 @@
       </c>
       <c r="T74" s="4">
         <f t="shared" si="7"/>
-        <v>184.7</v>
-      </c>
-    </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>3</v>
       </c>
@@ -13406,10 +13497,10 @@
       </c>
       <c r="T75" s="4">
         <f t="shared" si="7"/>
-        <v>188.2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+        <v>188.5</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>10</v>
       </c>
@@ -13463,10 +13554,10 @@
       </c>
       <c r="T76" s="4">
         <f t="shared" si="7"/>
-        <v>190.95</v>
-      </c>
-    </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+        <v>191.25</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>35</v>
       </c>
@@ -13510,10 +13601,10 @@
       </c>
       <c r="T77" s="4">
         <f t="shared" si="7"/>
-        <v>192.95</v>
-      </c>
-    </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+        <v>193.25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -13567,10 +13658,10 @@
       </c>
       <c r="T78" s="4">
         <f t="shared" si="7"/>
-        <v>196.45</v>
-      </c>
-    </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+        <v>196.75</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>1</v>
       </c>
@@ -13614,10 +13705,10 @@
       </c>
       <c r="T79" s="4">
         <f t="shared" si="7"/>
-        <v>200.2</v>
-      </c>
-    </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+        <v>200.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -13661,10 +13752,10 @@
       </c>
       <c r="T80" s="4">
         <f t="shared" si="7"/>
-        <v>204.45</v>
-      </c>
-    </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+        <v>204.75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>3</v>
       </c>
@@ -13708,10 +13799,10 @@
       </c>
       <c r="T81" s="4">
         <f t="shared" si="7"/>
-        <v>208.2</v>
-      </c>
-    </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+        <v>208.5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>10</v>
       </c>
@@ -13775,10 +13866,10 @@
       </c>
       <c r="T82" s="4">
         <f t="shared" si="7"/>
-        <v>210.95</v>
-      </c>
-    </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+        <v>211.25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>35</v>
       </c>
@@ -13822,10 +13913,10 @@
       </c>
       <c r="T83" s="4">
         <f t="shared" si="7"/>
-        <v>212.95</v>
-      </c>
-    </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+        <v>213.25</v>
+      </c>
+    </row>
+    <row r="84" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -13869,10 +13960,10 @@
       </c>
       <c r="T84" s="4">
         <f t="shared" si="7"/>
-        <v>217.7</v>
-      </c>
-    </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="85" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>1</v>
       </c>
@@ -13916,10 +14007,10 @@
       </c>
       <c r="T85" s="4">
         <f t="shared" si="7"/>
-        <v>220.45</v>
-      </c>
-    </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+        <v>220.75</v>
+      </c>
+    </row>
+    <row r="86" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -13960,10 +14051,10 @@
       </c>
       <c r="T86" s="4">
         <f t="shared" si="7"/>
-        <v>224.7</v>
-      </c>
-    </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="87" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>3</v>
       </c>
@@ -14004,10 +14095,10 @@
       </c>
       <c r="T87" s="4">
         <f t="shared" si="7"/>
-        <v>228.2</v>
-      </c>
-    </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+        <v>228.5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>10</v>
       </c>
@@ -14058,10 +14149,10 @@
       </c>
       <c r="T88" s="4">
         <f t="shared" si="7"/>
-        <v>230.2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+        <v>230.5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>35</v>
       </c>
@@ -14105,10 +14196,10 @@
       </c>
       <c r="T89" s="4">
         <f t="shared" si="7"/>
-        <v>230.95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+        <v>231.25</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -14162,10 +14253,10 @@
       </c>
       <c r="T90" s="4">
         <f t="shared" si="7"/>
-        <v>233.2</v>
-      </c>
-    </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+        <v>233.5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>1</v>
       </c>
@@ -14209,10 +14300,10 @@
       </c>
       <c r="T91" s="4">
         <f t="shared" si="7"/>
-        <v>235.2</v>
-      </c>
-    </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+        <v>235.5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -14266,10 +14357,10 @@
       </c>
       <c r="T92" s="4">
         <f t="shared" si="7"/>
-        <v>238.95</v>
-      </c>
-    </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+        <v>239.25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>3</v>
       </c>
@@ -14313,10 +14404,10 @@
       </c>
       <c r="T93" s="4">
         <f t="shared" si="7"/>
-        <v>239.95</v>
-      </c>
-    </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+        <v>240.25</v>
+      </c>
+    </row>
+    <row r="94" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>10</v>
       </c>
@@ -14360,10 +14451,10 @@
       </c>
       <c r="T94" s="4">
         <f t="shared" si="7"/>
-        <v>240.95</v>
-      </c>
-    </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+        <v>241.25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>67</v>
       </c>
@@ -14407,10 +14498,10 @@
       </c>
       <c r="T95" s="4">
         <f t="shared" si="7"/>
-        <v>241.45</v>
-      </c>
-    </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+        <v>241.75</v>
+      </c>
+    </row>
+    <row r="96" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>67</v>
       </c>
@@ -14454,10 +14545,10 @@
       </c>
       <c r="T96" s="4">
         <f t="shared" si="7"/>
-        <v>241.95</v>
-      </c>
-    </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+        <v>242.25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>35</v>
       </c>
@@ -14501,10 +14592,10 @@
       </c>
       <c r="T97" s="4">
         <f t="shared" si="7"/>
-        <v>244.95</v>
-      </c>
-    </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+        <v>245.25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -14545,10 +14636,10 @@
       </c>
       <c r="T98" s="4">
         <f t="shared" si="7"/>
-        <v>248.95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+        <v>249.25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>1</v>
       </c>
@@ -14592,10 +14683,10 @@
       </c>
       <c r="T99" s="4">
         <f t="shared" si="7"/>
-        <v>249.95</v>
-      </c>
-    </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+        <v>250.25</v>
+      </c>
+    </row>
+    <row r="100" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -14639,10 +14730,10 @@
       </c>
       <c r="T100" s="4">
         <f t="shared" si="7"/>
-        <v>257.95</v>
-      </c>
-    </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+        <v>258.25</v>
+      </c>
+    </row>
+    <row r="101" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>3</v>
       </c>
@@ -14683,10 +14774,10 @@
       </c>
       <c r="T101" s="4">
         <f t="shared" si="7"/>
-        <v>261.45</v>
-      </c>
-    </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+        <v>261.75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>67</v>
       </c>
@@ -14730,10 +14821,10 @@
       </c>
       <c r="T102" s="4">
         <f t="shared" si="7"/>
-        <v>262.2</v>
-      </c>
-    </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+        <v>262.5</v>
+      </c>
+    </row>
+    <row r="103" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>35</v>
       </c>
@@ -14777,10 +14868,10 @@
       </c>
       <c r="T103" s="4">
         <f t="shared" si="7"/>
-        <v>265.2</v>
-      </c>
-    </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+        <v>265.5</v>
+      </c>
+    </row>
+    <row r="104" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -14834,10 +14925,10 @@
       </c>
       <c r="T104" s="4">
         <f t="shared" si="7"/>
-        <v>269.7</v>
-      </c>
-    </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="105" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>1</v>
       </c>
@@ -14891,10 +14982,10 @@
       </c>
       <c r="T105" s="4">
         <f t="shared" si="7"/>
-        <v>273.2</v>
-      </c>
-    </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+        <v>273.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -14938,10 +15029,10 @@
       </c>
       <c r="T106" s="4">
         <f t="shared" si="7"/>
-        <v>278.45</v>
-      </c>
-    </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+        <v>278.75</v>
+      </c>
+    </row>
+    <row r="107" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>3</v>
       </c>
@@ -14985,10 +15076,10 @@
       </c>
       <c r="T107" s="4">
         <f t="shared" si="7"/>
-        <v>279.7</v>
-      </c>
-    </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="108" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>67</v>
       </c>
@@ -15032,10 +15123,10 @@
       </c>
       <c r="T108" s="4">
         <f t="shared" si="7"/>
-        <v>280.95</v>
-      </c>
-    </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+        <v>281.25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>35</v>
       </c>
@@ -15079,10 +15170,10 @@
       </c>
       <c r="T109" s="4">
         <f t="shared" si="7"/>
-        <v>283.95</v>
-      </c>
-    </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+        <v>284.25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -15136,10 +15227,10 @@
       </c>
       <c r="T110" s="4">
         <f t="shared" si="7"/>
-        <v>286.45</v>
-      </c>
-    </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+        <v>286.75</v>
+      </c>
+    </row>
+    <row r="111" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -15203,10 +15294,10 @@
       </c>
       <c r="T111" s="4">
         <f t="shared" si="7"/>
-        <v>293.2</v>
-      </c>
-    </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+        <v>293.5</v>
+      </c>
+    </row>
+    <row r="112" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>3</v>
       </c>
@@ -15247,10 +15338,10 @@
       </c>
       <c r="T112" s="4">
         <f t="shared" si="7"/>
-        <v>295.45</v>
-      </c>
-    </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+        <v>295.75</v>
+      </c>
+    </row>
+    <row r="113" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>67</v>
       </c>
@@ -15294,10 +15385,10 @@
       </c>
       <c r="T113" s="4">
         <f t="shared" si="7"/>
-        <v>296.45</v>
-      </c>
-    </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+        <v>296.75</v>
+      </c>
+    </row>
+    <row r="114" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>35</v>
       </c>
@@ -15341,10 +15432,10 @@
       </c>
       <c r="T114" s="4">
         <f t="shared" si="7"/>
-        <v>298.45</v>
-      </c>
-    </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+        <v>298.75</v>
+      </c>
+    </row>
+    <row r="115" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>1</v>
       </c>
@@ -15388,10 +15479,10 @@
       </c>
       <c r="T115" s="4">
         <f t="shared" si="7"/>
-        <v>299.45</v>
-      </c>
-    </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+        <v>299.75</v>
+      </c>
+    </row>
+    <row r="116" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>2</v>
       </c>
@@ -15455,10 +15546,10 @@
       </c>
       <c r="T116" s="4">
         <f t="shared" si="7"/>
-        <v>302.95</v>
-      </c>
-    </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+        <v>303.25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>3</v>
       </c>
@@ -15502,10 +15593,10 @@
       </c>
       <c r="T117" s="4">
         <f t="shared" si="7"/>
-        <v>304.2</v>
-      </c>
-    </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+        <v>304.5</v>
+      </c>
+    </row>
+    <row r="118" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>10</v>
       </c>
@@ -15549,10 +15640,10 @@
       </c>
       <c r="T118" s="4">
         <f t="shared" si="7"/>
-        <v>305.7</v>
-      </c>
-    </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="119" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>67</v>
       </c>
@@ -15596,10 +15687,10 @@
       </c>
       <c r="T119" s="4">
         <f t="shared" si="7"/>
-        <v>306.7</v>
-      </c>
-    </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="120" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>35</v>
       </c>
@@ -15640,10 +15731,10 @@
       </c>
       <c r="T120" s="4">
         <f t="shared" si="7"/>
-        <v>308.2</v>
-      </c>
-    </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+        <v>308.5</v>
+      </c>
+    </row>
+    <row r="121" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>0</v>
       </c>
@@ -15684,10 +15775,10 @@
       </c>
       <c r="T121" s="4">
         <f t="shared" si="7"/>
-        <v>312.2</v>
-      </c>
-    </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+        <v>312.5</v>
+      </c>
+    </row>
+    <row r="122" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>2</v>
       </c>
@@ -15740,10 +15831,10 @@
       </c>
       <c r="T122" s="4">
         <f t="shared" si="7"/>
-        <v>316.45</v>
-      </c>
-    </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+        <v>316.75</v>
+      </c>
+    </row>
+    <row r="123" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>10</v>
       </c>
@@ -15787,10 +15878,10 @@
       </c>
       <c r="T123" s="4">
         <f t="shared" si="7"/>
-        <v>319.95</v>
-      </c>
-    </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+        <v>320.25</v>
+      </c>
+    </row>
+    <row r="124" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>35</v>
       </c>
@@ -15834,10 +15925,10 @@
       </c>
       <c r="T124" s="4">
         <f t="shared" si="7"/>
-        <v>321.7</v>
-      </c>
-    </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="125" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -15881,10 +15972,10 @@
       </c>
       <c r="T125" s="4">
         <f t="shared" si="7"/>
-        <v>323.45</v>
-      </c>
-    </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+        <v>323.75</v>
+      </c>
+    </row>
+    <row r="126" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>1</v>
       </c>
@@ -15928,10 +16019,10 @@
       </c>
       <c r="T126" s="4">
         <f t="shared" si="7"/>
-        <v>325.2</v>
-      </c>
-    </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+        <v>325.5</v>
+      </c>
+    </row>
+    <row r="127" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>2</v>
       </c>
@@ -15985,10 +16076,10 @@
       </c>
       <c r="T127" s="4">
         <f t="shared" si="7"/>
-        <v>328.7</v>
-      </c>
-    </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="128" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>3</v>
       </c>
@@ -16042,10 +16133,10 @@
       </c>
       <c r="T128" s="4">
         <f t="shared" si="7"/>
-        <v>332.2</v>
-      </c>
-    </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+        <v>332.5</v>
+      </c>
+    </row>
+    <row r="129" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>0</v>
       </c>
@@ -16086,10 +16177,10 @@
       </c>
       <c r="T129" s="4">
         <f t="shared" si="7"/>
-        <v>335.45</v>
-      </c>
-    </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+        <v>335.75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>1</v>
       </c>
@@ -16130,10 +16221,10 @@
       </c>
       <c r="T130" s="4">
         <f t="shared" si="7"/>
-        <v>337.2</v>
-      </c>
-    </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+        <v>337.5</v>
+      </c>
+    </row>
+    <row r="131" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>3</v>
       </c>
@@ -16176,11 +16267,11 @@
         <v>3</v>
       </c>
       <c r="T131" s="4">
-        <f t="shared" ref="T131:T189" si="17">T130+M131</f>
-        <v>344.95</v>
-      </c>
-    </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+        <f t="shared" ref="T131:T194" si="17">T130+M131</f>
+        <v>345.25</v>
+      </c>
+    </row>
+    <row r="132" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>67</v>
       </c>
@@ -16221,10 +16312,10 @@
       </c>
       <c r="T132" s="4">
         <f t="shared" si="17"/>
-        <v>345.7</v>
-      </c>
-    </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="133" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>35</v>
       </c>
@@ -16268,10 +16359,10 @@
       </c>
       <c r="T133" s="4">
         <f t="shared" si="17"/>
-        <v>347.7</v>
-      </c>
-    </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="134" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>1</v>
       </c>
@@ -16312,10 +16403,10 @@
       </c>
       <c r="T134" s="4">
         <f t="shared" si="17"/>
-        <v>349.45</v>
-      </c>
-    </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+        <v>349.75</v>
+      </c>
+    </row>
+    <row r="135" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>2</v>
       </c>
@@ -16333,7 +16424,7 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="F135" s="2">
-        <f t="shared" ref="F135:F189" si="19">E135-D135</f>
+        <f t="shared" ref="F135:F193" si="19">E135-D135</f>
         <v>0.125</v>
       </c>
       <c r="G135" s="3">
@@ -16369,10 +16460,10 @@
       </c>
       <c r="T135" s="4">
         <f t="shared" si="17"/>
-        <v>354.45</v>
-      </c>
-    </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+        <v>354.75</v>
+      </c>
+    </row>
+    <row r="136" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>10</v>
       </c>
@@ -16426,10 +16517,10 @@
       </c>
       <c r="T136" s="4">
         <f t="shared" si="17"/>
-        <v>361.2</v>
-      </c>
-    </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+        <v>361.5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>35</v>
       </c>
@@ -16483,10 +16574,10 @@
       </c>
       <c r="T137" s="4">
         <f t="shared" si="17"/>
-        <v>363.45</v>
-      </c>
-    </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+        <v>363.75</v>
+      </c>
+    </row>
+    <row r="138" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>0</v>
       </c>
@@ -16530,10 +16621,10 @@
       </c>
       <c r="T138" s="4">
         <f t="shared" si="17"/>
-        <v>365.7</v>
-      </c>
-    </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="139" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>1</v>
       </c>
@@ -16584,10 +16675,10 @@
       </c>
       <c r="T139" s="4">
         <f t="shared" si="17"/>
-        <v>367.7</v>
-      </c>
-    </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="140" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>2</v>
       </c>
@@ -16628,10 +16719,10 @@
       </c>
       <c r="T140" s="4">
         <f t="shared" si="17"/>
-        <v>369.45</v>
-      </c>
-    </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
+        <v>369.75</v>
+      </c>
+    </row>
+    <row r="141" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>3</v>
       </c>
@@ -16672,10 +16763,10 @@
       </c>
       <c r="T141" s="4">
         <f t="shared" si="17"/>
-        <v>371.45</v>
-      </c>
-    </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
+        <v>371.75</v>
+      </c>
+    </row>
+    <row r="142" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>10</v>
       </c>
@@ -16716,10 +16807,10 @@
       </c>
       <c r="T142" s="4">
         <f t="shared" si="17"/>
-        <v>375.7</v>
-      </c>
-    </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="143" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>67</v>
       </c>
@@ -16760,10 +16851,10 @@
       </c>
       <c r="T143" s="4">
         <f t="shared" si="17"/>
-        <v>377.95</v>
-      </c>
-    </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
+        <v>378.25</v>
+      </c>
+    </row>
+    <row r="144" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>0</v>
       </c>
@@ -16801,10 +16892,10 @@
       </c>
       <c r="T144" s="4">
         <f t="shared" si="17"/>
-        <v>379.45</v>
-      </c>
-    </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
+        <v>379.75</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>3</v>
       </c>
@@ -16855,10 +16946,10 @@
       </c>
       <c r="T145" s="4">
         <f t="shared" si="17"/>
-        <v>381.95</v>
-      </c>
-    </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
+        <v>382.25</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>10</v>
       </c>
@@ -16896,10 +16987,10 @@
       </c>
       <c r="T146" s="4">
         <f t="shared" si="17"/>
-        <v>384.2</v>
-      </c>
-    </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
+        <v>384.5</v>
+      </c>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>35</v>
       </c>
@@ -16937,10 +17028,10 @@
       </c>
       <c r="T147" s="4">
         <f t="shared" si="17"/>
-        <v>387.2</v>
-      </c>
-    </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
+        <v>387.5</v>
+      </c>
+    </row>
+    <row r="148" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>0</v>
       </c>
@@ -16978,10 +17069,10 @@
       </c>
       <c r="T148" s="4">
         <f t="shared" si="17"/>
-        <v>388.2</v>
-      </c>
-    </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
+        <v>388.5</v>
+      </c>
+    </row>
+    <row r="149" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>1</v>
       </c>
@@ -17019,10 +17110,10 @@
       </c>
       <c r="T149" s="4">
         <f t="shared" si="17"/>
-        <v>389.95</v>
-      </c>
-    </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
+        <v>390.25</v>
+      </c>
+    </row>
+    <row r="150" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>2</v>
       </c>
@@ -17060,10 +17151,10 @@
       </c>
       <c r="T150" s="4">
         <f t="shared" si="17"/>
-        <v>392.7</v>
-      </c>
-    </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="151" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>3</v>
       </c>
@@ -17104,10 +17195,10 @@
       </c>
       <c r="T151" s="4">
         <f t="shared" si="17"/>
-        <v>394.95</v>
-      </c>
-    </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
+        <v>395.25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>2</v>
       </c>
@@ -17148,10 +17239,10 @@
       </c>
       <c r="T152" s="4">
         <f t="shared" si="17"/>
-        <v>400.7</v>
-      </c>
-    </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="153" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>3</v>
       </c>
@@ -17192,10 +17283,10 @@
       </c>
       <c r="T153" s="4">
         <f t="shared" si="17"/>
-        <v>404.2</v>
-      </c>
-    </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
+        <v>404.5</v>
+      </c>
+    </row>
+    <row r="154" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>67</v>
       </c>
@@ -17236,10 +17327,10 @@
       </c>
       <c r="T154" s="4">
         <f t="shared" si="17"/>
-        <v>404.95</v>
-      </c>
-    </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
+        <v>405.25</v>
+      </c>
+    </row>
+    <row r="155" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>0</v>
       </c>
@@ -17280,10 +17371,10 @@
       </c>
       <c r="T155" s="4">
         <f t="shared" si="17"/>
-        <v>405.45</v>
-      </c>
-    </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
+        <v>405.75</v>
+      </c>
+    </row>
+    <row r="156" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>1</v>
       </c>
@@ -17324,10 +17415,10 @@
       </c>
       <c r="T156" s="4">
         <f t="shared" si="17"/>
-        <v>408.95</v>
-      </c>
-    </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
+        <v>409.25</v>
+      </c>
+    </row>
+    <row r="157" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>2</v>
       </c>
@@ -17368,10 +17459,10 @@
       </c>
       <c r="T157" s="4">
         <f t="shared" si="17"/>
-        <v>410.95</v>
-      </c>
-    </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
+        <v>411.25</v>
+      </c>
+    </row>
+    <row r="158" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>3</v>
       </c>
@@ -17412,10 +17503,10 @@
       </c>
       <c r="T158" s="4">
         <f t="shared" si="17"/>
-        <v>411.45</v>
-      </c>
-    </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
+        <v>411.75</v>
+      </c>
+    </row>
+    <row r="159" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>10</v>
       </c>
@@ -17456,10 +17547,10 @@
       </c>
       <c r="T159" s="4">
         <f t="shared" si="17"/>
-        <v>412.7</v>
-      </c>
-    </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="160" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>67</v>
       </c>
@@ -17503,10 +17594,10 @@
       </c>
       <c r="T160" s="4">
         <f t="shared" si="17"/>
-        <v>413.7</v>
-      </c>
-    </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="161" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>35</v>
       </c>
@@ -17550,10 +17641,10 @@
       </c>
       <c r="T161" s="4">
         <f t="shared" si="17"/>
-        <v>416.45</v>
-      </c>
-    </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
+        <v>416.75</v>
+      </c>
+    </row>
+    <row r="162" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>0</v>
       </c>
@@ -17594,10 +17685,10 @@
       </c>
       <c r="T162" s="4">
         <f t="shared" si="17"/>
-        <v>417.45</v>
-      </c>
-    </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
+        <v>417.75</v>
+      </c>
+    </row>
+    <row r="163" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>1</v>
       </c>
@@ -17648,10 +17739,10 @@
       </c>
       <c r="T163" s="4">
         <f t="shared" si="17"/>
-        <v>419.2</v>
-      </c>
-    </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
+        <v>419.5</v>
+      </c>
+    </row>
+    <row r="164" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
         <v>2</v>
       </c>
@@ -17702,10 +17793,10 @@
       </c>
       <c r="T164" s="4">
         <f t="shared" si="17"/>
-        <v>423.7</v>
-      </c>
-    </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="165" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>3</v>
       </c>
@@ -17713,7 +17804,7 @@
         <v>43499</v>
       </c>
       <c r="C165" s="5">
-        <f t="shared" ref="C165:C189" si="20">B165</f>
+        <f t="shared" ref="C165:C194" si="20">B165</f>
         <v>43499</v>
       </c>
       <c r="D165" s="3">
@@ -17749,10 +17840,10 @@
       </c>
       <c r="T165" s="4">
         <f t="shared" si="17"/>
-        <v>425.95</v>
-      </c>
-    </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
+        <v>426.25</v>
+      </c>
+    </row>
+    <row r="166" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>67</v>
       </c>
@@ -17796,10 +17887,10 @@
       </c>
       <c r="T166" s="4">
         <f t="shared" si="17"/>
-        <v>426.95</v>
-      </c>
-    </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
+        <v>427.25</v>
+      </c>
+    </row>
+    <row r="167" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>35</v>
       </c>
@@ -17853,10 +17944,10 @@
       </c>
       <c r="T167" s="4">
         <f t="shared" si="17"/>
-        <v>429.2</v>
-      </c>
-    </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
+        <v>429.5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>0</v>
       </c>
@@ -17900,10 +17991,10 @@
       </c>
       <c r="T168" s="4">
         <f t="shared" si="17"/>
-        <v>430.7</v>
-      </c>
-    </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="169" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>1</v>
       </c>
@@ -17957,10 +18048,10 @@
       </c>
       <c r="T169" s="4">
         <f t="shared" si="17"/>
-        <v>432.45</v>
-      </c>
-    </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
+        <v>432.75</v>
+      </c>
+    </row>
+    <row r="170" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>2</v>
       </c>
@@ -18004,10 +18095,10 @@
       </c>
       <c r="T170" s="4">
         <f t="shared" si="17"/>
-        <v>437.45</v>
-      </c>
-    </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
+        <v>437.75</v>
+      </c>
+    </row>
+    <row r="171" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>3</v>
       </c>
@@ -18048,10 +18139,10 @@
       </c>
       <c r="T171" s="4">
         <f t="shared" si="17"/>
-        <v>439.2</v>
-      </c>
-    </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
+        <v>439.5</v>
+      </c>
+    </row>
+    <row r="172" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>10</v>
       </c>
@@ -18092,10 +18183,10 @@
       </c>
       <c r="T172" s="4">
         <f t="shared" si="17"/>
-        <v>440.2</v>
-      </c>
-    </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
+        <v>440.5</v>
+      </c>
+    </row>
+    <row r="173" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>67</v>
       </c>
@@ -18136,10 +18227,10 @@
       </c>
       <c r="T173" s="4">
         <f t="shared" si="17"/>
-        <v>441.45</v>
-      </c>
-    </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
+        <v>441.75</v>
+      </c>
+    </row>
+    <row r="174" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>1</v>
       </c>
@@ -18180,10 +18271,10 @@
       </c>
       <c r="T174" s="4">
         <f t="shared" si="17"/>
-        <v>441.7</v>
-      </c>
-    </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="175" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>2</v>
       </c>
@@ -18224,10 +18315,10 @@
       </c>
       <c r="T175" s="4">
         <f t="shared" si="17"/>
-        <v>441.95</v>
-      </c>
-    </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
+        <v>442.25</v>
+      </c>
+    </row>
+    <row r="176" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>3</v>
       </c>
@@ -18268,10 +18359,10 @@
       </c>
       <c r="T176" s="4">
         <f t="shared" si="17"/>
-        <v>442.45</v>
-      </c>
-    </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
+        <v>442.75</v>
+      </c>
+    </row>
+    <row r="177" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>67</v>
       </c>
@@ -18309,10 +18400,10 @@
       </c>
       <c r="T177" s="4">
         <f t="shared" si="17"/>
-        <v>443.45</v>
-      </c>
-    </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
+        <v>443.75</v>
+      </c>
+    </row>
+    <row r="178" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>35</v>
       </c>
@@ -18350,10 +18441,10 @@
       </c>
       <c r="T178" s="4">
         <f t="shared" si="17"/>
-        <v>445.45</v>
-      </c>
-    </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
+        <v>445.75</v>
+      </c>
+    </row>
+    <row r="179" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>0</v>
       </c>
@@ -18391,10 +18482,10 @@
       </c>
       <c r="T179" s="4">
         <f t="shared" si="17"/>
-        <v>446.45</v>
-      </c>
-    </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
+        <v>446.75</v>
+      </c>
+    </row>
+    <row r="180" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>1</v>
       </c>
@@ -18438,10 +18529,10 @@
       </c>
       <c r="T180" s="4">
         <f t="shared" si="17"/>
-        <v>450.7</v>
-      </c>
-    </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="181" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>3</v>
       </c>
@@ -18485,10 +18576,10 @@
       </c>
       <c r="T181" s="4">
         <f t="shared" si="17"/>
-        <v>452.7</v>
-      </c>
-    </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="182" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>10</v>
       </c>
@@ -18526,10 +18617,10 @@
       </c>
       <c r="T182" s="4">
         <f t="shared" si="17"/>
-        <v>453.7</v>
-      </c>
-    </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="183" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>67</v>
       </c>
@@ -18580,10 +18671,10 @@
       </c>
       <c r="T183" s="4">
         <f t="shared" si="17"/>
-        <v>454.95</v>
-      </c>
-    </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
+        <v>455.25</v>
+      </c>
+    </row>
+    <row r="184" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>35</v>
       </c>
@@ -18624,10 +18715,10 @@
       </c>
       <c r="T184" s="4">
         <f t="shared" si="17"/>
-        <v>455.45</v>
-      </c>
-    </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
+        <v>455.75</v>
+      </c>
+    </row>
+    <row r="185" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>0</v>
       </c>
@@ -18675,10 +18766,10 @@
       </c>
       <c r="T185" s="4">
         <f t="shared" si="17"/>
-        <v>458.95</v>
-      </c>
-    </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
+        <v>459.25</v>
+      </c>
+    </row>
+    <row r="186" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>1</v>
       </c>
@@ -18716,10 +18807,10 @@
       </c>
       <c r="T186" s="4">
         <f t="shared" si="17"/>
-        <v>460.45</v>
-      </c>
-    </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
+        <v>460.75</v>
+      </c>
+    </row>
+    <row r="187" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>2</v>
       </c>
@@ -18757,10 +18848,10 @@
       </c>
       <c r="T187" s="4">
         <f t="shared" si="17"/>
-        <v>462.7</v>
-      </c>
-    </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="188" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>3</v>
       </c>
@@ -18798,10 +18889,10 @@
       </c>
       <c r="T188" s="4">
         <f t="shared" si="17"/>
-        <v>463.95</v>
-      </c>
-    </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
+        <v>464.25</v>
+      </c>
+    </row>
+    <row r="189" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>10</v>
       </c>
@@ -18849,11 +18940,194 @@
       </c>
       <c r="T189" s="4">
         <f t="shared" si="17"/>
-        <v>465.7</v>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="190" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A190" t="s">
+        <v>0</v>
+      </c>
+      <c r="B190" s="1">
+        <v>43531</v>
+      </c>
+      <c r="C190" s="5">
+        <f t="shared" si="20"/>
+        <v>43531</v>
+      </c>
+      <c r="D190" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F190" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.6875</v>
+      </c>
+      <c r="G190" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="P190" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q190">
+        <v>9</v>
+      </c>
+      <c r="R190" t="s">
+        <v>282</v>
+      </c>
+      <c r="S190">
+        <v>3</v>
+      </c>
+      <c r="T190" s="4">
+        <f t="shared" si="17"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="191" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A191" t="s">
+        <v>1</v>
+      </c>
+      <c r="B191" s="1">
+        <v>43532</v>
+      </c>
+      <c r="C191" s="5">
+        <f t="shared" si="20"/>
+        <v>43532</v>
+      </c>
+      <c r="D191" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F191" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.8125</v>
+      </c>
+      <c r="P191" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q191">
+        <v>9</v>
+      </c>
+      <c r="R191" t="s">
+        <v>282</v>
+      </c>
+      <c r="S191">
+        <v>3</v>
+      </c>
+      <c r="T191" s="4">
+        <f t="shared" si="17"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="192" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A192" t="s">
+        <v>2</v>
+      </c>
+      <c r="B192" s="1">
+        <v>43533</v>
+      </c>
+      <c r="C192" s="5">
+        <f t="shared" si="20"/>
+        <v>43533</v>
+      </c>
+      <c r="D192" s="3">
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="F192" s="2">
+        <f t="shared" si="19"/>
+        <v>-0.27083333333333331</v>
+      </c>
+      <c r="N192" t="s">
+        <v>357</v>
+      </c>
+      <c r="P192" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q192">
+        <v>9</v>
+      </c>
+      <c r="R192" t="s">
+        <v>282</v>
+      </c>
+      <c r="S192">
+        <v>3</v>
+      </c>
+      <c r="T192" s="4">
+        <f t="shared" si="17"/>
+        <v>466</v>
+      </c>
+    </row>
+    <row r="193" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A193" t="s">
+        <v>3</v>
+      </c>
+      <c r="B193" s="1">
+        <v>43534</v>
+      </c>
+      <c r="C193" s="5">
+        <f t="shared" si="20"/>
+        <v>43534</v>
+      </c>
+      <c r="D193" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E193" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="F193" s="2">
+        <f t="shared" si="19"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="M193" s="4">
+        <v>2</v>
+      </c>
+      <c r="N193" t="s">
+        <v>356</v>
+      </c>
+      <c r="P193" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q193">
+        <v>9</v>
+      </c>
+      <c r="R193" t="s">
+        <v>282</v>
+      </c>
+      <c r="S193">
+        <v>3</v>
+      </c>
+      <c r="T193" s="4">
+        <f t="shared" si="17"/>
+        <v>468</v>
+      </c>
+    </row>
+    <row r="194" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A194" t="s">
+        <v>67</v>
+      </c>
+      <c r="B194" s="1">
+        <v>43536</v>
+      </c>
+      <c r="C194" s="5">
+        <f t="shared" si="20"/>
+        <v>43536</v>
+      </c>
+      <c r="P194" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q194">
+        <v>9</v>
+      </c>
+      <c r="R194" t="s">
+        <v>282</v>
+      </c>
+      <c r="S194">
+        <v>3</v>
+      </c>
+      <c r="T194" s="4">
+        <f t="shared" si="17"/>
+        <v>468</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T522">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T519">
     <cfRule type="expression" dxfId="17" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
@@ -18956,20 +19230,20 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="13.26953125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="11.54296875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="19.26953125" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="9" width="10.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -18998,7 +19272,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -19025,7 +19299,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -19052,7 +19326,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -19082,7 +19356,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -19121,11 +19395,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -19140,13 +19414,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.7265625" customWidth="1"/>
+    <col min="2" max="2" width="17.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>37</v>
       </c>
@@ -19154,7 +19428,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -19162,7 +19436,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -19170,7 +19444,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>40</v>
       </c>
@@ -19178,7 +19452,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>41</v>
       </c>
@@ -19186,7 +19460,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -19194,7 +19468,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>43</v>
       </c>
@@ -19202,7 +19476,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -19210,7 +19484,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -19218,7 +19492,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -19226,7 +19500,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -19234,7 +19508,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>48</v>
       </c>
@@ -19242,7 +19516,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -19250,7 +19524,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -19258,7 +19532,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -19266,7 +19540,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -19274,7 +19548,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -19282,7 +19556,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -19290,7 +19564,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -19298,7 +19572,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -19306,7 +19580,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -19314,7 +19588,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -19335,22 +19609,22 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" style="17" customWidth="1"/>
-    <col min="2" max="2" width="3.28515625" style="18" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="3.5703125" customWidth="1"/>
-    <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1"/>
+    <col min="2" max="2" width="3.26953125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" style="17" customWidth="1"/>
+    <col min="4" max="4" width="3.54296875" customWidth="1"/>
+    <col min="5" max="5" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="23.26953125" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
-    <col min="8" max="8" width="30.5703125" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" customWidth="1"/>
-    <col min="11" max="11" width="28.5703125" customWidth="1"/>
+    <col min="8" max="8" width="30.54296875" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+    <col min="10" max="10" width="28.81640625" customWidth="1"/>
+    <col min="11" max="11" width="28.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>99</v>
       </c>
@@ -19359,7 +19633,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="16" t="s">
         <v>100</v>
       </c>
@@ -19379,7 +19653,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="16" t="s">
         <v>101</v>
       </c>
@@ -19402,7 +19676,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="16" t="s">
         <v>102</v>
       </c>
@@ -19425,7 +19699,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="16" t="s">
         <v>105</v>
       </c>
@@ -19448,7 +19722,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="16" t="s">
         <v>103</v>
       </c>
@@ -19471,7 +19745,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="16" t="s">
         <v>104</v>
       </c>
@@ -19494,10 +19768,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="15" t="s">
         <v>106</v>
       </c>
@@ -19505,7 +19779,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
         <v>107</v>
       </c>
@@ -19519,7 +19793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
         <v>112</v>
       </c>
@@ -19533,7 +19807,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="16" t="s">
         <v>108</v>
       </c>
@@ -19547,7 +19821,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
         <v>109</v>
       </c>
@@ -19561,7 +19835,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
         <v>111</v>
       </c>
@@ -19575,7 +19849,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
         <v>110</v>
       </c>
@@ -19589,12 +19863,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
         <v>117</v>
       </c>
@@ -19602,7 +19876,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
         <v>114</v>
       </c>
@@ -19610,7 +19884,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
         <v>115</v>
       </c>
@@ -19618,7 +19892,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
         <v>116</v>
       </c>
@@ -19626,7 +19900,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
         <v>118</v>
       </c>
@@ -19634,7 +19908,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
         <v>110</v>
       </c>
@@ -19642,272 +19916,272 @@
         <v>253</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="16" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="16" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="16" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="16" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="16" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="16" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="16" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="16" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A51" s="16" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A52" s="16" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" s="16" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A54" s="16" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" s="16" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" s="16" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A59" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" s="16" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" s="16" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" s="16" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" s="16" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A64" s="16" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" s="16" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" s="16" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A68" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" s="16" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" s="16" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" s="16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" s="16" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A74" s="16" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A75" s="16" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:1" ht="18" x14ac:dyDescent="0.35">
       <c r="A77" s="15" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A78" s="17" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" s="17" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" s="17" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" s="17" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A82" s="17" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" s="17" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" s="17" t="s">
         <v>156</v>
       </c>

</xml_diff>

<commit_message>
Partial Update to 4/5/19
Former-commit-id: 7dbdf8538aeafd358833325a471191c1bacfa5a9
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aNDREW\Desktop\ice-skating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E1C0D80-373C-4036-B4C3-F523814B7A0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15EFC9E-4A0B-4BE7-B548-38696A952418}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="15600" windowHeight="8640" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39960" yWindow="1815" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1043" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="365">
   <si>
     <t>Thursday</t>
   </si>
@@ -1205,6 +1205,15 @@
   </si>
   <si>
     <t>Three Arabian Cartwheels or Butterfly Jumps in a Row (Choice of one)</t>
+  </si>
+  <si>
+    <t>Devon's FS5/FS6 class, worked on FS6 Footwork</t>
+  </si>
+  <si>
+    <t>Landed First Double Salchow, Sit-Change-Sit looking good, Larry 'wowed' at Axel</t>
+  </si>
+  <si>
+    <t>Got on the ice, but too sore to do anything, so I left</t>
   </si>
 </sst>
 </file>
@@ -1325,7 +1334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1355,11 +1364,33 @@
     <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2208,6 +2239,42 @@
                 <c:pt idx="198">
                   <c:v>43544</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>43545</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>43549</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>43550</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>43552</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>43553</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>43554</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>43555</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>43557</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>43558</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>43559</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>43560</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -2813,6 +2880,9 @@
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3716,6 +3786,42 @@
                 <c:pt idx="198">
                   <c:v>43544</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>43545</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>43549</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>43550</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>43552</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>43553</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>43554</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>43555</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>43557</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>43558</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>43559</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>43560</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -4320,6 +4426,42 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="198">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="210">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -4733,7 +4875,7 @@
                   <c:v>150.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41.25</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5118,7 +5260,7 @@
                   <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6008,6 +6150,42 @@
                 <c:pt idx="198">
                   <c:v>43544</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>43545</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>43549</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>43550</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>43552</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>43553</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>43554</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>43555</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>43556</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>43557</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>43558</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>43559</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>43560</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
@@ -6613,6 +6791,42 @@
                 </c:pt>
                 <c:pt idx="198">
                   <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>495.25</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10052,10 +10266,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z201"/>
+  <dimension ref="A1:Z212"/>
   <sheetViews>
-    <sheetView topLeftCell="O10" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="X19" sqref="X19"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="P219" sqref="P219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10240,11 +10454,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M:M)</f>
-        <v>495.25</v>
+        <v>496</v>
       </c>
       <c r="V3" s="4">
         <f>SUM(M152:M387)</f>
-        <v>100</v>
+        <v>100.75</v>
       </c>
       <c r="W3" s="4">
         <f>SUM(M19:M151)</f>
@@ -11063,11 +11277,11 @@
       </c>
       <c r="W19" s="4">
         <f>SUM(M183:M395)</f>
-        <v>41.25</v>
+        <v>42</v>
       </c>
       <c r="X19">
         <f>COUNTIF(P:P, "Freestyle 5")</f>
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -11274,19 +11488,19 @@
       </c>
       <c r="W23" s="4">
         <f>SUM(M100:M376)</f>
-        <v>245</v>
+        <v>245.75</v>
       </c>
       <c r="X23">
         <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="Y23" s="14">
         <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="Z23" s="14">
         <f>Y23-X23</f>
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -17945,7 +18159,7 @@
         <v>43499</v>
       </c>
       <c r="C165" s="5">
-        <f t="shared" ref="C165:C200" si="20">B165</f>
+        <f t="shared" ref="C165:C212" si="20">B165</f>
         <v>43499</v>
       </c>
       <c r="D165" s="3">
@@ -19376,7 +19590,7 @@
         <v>3</v>
       </c>
       <c r="T196" s="4">
-        <f t="shared" ref="T196:T200" si="21">T195+M196</f>
+        <f t="shared" ref="T196:T212" si="21">T195+M196</f>
         <v>488.5</v>
       </c>
     </row>
@@ -19483,7 +19697,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="F199" s="2">
-        <f t="shared" ref="F199:F200" si="22">E199-D199</f>
+        <f t="shared" ref="F199:F212" si="22">E199-D199</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="M199" s="4">
@@ -19554,96 +19768,568 @@
       </c>
     </row>
     <row r="201" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B201"/>
-      <c r="C201"/>
+      <c r="A201" t="s">
+        <v>0</v>
+      </c>
+      <c r="B201" s="1">
+        <v>43545</v>
+      </c>
+      <c r="C201" s="5">
+        <f t="shared" si="20"/>
+        <v>43545</v>
+      </c>
+      <c r="D201" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F201" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.6875</v>
+      </c>
+      <c r="P201" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q201">
+        <v>9</v>
+      </c>
+      <c r="R201" t="str">
+        <f t="shared" ref="R201:R212" si="23">R200</f>
+        <v>Dance 3</v>
+      </c>
+      <c r="S201">
+        <v>3</v>
+      </c>
+      <c r="T201" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>10</v>
+      </c>
+      <c r="B202" s="1">
+        <v>43549</v>
+      </c>
+      <c r="C202" s="5">
+        <f t="shared" si="20"/>
+        <v>43549</v>
+      </c>
+      <c r="D202" s="3">
+        <v>0.71875</v>
+      </c>
+      <c r="F202" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.71875</v>
+      </c>
+      <c r="P202" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q202">
+        <v>9</v>
+      </c>
+      <c r="R202" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S202">
+        <v>3</v>
+      </c>
+      <c r="T202" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>67</v>
+      </c>
+      <c r="B203" s="1">
+        <v>43550</v>
+      </c>
+      <c r="C203" s="5">
+        <f t="shared" si="20"/>
+        <v>43550</v>
+      </c>
+      <c r="D203" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F203" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.72916666666666663</v>
+      </c>
+      <c r="P203" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q203">
+        <v>9</v>
+      </c>
+      <c r="R203" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S203">
+        <v>3</v>
+      </c>
+      <c r="T203" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>0</v>
+      </c>
+      <c r="B204" s="1">
+        <v>43552</v>
+      </c>
+      <c r="C204" s="5">
+        <f t="shared" si="20"/>
+        <v>43552</v>
+      </c>
+      <c r="D204" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F204" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.70833333333333337</v>
+      </c>
+      <c r="P204" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q204">
+        <v>9</v>
+      </c>
+      <c r="R204" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S204">
+        <v>3</v>
+      </c>
+      <c r="T204" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="205" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>1</v>
+      </c>
+      <c r="B205" s="1">
+        <v>43553</v>
+      </c>
+      <c r="C205" s="5">
+        <f t="shared" si="20"/>
+        <v>43553</v>
+      </c>
+      <c r="D205" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="F205" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.80208333333333337</v>
+      </c>
+      <c r="P205" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q205">
+        <v>9</v>
+      </c>
+      <c r="R205" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S205">
+        <v>3</v>
+      </c>
+      <c r="T205" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="206" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>2</v>
+      </c>
+      <c r="B206" s="1">
+        <v>43554</v>
+      </c>
+      <c r="C206" s="5">
+        <f t="shared" si="20"/>
+        <v>43554</v>
+      </c>
+      <c r="D206" s="3">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="F206" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.58333333333333337</v>
+      </c>
+      <c r="P206" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q206">
+        <v>9</v>
+      </c>
+      <c r="R206" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S206">
+        <v>3</v>
+      </c>
+      <c r="T206" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="207" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>3</v>
+      </c>
+      <c r="B207" s="1">
+        <v>43555</v>
+      </c>
+      <c r="C207" s="5">
+        <f t="shared" si="20"/>
+        <v>43555</v>
+      </c>
+      <c r="D207" s="3">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="F207" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.38541666666666669</v>
+      </c>
+      <c r="P207" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q207">
+        <v>9</v>
+      </c>
+      <c r="R207" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S207">
+        <v>3</v>
+      </c>
+      <c r="T207" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="208" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>10</v>
+      </c>
+      <c r="B208" s="1">
+        <v>43556</v>
+      </c>
+      <c r="C208" s="5">
+        <f t="shared" si="20"/>
+        <v>43556</v>
+      </c>
+      <c r="D208" s="3">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="F208" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.67708333333333337</v>
+      </c>
+      <c r="P208" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q208">
+        <v>9</v>
+      </c>
+      <c r="R208" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S208">
+        <v>3</v>
+      </c>
+      <c r="T208" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="209" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>67</v>
+      </c>
+      <c r="B209" s="1">
+        <v>43557</v>
+      </c>
+      <c r="C209" s="5">
+        <f t="shared" si="20"/>
+        <v>43557</v>
+      </c>
+      <c r="D209" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F209" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.70833333333333337</v>
+      </c>
+      <c r="P209" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q209">
+        <v>9</v>
+      </c>
+      <c r="R209" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S209">
+        <v>3</v>
+      </c>
+      <c r="T209" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="210" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>35</v>
+      </c>
+      <c r="B210" s="1">
+        <v>43558</v>
+      </c>
+      <c r="C210" s="5">
+        <f t="shared" si="20"/>
+        <v>43558</v>
+      </c>
+      <c r="D210" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F210" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.70833333333333337</v>
+      </c>
+      <c r="G210" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="I210" s="2">
+        <f>H210-G210</f>
+        <v>-0.73958333333333337</v>
+      </c>
+      <c r="N210" t="s">
+        <v>362</v>
+      </c>
+      <c r="P210" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q210">
+        <v>9</v>
+      </c>
+      <c r="R210" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S210">
+        <v>3</v>
+      </c>
+      <c r="T210" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="211" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>0</v>
+      </c>
+      <c r="B211" s="1">
+        <v>43559</v>
+      </c>
+      <c r="C211" s="5">
+        <f t="shared" si="20"/>
+        <v>43559</v>
+      </c>
+      <c r="D211" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F211" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.70833333333333337</v>
+      </c>
+      <c r="G211" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="I211" s="2">
+        <f>H211-G211</f>
+        <v>-0.83333333333333337</v>
+      </c>
+      <c r="N211" t="s">
+        <v>363</v>
+      </c>
+      <c r="P211" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q211">
+        <v>9</v>
+      </c>
+      <c r="R211" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S211">
+        <v>3</v>
+      </c>
+      <c r="T211" s="4">
+        <f t="shared" si="21"/>
+        <v>495.25</v>
+      </c>
+    </row>
+    <row r="212" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>1</v>
+      </c>
+      <c r="B212" s="1">
+        <v>43560</v>
+      </c>
+      <c r="C212" s="5">
+        <f t="shared" si="20"/>
+        <v>43560</v>
+      </c>
+      <c r="D212" s="3">
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="E212" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="F212" s="2">
+        <f t="shared" si="22"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M212" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="N212" t="s">
+        <v>364</v>
+      </c>
+      <c r="P212" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q212">
+        <v>9</v>
+      </c>
+      <c r="R212" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S212">
+        <v>3</v>
+      </c>
+      <c r="T212" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T517">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T200 A213:T517">
+    <cfRule type="expression" dxfId="20" priority="35">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N104">
+    <cfRule type="expression" dxfId="19" priority="34">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P99:P100">
+    <cfRule type="expression" dxfId="18" priority="33">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P101:P102">
     <cfRule type="expression" dxfId="17" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N104">
+  <conditionalFormatting sqref="P103:P104">
     <cfRule type="expression" dxfId="16" priority="31">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P99:P100">
+  <conditionalFormatting sqref="P105:P106">
     <cfRule type="expression" dxfId="15" priority="30">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P101:P102">
+  <conditionalFormatting sqref="P107:P108">
     <cfRule type="expression" dxfId="14" priority="29">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P103:P104">
+  <conditionalFormatting sqref="P109:P110">
     <cfRule type="expression" dxfId="13" priority="28">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P105:P106">
-    <cfRule type="expression" dxfId="12" priority="27">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P107:P108">
-    <cfRule type="expression" dxfId="11" priority="26">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P109:P110">
-    <cfRule type="expression" dxfId="10" priority="25">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="P112">
-    <cfRule type="expression" dxfId="9" priority="23">
+    <cfRule type="expression" dxfId="12" priority="26">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P113:P114">
-    <cfRule type="expression" dxfId="8" priority="22">
+    <cfRule type="expression" dxfId="11" priority="25">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P115:P116">
-    <cfRule type="expression" dxfId="7" priority="20">
+    <cfRule type="expression" dxfId="10" priority="23">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P126:P128">
-    <cfRule type="expression" dxfId="6" priority="15">
+    <cfRule type="expression" dxfId="9" priority="18">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E124">
-    <cfRule type="expression" dxfId="5" priority="8">
+    <cfRule type="expression" dxfId="8" priority="11">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="7" priority="7">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E125">
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="6" priority="8">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H127">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H128">
+    <cfRule type="expression" dxfId="4" priority="5">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N123:N128">
+    <cfRule type="expression" dxfId="3" priority="4">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H209:O209 A201:F212 Q201:T212 G210:O212 G201:O208">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H128">
+  <conditionalFormatting sqref="P201:P206">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N123:N128">
+  <conditionalFormatting sqref="P207:P212">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
@@ -19826,7 +20512,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Partial Update to 4/17/19
Former-commit-id: 0dbcf8440a1fdb1256bb5b7c5cddee40123550eb
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15EFC9E-4A0B-4BE7-B548-38696A952418}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0854598-4F2B-413D-94CE-588D5870C61B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39960" yWindow="1815" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="368">
   <si>
     <t>Thursday</t>
   </si>
@@ -896,12 +896,6 @@
   </si>
   <si>
     <t>Currier, Private, Stroking</t>
-  </si>
-  <si>
-    <t>FS 3</t>
-  </si>
-  <si>
-    <t>FS 4</t>
   </si>
   <si>
     <t>Axels with Laurel</t>
@@ -1168,9 +1162,6 @@
     <t>Worked On FS4 Manuevers, High Confidence</t>
   </si>
   <si>
-    <t>FS 1 / FS 2</t>
-  </si>
-  <si>
     <t>Pain on blisters couldn't skate</t>
   </si>
   <si>
@@ -1214,6 +1205,24 @@
   </si>
   <si>
     <t>Got on the ice, but too sore to do anything, so I left</t>
+  </si>
+  <si>
+    <t>Landed crazy good axels consistently. Need to make sure that the cirlce I'm on is large. Also need to bend down when going backwards and not let my left shoulder go. Lesson with Devon working on backscratch, camels, Layback, and catchfoot.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public, Stroking, FS5/6, FSIce, Private </t>
+  </si>
+  <si>
+    <t>FS Ice</t>
+  </si>
+  <si>
+    <t>FS1 / FS2</t>
+  </si>
+  <si>
+    <t>FS4</t>
+  </si>
+  <si>
+    <t>FS3</t>
   </si>
 </sst>
 </file>
@@ -1369,14 +1378,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="20">
     <dxf>
       <fill>
         <patternFill>
@@ -1638,10 +1640,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$377</c:f>
+              <c:f>Data!$C$2:$C$372</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="376"/>
+                <c:ptCount val="371"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -2274,16 +2276,37 @@
                 </c:pt>
                 <c:pt idx="210">
                   <c:v>43560</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>43562</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>43564</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>43565</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>43566</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>43567</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>43571</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>43572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$377</c:f>
+              <c:f>Data!$M$2:$M$372</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="376"/>
+                <c:ptCount val="371"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -3185,10 +3208,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$377</c:f>
+              <c:f>Data!$C$2:$C$372</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="376"/>
+                <c:ptCount val="371"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -3821,16 +3844,37 @@
                 </c:pt>
                 <c:pt idx="210">
                   <c:v>43560</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>43562</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>43564</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>43565</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>43566</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>43567</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>43571</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>43572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$377</c:f>
+              <c:f>Data!$Q$2:$Q$372</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="376"/>
+                <c:ptCount val="371"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4462,6 +4506,27 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="210">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="217">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -4830,13 +4895,13 @@
                   <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FS 1 / FS 2</c:v>
+                  <c:v>FS1 / FS2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>FS 3</c:v>
+                  <c:v>FS3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FS 4</c:v>
+                  <c:v>FS4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>FS5</c:v>
@@ -5215,13 +5280,13 @@
                   <c:v>Delta</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>FS 1 / FS 2</c:v>
+                  <c:v>FS1 / FS2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>FS 3</c:v>
+                  <c:v>FS3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>FS 4</c:v>
+                  <c:v>FS4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>FS5</c:v>
@@ -5260,7 +5325,7 @@
                   <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>30</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5549,10 +5614,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$377</c:f>
+              <c:f>Data!$C$2:$C$372</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="376"/>
+                <c:ptCount val="371"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -6185,16 +6250,37 @@
                 </c:pt>
                 <c:pt idx="210">
                   <c:v>43560</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>43562</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>43564</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>43565</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>43566</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>43567</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>43571</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>43572</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$T$2:$T$377</c:f>
+              <c:f>Data!$T$2:$T$372</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="376"/>
+                <c:ptCount val="371"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -6826,6 +6912,27 @@
                   <c:v>495.25</c:v>
                 </c:pt>
                 <c:pt idx="210">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>496</c:v>
+                </c:pt>
+                <c:pt idx="217">
                   <c:v>496</c:v>
                 </c:pt>
               </c:numCache>
@@ -10266,10 +10373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z212"/>
+  <dimension ref="A1:Z232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="P219" sqref="P219"/>
+    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10406,13 +10513,13 @@
         <v>4</v>
       </c>
       <c r="V2" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
@@ -10457,7 +10564,7 @@
         <v>496</v>
       </c>
       <c r="V3" s="4">
-        <f>SUM(M152:M387)</f>
+        <f>SUM(M152:M382)</f>
         <v>100.75</v>
       </c>
       <c r="W3" s="4">
@@ -11082,7 +11189,7 @@
         <v>32</v>
       </c>
       <c r="V16" t="s">
-        <v>349</v>
+        <v>365</v>
       </c>
       <c r="W16" s="4">
         <f>SUM(M43:M96)</f>
@@ -11153,7 +11260,7 @@
         <v>38.25</v>
       </c>
       <c r="V17" t="s">
-        <v>287</v>
+        <v>367</v>
       </c>
       <c r="W17" s="4">
         <f>SUM(M97:M116)</f>
@@ -11213,7 +11320,7 @@
         <v>41.75</v>
       </c>
       <c r="V18" t="s">
-        <v>288</v>
+        <v>366</v>
       </c>
       <c r="W18" s="4">
         <f>SUM(M117:M182)</f>
@@ -11273,15 +11380,15 @@
         <v>42.75</v>
       </c>
       <c r="V19" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="W19" s="4">
-        <f>SUM(M183:M395)</f>
+        <f>SUM(M183:M390)</f>
         <v>42</v>
       </c>
       <c r="X19">
         <f>COUNTIF(P:P, "Freestyle 5")</f>
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -11487,20 +11594,20 @@
         <v>280</v>
       </c>
       <c r="W23" s="4">
-        <f>SUM(M100:M376)</f>
+        <f>SUM(M100:M371)</f>
         <v>245.75</v>
       </c>
       <c r="X23">
         <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="Y23" s="14">
         <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="Z23" s="14">
         <f>Y23-X23</f>
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -15563,10 +15670,10 @@
         <v>2.5</v>
       </c>
       <c r="N110" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="O110" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="P110" s="20" t="s">
         <v>113</v>
@@ -15630,10 +15737,10 @@
         <v>6.75</v>
       </c>
       <c r="N111" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="O111" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="P111" s="20" t="s">
         <v>113</v>
@@ -15721,7 +15828,7 @@
         <v>1</v>
       </c>
       <c r="N113" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="O113" t="s">
         <v>282</v>
@@ -15815,7 +15922,7 @@
         <v>1</v>
       </c>
       <c r="N115" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="O115" t="s">
         <v>68</v>
@@ -16023,7 +16130,7 @@
         <v>1</v>
       </c>
       <c r="N119" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="O119" t="s">
         <v>282</v>
@@ -16114,7 +16221,7 @@
         <v>4</v>
       </c>
       <c r="O121" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="P121" s="20" t="s">
         <v>119</v>
@@ -16170,7 +16277,7 @@
         <v>4.25</v>
       </c>
       <c r="O122" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P122" s="20" t="s">
         <v>119</v>
@@ -16214,10 +16321,10 @@
         <v>3.5</v>
       </c>
       <c r="N123" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="O123" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="P123" s="20" t="s">
         <v>119</v>
@@ -16261,10 +16368,10 @@
         <v>1.75</v>
       </c>
       <c r="N124" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O124" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P124" s="20" t="s">
         <v>119</v>
@@ -16308,10 +16415,10 @@
         <v>1.75</v>
       </c>
       <c r="N125" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O125" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P125" s="20" t="s">
         <v>119</v>
@@ -16355,10 +16462,10 @@
         <v>1.75</v>
       </c>
       <c r="N126" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O126" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P126" s="20" t="s">
         <v>119</v>
@@ -16412,10 +16519,10 @@
         <v>3.5</v>
       </c>
       <c r="N127" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O127" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P127" s="20" t="s">
         <v>119</v>
@@ -16469,10 +16576,10 @@
         <v>3.5</v>
       </c>
       <c r="N128" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="O128" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="P128" s="20" t="s">
         <v>119</v>
@@ -16604,10 +16711,10 @@
         <v>7.75</v>
       </c>
       <c r="N131" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="O131" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="P131" s="20" t="s">
         <v>119</v>
@@ -16695,7 +16802,7 @@
         <v>2</v>
       </c>
       <c r="N133" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="O133" t="s">
         <v>17</v>
@@ -16796,10 +16903,10 @@
         <v>5</v>
       </c>
       <c r="N135" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O135" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P135" s="20" t="s">
         <v>119</v>
@@ -16853,10 +16960,10 @@
         <v>6.75</v>
       </c>
       <c r="N136" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="O136" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="P136" s="20" t="s">
         <v>119</v>
@@ -16910,7 +17017,7 @@
         <v>2.25</v>
       </c>
       <c r="N137" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="O137" t="s">
         <v>21</v>
@@ -16957,10 +17064,10 @@
         <v>2.25</v>
       </c>
       <c r="N138" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="O138" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P138" s="20" t="s">
         <v>119</v>
@@ -17014,7 +17121,7 @@
         <v>2</v>
       </c>
       <c r="N139" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P139" s="20" t="s">
         <v>119</v>
@@ -17058,7 +17165,7 @@
         <v>1.75</v>
       </c>
       <c r="N140" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P140" s="20" t="s">
         <v>119</v>
@@ -17102,7 +17209,7 @@
         <v>2</v>
       </c>
       <c r="N141" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P141" s="20" t="s">
         <v>119</v>
@@ -17146,7 +17253,7 @@
         <v>4.25</v>
       </c>
       <c r="N142" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="P142" s="20" t="s">
         <v>119</v>
@@ -17190,7 +17297,7 @@
         <v>2.25</v>
       </c>
       <c r="N143" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="P143" s="20" t="s">
         <v>119</v>
@@ -17285,7 +17392,7 @@
         <v>2.5</v>
       </c>
       <c r="N145" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P145" s="20" t="s">
         <v>119</v>
@@ -17534,7 +17641,7 @@
         <v>2.25</v>
       </c>
       <c r="N151" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="P151" s="20" t="s">
         <v>119</v>
@@ -17578,7 +17685,7 @@
         <v>5.75</v>
       </c>
       <c r="N152" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="P152" s="20" t="s">
         <v>119</v>
@@ -17622,7 +17729,7 @@
         <v>3.5</v>
       </c>
       <c r="N153" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="P153" s="20" t="s">
         <v>119</v>
@@ -17666,7 +17773,7 @@
         <v>0.75</v>
       </c>
       <c r="N154" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="P154" s="20" t="s">
         <v>119</v>
@@ -17710,7 +17817,7 @@
         <v>0.5</v>
       </c>
       <c r="N155" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="P155" s="20" t="s">
         <v>119</v>
@@ -17754,7 +17861,7 @@
         <v>3.5</v>
       </c>
       <c r="N156" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="P156" s="20" t="s">
         <v>119</v>
@@ -17798,7 +17905,7 @@
         <v>2</v>
       </c>
       <c r="N157" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="P157" s="20" t="s">
         <v>119</v>
@@ -17842,7 +17949,7 @@
         <v>0.5</v>
       </c>
       <c r="N158" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="P158" s="20" t="s">
         <v>119</v>
@@ -17886,7 +17993,7 @@
         <v>1.25</v>
       </c>
       <c r="N159" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="P159" s="20" t="s">
         <v>119</v>
@@ -17930,10 +18037,10 @@
         <v>1</v>
       </c>
       <c r="N160" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="O160" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="P160" s="20" t="s">
         <v>119</v>
@@ -17977,10 +18084,10 @@
         <v>2.75</v>
       </c>
       <c r="N161" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="O161" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="P161" s="20" t="s">
         <v>119</v>
@@ -18024,7 +18131,7 @@
         <v>1</v>
       </c>
       <c r="N162" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="P162" s="20" t="s">
         <v>119</v>
@@ -18078,7 +18185,7 @@
         <v>1.75</v>
       </c>
       <c r="N163" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="P163" s="20" t="s">
         <v>119</v>
@@ -18132,7 +18239,7 @@
         <v>4.5</v>
       </c>
       <c r="N164" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="P164" s="20" t="s">
         <v>119</v>
@@ -18159,7 +18266,7 @@
         <v>43499</v>
       </c>
       <c r="C165" s="5">
-        <f t="shared" ref="C165:C212" si="20">B165</f>
+        <f t="shared" ref="C165:C219" si="20">B165</f>
         <v>43499</v>
       </c>
       <c r="D165" s="3">
@@ -18176,7 +18283,7 @@
         <v>2.25</v>
       </c>
       <c r="N165" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="O165" t="s">
         <v>17</v>
@@ -18223,7 +18330,7 @@
         <v>1</v>
       </c>
       <c r="N166" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="O166" t="s">
         <v>68</v>
@@ -18280,10 +18387,10 @@
         <v>2.25</v>
       </c>
       <c r="N167" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="O167" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="P167" s="20" t="s">
         <v>119</v>
@@ -18327,7 +18434,7 @@
         <v>1.5</v>
       </c>
       <c r="N168" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O168" t="s">
         <v>264</v>
@@ -18384,10 +18491,10 @@
         <v>1.75</v>
       </c>
       <c r="N169" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="O169" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="P169" s="20" t="s">
         <v>119</v>
@@ -18431,10 +18538,10 @@
         <v>5</v>
       </c>
       <c r="N170" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O170" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="P170" s="20" t="s">
         <v>119</v>
@@ -18478,7 +18585,7 @@
         <v>1.75</v>
       </c>
       <c r="N171" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="P171" s="20" t="s">
         <v>119</v>
@@ -18522,7 +18629,7 @@
         <v>1</v>
       </c>
       <c r="N172" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="P172" s="20" t="s">
         <v>119</v>
@@ -18566,7 +18673,7 @@
         <v>1.25</v>
       </c>
       <c r="N173" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="P173" s="20" t="s">
         <v>119</v>
@@ -18610,7 +18717,7 @@
         <v>0.25</v>
       </c>
       <c r="N174" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="P174" s="20" t="s">
         <v>119</v>
@@ -18654,7 +18761,7 @@
         <v>0.25</v>
       </c>
       <c r="N175" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="P175" s="20" t="s">
         <v>119</v>
@@ -18698,7 +18805,7 @@
         <v>0.5</v>
       </c>
       <c r="N176" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="P176" s="20" t="s">
         <v>119</v>
@@ -18865,7 +18972,7 @@
         <v>4.25</v>
       </c>
       <c r="N180" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="O180" t="s">
         <v>17</v>
@@ -18912,7 +19019,7 @@
         <v>2</v>
       </c>
       <c r="N181" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="O181" t="s">
         <v>17</v>
@@ -19010,7 +19117,7 @@
         <v>1.25</v>
       </c>
       <c r="N183" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="P183" s="20" t="s">
         <v>125</v>
@@ -19054,7 +19161,7 @@
         <v>0.5</v>
       </c>
       <c r="N184" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="P184" s="20" t="s">
         <v>125</v>
@@ -19405,7 +19512,7 @@
         <v>3.25</v>
       </c>
       <c r="N192" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="P192" s="20" t="s">
         <v>125</v>
@@ -19449,7 +19556,7 @@
         <v>2</v>
       </c>
       <c r="N193" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="P193" s="20" t="s">
         <v>125</v>
@@ -19534,7 +19641,7 @@
         <v>3.5</v>
       </c>
       <c r="N195" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="P195" s="20" t="s">
         <v>125</v>
@@ -19590,7 +19697,7 @@
         <v>3</v>
       </c>
       <c r="T196" s="4">
-        <f t="shared" ref="T196:T212" si="21">T195+M196</f>
+        <f t="shared" ref="T196:T219" si="21">T195+M196</f>
         <v>488.5</v>
       </c>
     </row>
@@ -19660,7 +19767,7 @@
         <v>1.5</v>
       </c>
       <c r="N198" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="P198" s="20" t="s">
         <v>125</v>
@@ -19697,14 +19804,14 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="F199" s="2">
-        <f t="shared" ref="F199:F212" si="22">E199-D199</f>
+        <f t="shared" ref="F199:F219" si="22">E199-D199</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="M199" s="4">
         <v>1</v>
       </c>
       <c r="N199" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="P199" s="20" t="s">
         <v>125</v>
@@ -19748,7 +19855,7 @@
         <v>2</v>
       </c>
       <c r="N200" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="P200" s="20" t="s">
         <v>125</v>
@@ -19792,7 +19899,7 @@
         <v>9</v>
       </c>
       <c r="R201" t="str">
-        <f t="shared" ref="R201:R212" si="23">R200</f>
+        <f t="shared" ref="R201:R219" si="23">R200</f>
         <v>Dance 3</v>
       </c>
       <c r="S201">
@@ -20117,7 +20224,10 @@
         <v>-0.73958333333333337</v>
       </c>
       <c r="N210" t="s">
-        <v>362</v>
+        <v>359</v>
+      </c>
+      <c r="O210" t="s">
+        <v>363</v>
       </c>
       <c r="P210" s="20" t="s">
         <v>125</v>
@@ -20163,7 +20273,10 @@
         <v>-0.83333333333333337</v>
       </c>
       <c r="N211" t="s">
-        <v>363</v>
+        <v>360</v>
+      </c>
+      <c r="O211" t="s">
+        <v>217</v>
       </c>
       <c r="P211" s="20" t="s">
         <v>125</v>
@@ -20208,6 +20321,9 @@
         <v>0.75</v>
       </c>
       <c r="N212" t="s">
+        <v>361</v>
+      </c>
+      <c r="O212" t="s">
         <v>364</v>
       </c>
       <c r="P212" s="25" t="s">
@@ -20228,109 +20344,417 @@
         <v>496</v>
       </c>
     </row>
+    <row r="213" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>3</v>
+      </c>
+      <c r="B213" s="1">
+        <v>43562</v>
+      </c>
+      <c r="C213" s="5">
+        <f t="shared" si="20"/>
+        <v>43562</v>
+      </c>
+      <c r="D213" s="3">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F213" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.54166666666666663</v>
+      </c>
+      <c r="P213" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q213">
+        <v>9</v>
+      </c>
+      <c r="R213" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S213">
+        <v>3</v>
+      </c>
+      <c r="T213" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="214" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>67</v>
+      </c>
+      <c r="B214" s="1">
+        <v>43564</v>
+      </c>
+      <c r="C214" s="5">
+        <f t="shared" si="20"/>
+        <v>43564</v>
+      </c>
+      <c r="D214" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F214" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.6875</v>
+      </c>
+      <c r="P214" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q214">
+        <v>9</v>
+      </c>
+      <c r="R214" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S214">
+        <v>3</v>
+      </c>
+      <c r="T214" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="215" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>35</v>
+      </c>
+      <c r="B215" s="1">
+        <v>43565</v>
+      </c>
+      <c r="C215" s="5">
+        <f t="shared" si="20"/>
+        <v>43565</v>
+      </c>
+      <c r="D215" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F215" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.6875</v>
+      </c>
+      <c r="P215" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q215">
+        <v>9</v>
+      </c>
+      <c r="R215" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S215">
+        <v>3</v>
+      </c>
+      <c r="T215" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="216" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>0</v>
+      </c>
+      <c r="B216" s="1">
+        <v>43566</v>
+      </c>
+      <c r="C216" s="5">
+        <f t="shared" si="20"/>
+        <v>43566</v>
+      </c>
+      <c r="D216" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F216" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.6875</v>
+      </c>
+      <c r="G216" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="P216" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q216">
+        <v>9</v>
+      </c>
+      <c r="R216" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S216">
+        <v>3</v>
+      </c>
+      <c r="T216" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="217" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>1</v>
+      </c>
+      <c r="B217" s="1">
+        <v>43567</v>
+      </c>
+      <c r="C217" s="5">
+        <f t="shared" si="20"/>
+        <v>43567</v>
+      </c>
+      <c r="D217" s="3">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="F217" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.80208333333333337</v>
+      </c>
+      <c r="P217" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q217">
+        <v>9</v>
+      </c>
+      <c r="R217" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S217">
+        <v>3</v>
+      </c>
+      <c r="T217" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="218" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>67</v>
+      </c>
+      <c r="B218" s="1">
+        <v>43571</v>
+      </c>
+      <c r="C218" s="5">
+        <f t="shared" si="20"/>
+        <v>43571</v>
+      </c>
+      <c r="D218" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F218" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.64583333333333337</v>
+      </c>
+      <c r="P218" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q218">
+        <v>9</v>
+      </c>
+      <c r="R218" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S218">
+        <v>3</v>
+      </c>
+      <c r="T218" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="219" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>35</v>
+      </c>
+      <c r="B219" s="1">
+        <v>43572</v>
+      </c>
+      <c r="C219" s="5">
+        <f t="shared" si="20"/>
+        <v>43572</v>
+      </c>
+      <c r="D219" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F219" s="2">
+        <f t="shared" si="22"/>
+        <v>-0.66666666666666663</v>
+      </c>
+      <c r="N219" t="s">
+        <v>362</v>
+      </c>
+      <c r="O219" t="s">
+        <v>363</v>
+      </c>
+      <c r="P219" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q219">
+        <v>9</v>
+      </c>
+      <c r="R219" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S219">
+        <v>3</v>
+      </c>
+      <c r="T219" s="4">
+        <f t="shared" si="21"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="220" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B220"/>
+      <c r="C220"/>
+    </row>
+    <row r="221" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B221"/>
+      <c r="C221"/>
+    </row>
+    <row r="222" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B222"/>
+      <c r="C222"/>
+    </row>
+    <row r="223" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B223"/>
+      <c r="C223"/>
+    </row>
+    <row r="224" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B224"/>
+      <c r="C224"/>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B225"/>
+      <c r="C225"/>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B226"/>
+      <c r="C226"/>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B227"/>
+      <c r="C227"/>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B228"/>
+      <c r="C228"/>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B229"/>
+      <c r="C229"/>
+    </row>
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B230"/>
+      <c r="C230"/>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B231"/>
+      <c r="C231"/>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B232"/>
+      <c r="C232"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T200 A213:T517">
-    <cfRule type="expression" dxfId="20" priority="35">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T200 A220:T512 A213:O219 P207:P219 Q201:T219">
+    <cfRule type="expression" dxfId="19" priority="35">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N104">
-    <cfRule type="expression" dxfId="19" priority="34">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P99:P100">
-    <cfRule type="expression" dxfId="18" priority="33">
+    <cfRule type="expression" dxfId="17" priority="33">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P101:P102">
-    <cfRule type="expression" dxfId="17" priority="32">
+    <cfRule type="expression" dxfId="16" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P103:P104">
-    <cfRule type="expression" dxfId="16" priority="31">
+    <cfRule type="expression" dxfId="15" priority="31">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P105:P106">
-    <cfRule type="expression" dxfId="15" priority="30">
+    <cfRule type="expression" dxfId="14" priority="30">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P107:P108">
-    <cfRule type="expression" dxfId="14" priority="29">
+    <cfRule type="expression" dxfId="13" priority="29">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P109:P110">
-    <cfRule type="expression" dxfId="13" priority="28">
+    <cfRule type="expression" dxfId="12" priority="28">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P112">
-    <cfRule type="expression" dxfId="12" priority="26">
+    <cfRule type="expression" dxfId="11" priority="26">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P113:P114">
-    <cfRule type="expression" dxfId="11" priority="25">
+    <cfRule type="expression" dxfId="10" priority="25">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P115:P116">
-    <cfRule type="expression" dxfId="10" priority="23">
+    <cfRule type="expression" dxfId="9" priority="23">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P126:P128">
-    <cfRule type="expression" dxfId="9" priority="18">
+    <cfRule type="expression" dxfId="8" priority="18">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E124">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="7" priority="11">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126">
-    <cfRule type="expression" dxfId="7" priority="7">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E125">
-    <cfRule type="expression" dxfId="6" priority="8">
+    <cfRule type="expression" dxfId="5" priority="8">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H127">
-    <cfRule type="expression" dxfId="5" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H128">
-    <cfRule type="expression" dxfId="4" priority="5">
+    <cfRule type="expression" dxfId="3" priority="5">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N123:N128">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H209:O209 A201:F212 Q201:T212 G210:O212 G201:O208">
-    <cfRule type="expression" dxfId="2" priority="3">
+  <conditionalFormatting sqref="H209:O209 A201:F212 G210:O212 G201:O208">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P201:P206">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P207:P212">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20500,7 +20924,7 @@
         <v>207</v>
       </c>
       <c r="I5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
   </sheetData>
@@ -20512,7 +20936,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -21290,12 +21714,12 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="24" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fully Updated to 5/19/19
Former-commit-id: fa6986ecf5e968b6ec684039a30bdeea615fde9c
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\8ag\Desktop\ice-skating\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aNDREW\Desktop\ice-skating\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0854598-4F2B-413D-94CE-588D5870C61B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B45F27-9FA7-4CAA-B355-AEE4C96D4EAB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1089" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="383">
   <si>
     <t>Thursday</t>
   </si>
@@ -1223,6 +1223,51 @@
   </si>
   <si>
     <t>FS3</t>
+  </si>
+  <si>
+    <t>Competition: Pandas</t>
+  </si>
+  <si>
+    <t>Competition: J&amp;S, FS4, Group Interp</t>
+  </si>
+  <si>
+    <t>Competition: Pairs, Silver, WTIC</t>
+  </si>
+  <si>
+    <t>DEVON</t>
+  </si>
+  <si>
+    <t>Converted Axels, OneFoot to backscratch, Waltz loop loop backspin</t>
+  </si>
+  <si>
+    <t>With Reagen and Ellie, did axels</t>
+  </si>
+  <si>
+    <t>Did two wallies with Privo, worked on general skating ability</t>
+  </si>
+  <si>
+    <t>Wallies, Axels, Axel-halfloop-flip, remember to wind up when stepping into axel</t>
+  </si>
+  <si>
+    <t>Class and Stroking with Devon, worked on axels and couldn't do any, Camels in private</t>
+  </si>
+  <si>
+    <t>Axel Work, Worked on singles</t>
+  </si>
+  <si>
+    <t>Pairs with Laurel, worked on edge control and loop takeoff direction</t>
+  </si>
+  <si>
+    <t>Couples spotlight, program prep</t>
+  </si>
+  <si>
+    <t>Program Runthrough</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Late Night Skate</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1423,63 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1640,10 +1741,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$372</c:f>
+              <c:f>Data!$C$2:$C$361</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="371"/>
+                <c:ptCount val="360"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -2297,16 +2398,85 @@
                 </c:pt>
                 <c:pt idx="217">
                   <c:v>43572</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>43573</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>43574</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>43575</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>43576</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>43577</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>43578</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>43580</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>43581</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>43582</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>43601</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>43603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$M$2:$M$372</c:f>
+              <c:f>Data!$M$2:$M$361</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="371"/>
+                <c:ptCount val="360"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -2904,8 +3074,122 @@
                 <c:pt idx="198">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="199">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>2.25</c:v>
+                </c:pt>
                 <c:pt idx="210">
                   <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>2.25</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>3.75</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>1.25</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>2.75</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>1.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3208,10 +3492,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$372</c:f>
+              <c:f>Data!$C$2:$C$361</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="371"/>
+                <c:ptCount val="360"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -3865,16 +4149,85 @@
                 </c:pt>
                 <c:pt idx="217">
                   <c:v>43572</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>43573</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>43574</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>43575</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>43576</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>43577</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>43578</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>43580</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>43581</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>43582</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>43601</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>43603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$Q$2:$Q$372</c:f>
+              <c:f>Data!$Q$2:$Q$361</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="371"/>
+                <c:ptCount val="360"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4527,6 +4880,75 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="217">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="240">
                   <c:v>9</c:v>
                 </c:pt>
               </c:numCache>
@@ -4940,7 +5362,7 @@
                   <c:v>150.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42</c:v>
+                  <c:v>124.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5325,7 +5747,7 @@
                   <c:v>66</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>37</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5614,10 +6036,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Data!$C$2:$C$372</c:f>
+              <c:f>Data!$C$2:$C$361</c:f>
               <c:numCache>
                 <c:formatCode>m/d;@</c:formatCode>
-                <c:ptCount val="371"/>
+                <c:ptCount val="360"/>
                 <c:pt idx="0">
                   <c:v>43286</c:v>
                 </c:pt>
@@ -6271,16 +6693,85 @@
                 </c:pt>
                 <c:pt idx="217">
                   <c:v>43572</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>43573</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>43574</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>43575</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>43576</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>43577</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>43578</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>43580</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>43581</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>43582</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>43584</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>43585</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>43586</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>43587</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>43588</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>43589</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>43590</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>43592</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>43594</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>43595</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>43600</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>43601</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>43602</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>43603</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Data!$T$2:$T$372</c:f>
+              <c:f>Data!$T$2:$T$361</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="371"/>
+                <c:ptCount val="360"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -6879,61 +7370,130 @@
                   <c:v>495.25</c:v>
                 </c:pt>
                 <c:pt idx="199">
-                  <c:v>495.25</c:v>
+                  <c:v>498.25</c:v>
                 </c:pt>
                 <c:pt idx="200">
-                  <c:v>495.25</c:v>
+                  <c:v>498.75</c:v>
                 </c:pt>
                 <c:pt idx="201">
-                  <c:v>495.25</c:v>
+                  <c:v>499</c:v>
                 </c:pt>
                 <c:pt idx="202">
-                  <c:v>495.25</c:v>
+                  <c:v>499.75</c:v>
                 </c:pt>
                 <c:pt idx="203">
-                  <c:v>495.25</c:v>
+                  <c:v>503.5</c:v>
                 </c:pt>
                 <c:pt idx="204">
-                  <c:v>495.25</c:v>
+                  <c:v>507</c:v>
                 </c:pt>
                 <c:pt idx="205">
-                  <c:v>495.25</c:v>
+                  <c:v>508.75</c:v>
                 </c:pt>
                 <c:pt idx="206">
-                  <c:v>495.25</c:v>
+                  <c:v>510.25</c:v>
                 </c:pt>
                 <c:pt idx="207">
-                  <c:v>495.25</c:v>
+                  <c:v>511</c:v>
                 </c:pt>
                 <c:pt idx="208">
-                  <c:v>495.25</c:v>
+                  <c:v>513.75</c:v>
                 </c:pt>
                 <c:pt idx="209">
-                  <c:v>495.25</c:v>
+                  <c:v>516</c:v>
                 </c:pt>
                 <c:pt idx="210">
-                  <c:v>496</c:v>
+                  <c:v>516.75</c:v>
                 </c:pt>
                 <c:pt idx="211">
-                  <c:v>496</c:v>
+                  <c:v>520.25</c:v>
                 </c:pt>
                 <c:pt idx="212">
-                  <c:v>496</c:v>
+                  <c:v>521.5</c:v>
                 </c:pt>
                 <c:pt idx="213">
-                  <c:v>496</c:v>
+                  <c:v>524.75</c:v>
                 </c:pt>
                 <c:pt idx="214">
-                  <c:v>496</c:v>
+                  <c:v>528.5</c:v>
                 </c:pt>
                 <c:pt idx="215">
-                  <c:v>496</c:v>
+                  <c:v>530.5</c:v>
                 </c:pt>
                 <c:pt idx="216">
-                  <c:v>496</c:v>
+                  <c:v>532.75</c:v>
                 </c:pt>
                 <c:pt idx="217">
-                  <c:v>496</c:v>
+                  <c:v>536.5</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>538.25</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>539.25</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>542.5</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>545.25</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>546</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>547.5</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>551.5</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>553.25</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>556.75</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>558.75</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>560.5</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>561</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>562</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>563</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>564.25</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>566.25</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>569.75</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>574.25</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>577</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>578.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10373,10 +10933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z232"/>
+  <dimension ref="A1:Z242"/>
   <sheetViews>
-    <sheetView zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10561,11 +11121,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M:M)</f>
-        <v>496</v>
+        <v>578.75</v>
       </c>
       <c r="V3" s="4">
-        <f>SUM(M152:M382)</f>
-        <v>100.75</v>
+        <f>SUM(M152:M371)</f>
+        <v>183.5</v>
       </c>
       <c r="W3" s="4">
         <f>SUM(M19:M151)</f>
@@ -11383,12 +11943,12 @@
         <v>350</v>
       </c>
       <c r="W19" s="4">
-        <f>SUM(M183:M390)</f>
-        <v>42</v>
+        <f>SUM(M183:M379)</f>
+        <v>124.75</v>
       </c>
       <c r="X19">
         <f>COUNTIF(P:P, "Freestyle 5")</f>
-        <v>37</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
@@ -11594,20 +12154,20 @@
         <v>280</v>
       </c>
       <c r="W23" s="4">
-        <f>SUM(M100:M371)</f>
-        <v>245.75</v>
+        <f>SUM(M100:M360)</f>
+        <v>328.5</v>
       </c>
       <c r="X23">
         <f>COUNTIF(R:R, "Dance 3")</f>
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="Y23" s="14">
         <f>(INDEX(C:C,COUNTA(C:C))) - C100</f>
-        <v>165</v>
+        <v>196</v>
       </c>
       <c r="Z23" s="14">
         <f>Y23-X23</f>
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
@@ -18266,7 +18826,7 @@
         <v>43499</v>
       </c>
       <c r="C165" s="5">
-        <f t="shared" ref="C165:C219" si="20">B165</f>
+        <f t="shared" ref="C165:C227" si="20">B165</f>
         <v>43499</v>
       </c>
       <c r="D165" s="3">
@@ -19697,7 +20257,7 @@
         <v>3</v>
       </c>
       <c r="T196" s="4">
-        <f t="shared" ref="T196:T219" si="21">T195+M196</f>
+        <f t="shared" ref="T196:T242" si="21">T195+M196</f>
         <v>488.5</v>
       </c>
     </row>
@@ -19804,7 +20364,7 @@
         <v>0.73958333333333337</v>
       </c>
       <c r="F199" s="2">
-        <f t="shared" ref="F199:F219" si="22">E199-D199</f>
+        <f t="shared" ref="F199:F242" si="22">E199-D199</f>
         <v>4.1666666666666741E-2</v>
       </c>
       <c r="M199" s="4">
@@ -19845,11 +20405,11 @@
         <v>0.75</v>
       </c>
       <c r="E200" s="3">
-        <v>0.83333333333333337</v>
+        <v>0.82291666666666663</v>
       </c>
       <c r="F200" s="2">
         <f t="shared" si="22"/>
-        <v>8.333333333333337E-2</v>
+        <v>7.291666666666663E-2</v>
       </c>
       <c r="M200" s="4">
         <v>2</v>
@@ -19888,9 +20448,15 @@
       <c r="D201" s="3">
         <v>0.6875</v>
       </c>
+      <c r="E201" s="3">
+        <v>0.8125</v>
+      </c>
       <c r="F201" s="2">
         <f t="shared" si="22"/>
-        <v>-0.6875</v>
+        <v>0.125</v>
+      </c>
+      <c r="M201" s="4">
+        <v>3</v>
       </c>
       <c r="P201" s="20" t="s">
         <v>125</v>
@@ -19899,7 +20465,7 @@
         <v>9</v>
       </c>
       <c r="R201" t="str">
-        <f t="shared" ref="R201:R219" si="23">R200</f>
+        <f t="shared" ref="R201:R242" si="23">R200</f>
         <v>Dance 3</v>
       </c>
       <c r="S201">
@@ -19907,7 +20473,7 @@
       </c>
       <c r="T201" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>498.25</v>
       </c>
     </row>
     <row r="202" spans="1:20" x14ac:dyDescent="0.25">
@@ -19924,9 +20490,15 @@
       <c r="D202" s="3">
         <v>0.71875</v>
       </c>
+      <c r="E202" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F202" s="2">
         <f t="shared" si="22"/>
-        <v>-0.71875</v>
+        <v>2.083333333333337E-2</v>
+      </c>
+      <c r="M202" s="4">
+        <v>0.5</v>
       </c>
       <c r="P202" s="20" t="s">
         <v>125</v>
@@ -19943,7 +20515,7 @@
       </c>
       <c r="T202" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>498.75</v>
       </c>
     </row>
     <row r="203" spans="1:20" x14ac:dyDescent="0.25">
@@ -19960,9 +20532,15 @@
       <c r="D203" s="3">
         <v>0.72916666666666663</v>
       </c>
+      <c r="E203" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F203" s="2">
         <f t="shared" si="22"/>
-        <v>-0.72916666666666663</v>
+        <v>1.0416666666666741E-2</v>
+      </c>
+      <c r="M203" s="4">
+        <v>0.25</v>
       </c>
       <c r="P203" s="20" t="s">
         <v>125</v>
@@ -19979,7 +20557,7 @@
       </c>
       <c r="T203" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>499</v>
       </c>
     </row>
     <row r="204" spans="1:20" x14ac:dyDescent="0.25">
@@ -19996,9 +20574,15 @@
       <c r="D204" s="3">
         <v>0.70833333333333337</v>
       </c>
+      <c r="E204" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F204" s="2">
         <f t="shared" si="22"/>
-        <v>-0.70833333333333337</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M204" s="4">
+        <v>0.75</v>
       </c>
       <c r="P204" s="20" t="s">
         <v>125</v>
@@ -20015,7 +20599,7 @@
       </c>
       <c r="T204" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>499.75</v>
       </c>
     </row>
     <row r="205" spans="1:20" x14ac:dyDescent="0.25">
@@ -20032,9 +20616,18 @@
       <c r="D205" s="3">
         <v>0.80208333333333337</v>
       </c>
+      <c r="E205" s="3">
+        <v>0.95833333333333337</v>
+      </c>
       <c r="F205" s="2">
         <f t="shared" si="22"/>
-        <v>-0.80208333333333337</v>
+        <v>0.15625</v>
+      </c>
+      <c r="M205" s="4">
+        <v>3.75</v>
+      </c>
+      <c r="N205" t="s">
+        <v>382</v>
       </c>
       <c r="P205" s="20" t="s">
         <v>125</v>
@@ -20051,7 +20644,7 @@
       </c>
       <c r="T205" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>503.5</v>
       </c>
     </row>
     <row r="206" spans="1:20" x14ac:dyDescent="0.25">
@@ -20068,9 +20661,15 @@
       <c r="D206" s="3">
         <v>0.58333333333333337</v>
       </c>
+      <c r="E206" s="3">
+        <v>0.72916666666666663</v>
+      </c>
       <c r="F206" s="2">
         <f t="shared" si="22"/>
-        <v>-0.58333333333333337</v>
+        <v>0.14583333333333326</v>
+      </c>
+      <c r="M206" s="4">
+        <v>3.5</v>
       </c>
       <c r="P206" s="25" t="s">
         <v>125</v>
@@ -20087,7 +20686,7 @@
       </c>
       <c r="T206" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>507</v>
       </c>
     </row>
     <row r="207" spans="1:20" x14ac:dyDescent="0.25">
@@ -20104,9 +20703,15 @@
       <c r="D207" s="3">
         <v>0.38541666666666669</v>
       </c>
+      <c r="E207" s="3">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="F207" s="2">
         <f t="shared" si="22"/>
-        <v>-0.38541666666666669</v>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="M207" s="4">
+        <v>1.75</v>
       </c>
       <c r="P207" s="20" t="s">
         <v>125</v>
@@ -20123,7 +20728,7 @@
       </c>
       <c r="T207" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>508.75</v>
       </c>
     </row>
     <row r="208" spans="1:20" x14ac:dyDescent="0.25">
@@ -20140,9 +20745,15 @@
       <c r="D208" s="3">
         <v>0.67708333333333337</v>
       </c>
+      <c r="E208" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F208" s="2">
         <f t="shared" si="22"/>
-        <v>-0.67708333333333337</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M208" s="4">
+        <v>1.5</v>
       </c>
       <c r="P208" s="20" t="s">
         <v>125</v>
@@ -20159,7 +20770,7 @@
       </c>
       <c r="T208" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>510.25</v>
       </c>
     </row>
     <row r="209" spans="1:20" x14ac:dyDescent="0.25">
@@ -20176,9 +20787,15 @@
       <c r="D209" s="3">
         <v>0.70833333333333337</v>
       </c>
+      <c r="E209" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F209" s="2">
         <f t="shared" si="22"/>
-        <v>-0.70833333333333337</v>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M209" s="4">
+        <v>0.75</v>
       </c>
       <c r="P209" s="20" t="s">
         <v>125</v>
@@ -20195,7 +20812,7 @@
       </c>
       <c r="T209" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>511</v>
       </c>
     </row>
     <row r="210" spans="1:20" x14ac:dyDescent="0.25">
@@ -20212,16 +20829,15 @@
       <c r="D210" s="3">
         <v>0.70833333333333337</v>
       </c>
+      <c r="E210" s="3">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="F210" s="2">
         <f t="shared" si="22"/>
-        <v>-0.70833333333333337</v>
-      </c>
-      <c r="G210" s="3">
-        <v>0.73958333333333337</v>
-      </c>
-      <c r="I210" s="2">
-        <f>H210-G210</f>
-        <v>-0.73958333333333337</v>
+        <v>0.11458333333333326</v>
+      </c>
+      <c r="M210" s="4">
+        <v>2.75</v>
       </c>
       <c r="N210" t="s">
         <v>359</v>
@@ -20244,7 +20860,7 @@
       </c>
       <c r="T210" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>513.75</v>
       </c>
     </row>
     <row r="211" spans="1:20" x14ac:dyDescent="0.25">
@@ -20261,16 +20877,25 @@
       <c r="D211" s="3">
         <v>0.70833333333333337</v>
       </c>
+      <c r="E211" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F211" s="2">
         <f t="shared" si="22"/>
-        <v>-0.70833333333333337</v>
+        <v>3.125E-2</v>
       </c>
       <c r="G211" s="3">
         <v>0.83333333333333337</v>
       </c>
+      <c r="H211" s="3">
+        <v>0.89583333333333337</v>
+      </c>
       <c r="I211" s="2">
         <f>H211-G211</f>
-        <v>-0.83333333333333337</v>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M211" s="4">
+        <v>2.25</v>
       </c>
       <c r="N211" t="s">
         <v>360</v>
@@ -20293,7 +20918,7 @@
       </c>
       <c r="T211" s="4">
         <f t="shared" si="21"/>
-        <v>495.25</v>
+        <v>516</v>
       </c>
     </row>
     <row r="212" spans="1:20" x14ac:dyDescent="0.25">
@@ -20341,7 +20966,7 @@
       </c>
       <c r="T212" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>516.75</v>
       </c>
     </row>
     <row r="213" spans="1:20" x14ac:dyDescent="0.25">
@@ -20358,9 +20983,15 @@
       <c r="D213" s="3">
         <v>0.54166666666666663</v>
       </c>
+      <c r="E213" s="3">
+        <v>0.6875</v>
+      </c>
       <c r="F213" s="2">
         <f t="shared" si="22"/>
-        <v>-0.54166666666666663</v>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="M213" s="4">
+        <v>3.5</v>
       </c>
       <c r="P213" s="25" t="s">
         <v>125</v>
@@ -20377,7 +21008,7 @@
       </c>
       <c r="T213" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>520.25</v>
       </c>
     </row>
     <row r="214" spans="1:20" x14ac:dyDescent="0.25">
@@ -20394,9 +21025,15 @@
       <c r="D214" s="3">
         <v>0.6875</v>
       </c>
+      <c r="E214" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F214" s="2">
         <f t="shared" si="22"/>
-        <v>-0.6875</v>
+        <v>5.208333333333337E-2</v>
+      </c>
+      <c r="M214" s="4">
+        <v>1.25</v>
       </c>
       <c r="P214" s="25" t="s">
         <v>125</v>
@@ -20413,7 +21050,7 @@
       </c>
       <c r="T214" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>521.5</v>
       </c>
     </row>
     <row r="215" spans="1:20" x14ac:dyDescent="0.25">
@@ -20430,9 +21067,15 @@
       <c r="D215" s="3">
         <v>0.6875</v>
       </c>
+      <c r="E215" s="3">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="F215" s="2">
         <f t="shared" si="22"/>
-        <v>-0.6875</v>
+        <v>0.13541666666666663</v>
+      </c>
+      <c r="M215" s="4">
+        <v>3.25</v>
       </c>
       <c r="P215" s="25" t="s">
         <v>125</v>
@@ -20449,7 +21092,7 @@
       </c>
       <c r="T215" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>524.75</v>
       </c>
     </row>
     <row r="216" spans="1:20" x14ac:dyDescent="0.25">
@@ -20466,12 +21109,25 @@
       <c r="D216" s="3">
         <v>0.6875</v>
       </c>
+      <c r="E216" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F216" s="2">
         <f t="shared" si="22"/>
-        <v>-0.6875</v>
+        <v>5.208333333333337E-2</v>
       </c>
       <c r="G216" s="3">
         <v>0.8125</v>
+      </c>
+      <c r="H216" s="3">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="I216" s="2">
+        <f t="shared" ref="I216" si="24">H216-G216</f>
+        <v>0.10416666666666663</v>
+      </c>
+      <c r="M216" s="4">
+        <v>3.75</v>
       </c>
       <c r="P216" s="25" t="s">
         <v>125</v>
@@ -20488,7 +21144,7 @@
       </c>
       <c r="T216" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>528.5</v>
       </c>
     </row>
     <row r="217" spans="1:20" x14ac:dyDescent="0.25">
@@ -20505,9 +21161,15 @@
       <c r="D217" s="3">
         <v>0.80208333333333337</v>
       </c>
+      <c r="E217" s="3">
+        <v>0.88541666666666663</v>
+      </c>
       <c r="F217" s="2">
         <f t="shared" si="22"/>
-        <v>-0.80208333333333337</v>
+        <v>8.3333333333333259E-2</v>
+      </c>
+      <c r="M217" s="4">
+        <v>2</v>
       </c>
       <c r="P217" s="25" t="s">
         <v>125</v>
@@ -20524,7 +21186,7 @@
       </c>
       <c r="T217" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>530.5</v>
       </c>
     </row>
     <row r="218" spans="1:20" x14ac:dyDescent="0.25">
@@ -20541,9 +21203,15 @@
       <c r="D218" s="3">
         <v>0.64583333333333337</v>
       </c>
+      <c r="E218" s="3">
+        <v>0.73958333333333337</v>
+      </c>
       <c r="F218" s="2">
         <f t="shared" si="22"/>
-        <v>-0.64583333333333337</v>
+        <v>9.375E-2</v>
+      </c>
+      <c r="M218" s="4">
+        <v>2.25</v>
       </c>
       <c r="P218" s="25" t="s">
         <v>125</v>
@@ -20560,7 +21228,7 @@
       </c>
       <c r="T218" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>532.75</v>
       </c>
     </row>
     <row r="219" spans="1:20" x14ac:dyDescent="0.25">
@@ -20577,9 +21245,15 @@
       <c r="D219" s="3">
         <v>0.66666666666666663</v>
       </c>
+      <c r="E219" s="3">
+        <v>0.82291666666666663</v>
+      </c>
       <c r="F219" s="2">
         <f t="shared" si="22"/>
-        <v>-0.66666666666666663</v>
+        <v>0.15625</v>
+      </c>
+      <c r="M219" s="4">
+        <v>3.75</v>
       </c>
       <c r="N219" t="s">
         <v>362</v>
@@ -20602,159 +21276,1156 @@
       </c>
       <c r="T219" s="4">
         <f t="shared" si="21"/>
-        <v>496</v>
+        <v>536.5</v>
       </c>
     </row>
     <row r="220" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B220"/>
-      <c r="C220"/>
+      <c r="A220" t="s">
+        <v>0</v>
+      </c>
+      <c r="B220" s="1">
+        <v>43573</v>
+      </c>
+      <c r="C220" s="5">
+        <f t="shared" si="20"/>
+        <v>43573</v>
+      </c>
+      <c r="D220" s="3">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="E220" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="F220" s="2">
+        <f t="shared" si="22"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="M220" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="P220" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q220">
+        <v>9</v>
+      </c>
+      <c r="R220" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S220">
+        <v>3</v>
+      </c>
+      <c r="T220" s="4">
+        <f t="shared" si="21"/>
+        <v>538.25</v>
+      </c>
     </row>
     <row r="221" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B221"/>
-      <c r="C221"/>
+      <c r="A221" t="s">
+        <v>1</v>
+      </c>
+      <c r="B221" s="1">
+        <v>43574</v>
+      </c>
+      <c r="C221" s="5">
+        <f t="shared" si="20"/>
+        <v>43574</v>
+      </c>
+      <c r="D221" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E221" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="F221" s="2">
+        <f t="shared" si="22"/>
+        <v>4.1666666666666685E-2</v>
+      </c>
+      <c r="M221" s="4">
+        <v>1</v>
+      </c>
+      <c r="P221" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q221">
+        <v>9</v>
+      </c>
+      <c r="R221" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S221">
+        <v>3</v>
+      </c>
+      <c r="T221" s="4">
+        <f t="shared" si="21"/>
+        <v>539.25</v>
+      </c>
     </row>
     <row r="222" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B222"/>
-      <c r="C222"/>
+      <c r="A222" t="s">
+        <v>2</v>
+      </c>
+      <c r="B222" s="1">
+        <v>43575</v>
+      </c>
+      <c r="C222" s="5">
+        <f t="shared" si="20"/>
+        <v>43575</v>
+      </c>
+      <c r="D222" s="3">
+        <v>0.46875</v>
+      </c>
+      <c r="E222" s="3">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="F222" s="2">
+        <f t="shared" si="22"/>
+        <v>1.0416666666666685E-2</v>
+      </c>
+      <c r="G222" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="H222" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="I222" s="2">
+        <f t="shared" ref="I222" si="25">H222-G222</f>
+        <v>0.125</v>
+      </c>
+      <c r="M222" s="4">
+        <v>3.25</v>
+      </c>
+      <c r="P222" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q222">
+        <v>9</v>
+      </c>
+      <c r="R222" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S222">
+        <v>3</v>
+      </c>
+      <c r="T222" s="4">
+        <f t="shared" si="21"/>
+        <v>542.5</v>
+      </c>
     </row>
     <row r="223" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B223"/>
-      <c r="C223"/>
+      <c r="A223" t="s">
+        <v>3</v>
+      </c>
+      <c r="B223" s="1">
+        <v>43576</v>
+      </c>
+      <c r="C223" s="5">
+        <f t="shared" si="20"/>
+        <v>43576</v>
+      </c>
+      <c r="D223" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E223" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="F223" s="2">
+        <f t="shared" si="22"/>
+        <v>0.11458333333333337</v>
+      </c>
+      <c r="M223" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="P223" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q223">
+        <v>9</v>
+      </c>
+      <c r="R223" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S223">
+        <v>3</v>
+      </c>
+      <c r="T223" s="4">
+        <f t="shared" si="21"/>
+        <v>545.25</v>
+      </c>
     </row>
     <row r="224" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B224"/>
-      <c r="C224"/>
-    </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B225"/>
-      <c r="C225"/>
-    </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B226"/>
-      <c r="C226"/>
-    </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B227"/>
-      <c r="C227"/>
-    </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B228"/>
-      <c r="C228"/>
-    </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229"/>
-      <c r="C229"/>
-    </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B230"/>
-      <c r="C230"/>
-    </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231"/>
-      <c r="C231"/>
-    </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B232"/>
-      <c r="C232"/>
+      <c r="A224" t="s">
+        <v>10</v>
+      </c>
+      <c r="B224" s="1">
+        <v>43577</v>
+      </c>
+      <c r="C224" s="5">
+        <f t="shared" si="20"/>
+        <v>43577</v>
+      </c>
+      <c r="D224" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E224" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F224" s="2">
+        <f t="shared" si="22"/>
+        <v>3.125E-2</v>
+      </c>
+      <c r="M224" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="P224" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q224">
+        <v>9</v>
+      </c>
+      <c r="R224" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S224">
+        <v>3</v>
+      </c>
+      <c r="T224" s="4">
+        <f t="shared" si="21"/>
+        <v>546</v>
+      </c>
+    </row>
+    <row r="225" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>67</v>
+      </c>
+      <c r="B225" s="1">
+        <v>43578</v>
+      </c>
+      <c r="C225" s="5">
+        <f t="shared" si="20"/>
+        <v>43578</v>
+      </c>
+      <c r="D225" s="3">
+        <v>0.67708333333333337</v>
+      </c>
+      <c r="E225" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F225" s="2">
+        <f t="shared" si="22"/>
+        <v>6.25E-2</v>
+      </c>
+      <c r="M225" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="P225" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q225">
+        <v>9</v>
+      </c>
+      <c r="R225" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S225">
+        <v>3</v>
+      </c>
+      <c r="T225" s="4">
+        <f t="shared" si="21"/>
+        <v>547.5</v>
+      </c>
+    </row>
+    <row r="226" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>0</v>
+      </c>
+      <c r="B226" s="1">
+        <v>43580</v>
+      </c>
+      <c r="C226" s="5">
+        <f t="shared" si="20"/>
+        <v>43580</v>
+      </c>
+      <c r="D226" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E226" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F226" s="2">
+        <f t="shared" si="22"/>
+        <v>0.16666666666666663</v>
+      </c>
+      <c r="M226" s="4">
+        <v>4</v>
+      </c>
+      <c r="P226" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q226">
+        <v>9</v>
+      </c>
+      <c r="R226" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S226">
+        <v>3</v>
+      </c>
+      <c r="T226" s="4">
+        <f t="shared" si="21"/>
+        <v>551.5</v>
+      </c>
+    </row>
+    <row r="227" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>1</v>
+      </c>
+      <c r="B227" s="1">
+        <v>43581</v>
+      </c>
+      <c r="C227" s="5">
+        <f t="shared" si="20"/>
+        <v>43581</v>
+      </c>
+      <c r="D227" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="E227" s="3">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="F227" s="2">
+        <f t="shared" si="22"/>
+        <v>7.291666666666663E-2</v>
+      </c>
+      <c r="M227" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="P227" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q227">
+        <v>9</v>
+      </c>
+      <c r="R227" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S227">
+        <v>3</v>
+      </c>
+      <c r="T227" s="4">
+        <f t="shared" si="21"/>
+        <v>553.25</v>
+      </c>
+    </row>
+    <row r="228" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>2</v>
+      </c>
+      <c r="B228" s="1">
+        <v>43582</v>
+      </c>
+      <c r="C228" s="5">
+        <f t="shared" ref="C228:C242" si="26">B228</f>
+        <v>43582</v>
+      </c>
+      <c r="D228" s="3">
+        <v>0.5625</v>
+      </c>
+      <c r="E228" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F228" s="2">
+        <f t="shared" si="22"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="M228" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="P228" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q228">
+        <v>9</v>
+      </c>
+      <c r="R228" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S228">
+        <v>3</v>
+      </c>
+      <c r="T228" s="4">
+        <f t="shared" si="21"/>
+        <v>556.75</v>
+      </c>
+    </row>
+    <row r="229" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>10</v>
+      </c>
+      <c r="B229" s="1">
+        <v>43584</v>
+      </c>
+      <c r="C229" s="5">
+        <f t="shared" si="26"/>
+        <v>43584</v>
+      </c>
+      <c r="D229" s="3">
+        <v>0.65625</v>
+      </c>
+      <c r="E229" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F229" s="2">
+        <f t="shared" si="22"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="M229" s="4">
+        <v>2</v>
+      </c>
+      <c r="P229" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q229">
+        <v>9</v>
+      </c>
+      <c r="R229" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S229">
+        <v>3</v>
+      </c>
+      <c r="T229" s="4">
+        <f t="shared" si="21"/>
+        <v>558.75</v>
+      </c>
+    </row>
+    <row r="230" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>67</v>
+      </c>
+      <c r="B230" s="1">
+        <v>43585</v>
+      </c>
+      <c r="C230" s="5">
+        <f t="shared" si="26"/>
+        <v>43585</v>
+      </c>
+      <c r="D230" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E230" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="F230" s="2">
+        <f t="shared" si="22"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="M230" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="P230" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q230">
+        <v>9</v>
+      </c>
+      <c r="R230" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S230">
+        <v>3</v>
+      </c>
+      <c r="T230" s="4">
+        <f t="shared" si="21"/>
+        <v>560.5</v>
+      </c>
+    </row>
+    <row r="231" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>35</v>
+      </c>
+      <c r="B231" s="1">
+        <v>43586</v>
+      </c>
+      <c r="C231" s="5">
+        <f t="shared" si="26"/>
+        <v>43586</v>
+      </c>
+      <c r="D231" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E231" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F231" s="2">
+        <f t="shared" si="22"/>
+        <v>2.0833333333333259E-2</v>
+      </c>
+      <c r="M231" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="N231" t="s">
+        <v>380</v>
+      </c>
+      <c r="P231" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q231">
+        <v>9</v>
+      </c>
+      <c r="R231" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S231">
+        <v>3</v>
+      </c>
+      <c r="T231" s="4">
+        <f t="shared" si="21"/>
+        <v>561</v>
+      </c>
+    </row>
+    <row r="232" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>0</v>
+      </c>
+      <c r="B232" s="1">
+        <v>43587</v>
+      </c>
+      <c r="C232" s="5">
+        <f t="shared" si="26"/>
+        <v>43587</v>
+      </c>
+      <c r="D232" s="3">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="E232" s="3">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="F232" s="2">
+        <f t="shared" si="22"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="M232" s="4">
+        <v>1</v>
+      </c>
+      <c r="N232" t="s">
+        <v>379</v>
+      </c>
+      <c r="O232" s="4"/>
+      <c r="P232" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q232">
+        <v>9</v>
+      </c>
+      <c r="R232" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S232">
+        <v>3</v>
+      </c>
+      <c r="T232" s="4">
+        <f t="shared" si="21"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="233" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>1</v>
+      </c>
+      <c r="B233" s="1">
+        <v>43588</v>
+      </c>
+      <c r="C233" s="5">
+        <f t="shared" si="26"/>
+        <v>43588</v>
+      </c>
+      <c r="D233" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E233" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F233" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="N233" t="s">
+        <v>369</v>
+      </c>
+      <c r="P233" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q233">
+        <v>9</v>
+      </c>
+      <c r="R233" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S233">
+        <v>3</v>
+      </c>
+      <c r="T233" s="4">
+        <f t="shared" si="21"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="234" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>2</v>
+      </c>
+      <c r="B234" s="1">
+        <v>43589</v>
+      </c>
+      <c r="C234" s="5">
+        <f t="shared" si="26"/>
+        <v>43589</v>
+      </c>
+      <c r="D234" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F234" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="N234" t="s">
+        <v>370</v>
+      </c>
+      <c r="O234" s="4"/>
+      <c r="P234" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q234">
+        <v>9</v>
+      </c>
+      <c r="R234" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S234">
+        <v>3</v>
+      </c>
+      <c r="T234" s="4">
+        <f t="shared" si="21"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="235" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>3</v>
+      </c>
+      <c r="B235" s="1">
+        <v>43590</v>
+      </c>
+      <c r="C235" s="5">
+        <f t="shared" si="26"/>
+        <v>43590</v>
+      </c>
+      <c r="D235" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E235" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="F235" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="N235" t="s">
+        <v>368</v>
+      </c>
+      <c r="P235" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q235">
+        <v>9</v>
+      </c>
+      <c r="R235" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S235">
+        <v>3</v>
+      </c>
+      <c r="T235" s="4">
+        <f t="shared" si="21"/>
+        <v>562</v>
+      </c>
+    </row>
+    <row r="236" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>67</v>
+      </c>
+      <c r="B236" s="1">
+        <v>43592</v>
+      </c>
+      <c r="C236" s="5">
+        <f t="shared" si="26"/>
+        <v>43592</v>
+      </c>
+      <c r="D236" s="3">
+        <v>0.6875</v>
+      </c>
+      <c r="E236" s="3">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="F236" s="2">
+        <f t="shared" si="22"/>
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="G236" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="M236" s="4">
+        <v>1</v>
+      </c>
+      <c r="N236" t="s">
+        <v>372</v>
+      </c>
+      <c r="O236" s="4"/>
+      <c r="P236" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q236">
+        <v>9</v>
+      </c>
+      <c r="R236" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S236">
+        <v>3</v>
+      </c>
+      <c r="T236" s="4">
+        <f t="shared" si="21"/>
+        <v>563</v>
+      </c>
+    </row>
+    <row r="237" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>0</v>
+      </c>
+      <c r="B237" s="1">
+        <v>43594</v>
+      </c>
+      <c r="C237" s="5">
+        <f t="shared" si="26"/>
+        <v>43594</v>
+      </c>
+      <c r="D237" s="3">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="E237" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="F237" s="2">
+        <f t="shared" si="22"/>
+        <v>5.2083333333333259E-2</v>
+      </c>
+      <c r="M237" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="N237" t="s">
+        <v>377</v>
+      </c>
+      <c r="P237" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q237">
+        <v>9</v>
+      </c>
+      <c r="R237" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S237">
+        <v>3</v>
+      </c>
+      <c r="T237" s="4">
+        <f t="shared" si="21"/>
+        <v>564.25</v>
+      </c>
+    </row>
+    <row r="238" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>1</v>
+      </c>
+      <c r="B238" s="1">
+        <v>43595</v>
+      </c>
+      <c r="C238" s="5">
+        <f t="shared" si="26"/>
+        <v>43595</v>
+      </c>
+      <c r="D238" s="3">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="E238" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F238" s="2">
+        <f t="shared" si="22"/>
+        <v>8.333333333333337E-2</v>
+      </c>
+      <c r="M238" s="4">
+        <v>2</v>
+      </c>
+      <c r="N238" t="s">
+        <v>373</v>
+      </c>
+      <c r="O238" s="4"/>
+      <c r="P238" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q238">
+        <v>9</v>
+      </c>
+      <c r="R238" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S238">
+        <v>3</v>
+      </c>
+      <c r="T238" s="4">
+        <f t="shared" si="21"/>
+        <v>566.25</v>
+      </c>
+    </row>
+    <row r="239" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>35</v>
+      </c>
+      <c r="B239" s="1">
+        <v>43600</v>
+      </c>
+      <c r="C239" s="5">
+        <f t="shared" si="26"/>
+        <v>43600</v>
+      </c>
+      <c r="D239" s="3">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E239" s="3">
+        <v>0.8125</v>
+      </c>
+      <c r="F239" s="2">
+        <f t="shared" si="22"/>
+        <v>0.14583333333333337</v>
+      </c>
+      <c r="M239" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="N239" t="s">
+        <v>376</v>
+      </c>
+      <c r="P239" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q239">
+        <v>9</v>
+      </c>
+      <c r="R239" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S239">
+        <v>3</v>
+      </c>
+      <c r="T239" s="4">
+        <f t="shared" si="21"/>
+        <v>569.75</v>
+      </c>
+    </row>
+    <row r="240" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>0</v>
+      </c>
+      <c r="B240" s="1">
+        <v>43601</v>
+      </c>
+      <c r="C240" s="5">
+        <f t="shared" si="26"/>
+        <v>43601</v>
+      </c>
+      <c r="D240" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="E240" s="3">
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="F240" s="2">
+        <f t="shared" si="22"/>
+        <v>0.1875</v>
+      </c>
+      <c r="M240" s="4">
+        <v>4.5</v>
+      </c>
+      <c r="N240" t="s">
+        <v>378</v>
+      </c>
+      <c r="O240" s="4"/>
+      <c r="P240" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q240">
+        <v>9</v>
+      </c>
+      <c r="R240" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S240">
+        <v>3</v>
+      </c>
+      <c r="T240" s="4">
+        <f t="shared" si="21"/>
+        <v>574.25</v>
+      </c>
+    </row>
+    <row r="241" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>1</v>
+      </c>
+      <c r="B241" s="1">
+        <v>43602</v>
+      </c>
+      <c r="C241" s="5">
+        <f t="shared" si="26"/>
+        <v>43602</v>
+      </c>
+      <c r="D241" s="3">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E241" s="3">
+        <v>0.875</v>
+      </c>
+      <c r="F241" s="2">
+        <f t="shared" si="22"/>
+        <v>0.11458333333333337</v>
+      </c>
+      <c r="M241" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="N241" t="s">
+        <v>374</v>
+      </c>
+      <c r="P241" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q241">
+        <v>9</v>
+      </c>
+      <c r="R241" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S241">
+        <v>3</v>
+      </c>
+      <c r="T241" s="4">
+        <f t="shared" si="21"/>
+        <v>577</v>
+      </c>
+    </row>
+    <row r="242" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>2</v>
+      </c>
+      <c r="B242" s="1">
+        <v>43603</v>
+      </c>
+      <c r="C242" s="5">
+        <f t="shared" si="26"/>
+        <v>43603</v>
+      </c>
+      <c r="D242" s="3">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="E242" s="3">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="F242" s="2">
+        <f t="shared" si="22"/>
+        <v>7.2916666666666741E-2</v>
+      </c>
+      <c r="M242" s="4">
+        <v>1.75</v>
+      </c>
+      <c r="N242" t="s">
+        <v>375</v>
+      </c>
+      <c r="O242" s="4"/>
+      <c r="P242" s="25" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q242">
+        <v>9</v>
+      </c>
+      <c r="R242" t="str">
+        <f t="shared" si="23"/>
+        <v>Dance 3</v>
+      </c>
+      <c r="S242">
+        <v>3</v>
+      </c>
+      <c r="T242" s="4">
+        <f t="shared" si="21"/>
+        <v>578.75</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T200 A220:T512 A213:O219 P207:P219 Q201:T219">
+  <conditionalFormatting sqref="O104 A104:M104 A98:O103 A2:T97 P98:T98 A105:O109 Q99:T109 Q110:Q116 A110:F119 P111 G110:O116 G117:Q119 A120:Q120 L122:O122 A123:D128 F127:G128 A129:P130 R110:T119 A122:I122 F123:M126 I127:M128 A121:O121 Q121:Q130 P121:P125 R120:S130 O123:O128 A131:S137 T120:T137 A138:T200 A231:N242 Q201:T235 P207:P235 A243:T501 P236:T242 A213:O230">
+    <cfRule type="expression" dxfId="27" priority="44">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N104">
+    <cfRule type="expression" dxfId="26" priority="43">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P99:P100">
+    <cfRule type="expression" dxfId="25" priority="42">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P101:P102">
+    <cfRule type="expression" dxfId="24" priority="41">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P103:P104">
+    <cfRule type="expression" dxfId="23" priority="40">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P105:P106">
+    <cfRule type="expression" dxfId="22" priority="39">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P107:P108">
+    <cfRule type="expression" dxfId="21" priority="38">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P109:P110">
+    <cfRule type="expression" dxfId="20" priority="37">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P112">
     <cfRule type="expression" dxfId="19" priority="35">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N104">
+  <conditionalFormatting sqref="P113:P114">
     <cfRule type="expression" dxfId="18" priority="34">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P99:P100">
-    <cfRule type="expression" dxfId="17" priority="33">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P101:P102">
-    <cfRule type="expression" dxfId="16" priority="32">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P103:P104">
-    <cfRule type="expression" dxfId="15" priority="31">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P105:P106">
-    <cfRule type="expression" dxfId="14" priority="30">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P107:P108">
-    <cfRule type="expression" dxfId="13" priority="29">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P109:P110">
-    <cfRule type="expression" dxfId="12" priority="28">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P112">
-    <cfRule type="expression" dxfId="11" priority="26">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P113:P114">
-    <cfRule type="expression" dxfId="10" priority="25">
-      <formula>MOD(ROW(), 2) = 0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="P115:P116">
-    <cfRule type="expression" dxfId="9" priority="23">
+    <cfRule type="expression" dxfId="17" priority="32">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P126:P128">
-    <cfRule type="expression" dxfId="8" priority="18">
+    <cfRule type="expression" dxfId="16" priority="27">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E124">
-    <cfRule type="expression" dxfId="7" priority="11">
+    <cfRule type="expression" dxfId="15" priority="20">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E126">
+    <cfRule type="expression" dxfId="14" priority="16">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E125">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H127">
+    <cfRule type="expression" dxfId="12" priority="15">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H128">
+    <cfRule type="expression" dxfId="11" priority="14">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N123:N128">
+    <cfRule type="expression" dxfId="10" priority="13">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H209:O209 A201:F201 G210:O212 G201:O208 A209:F212 A208:D208 F208 A203:F207 A202:D202 F202">
+    <cfRule type="expression" dxfId="9" priority="12">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P201:P206">
+    <cfRule type="expression" dxfId="8" priority="11">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O232">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>MOD(ROW(), 2) = 0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O234">
     <cfRule type="expression" dxfId="6" priority="7">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E125">
-    <cfRule type="expression" dxfId="5" priority="8">
+  <conditionalFormatting sqref="O236">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H127">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="O238">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H128">
-    <cfRule type="expression" dxfId="3" priority="5">
+  <conditionalFormatting sqref="O240">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N123:N128">
-    <cfRule type="expression" dxfId="2" priority="4">
+  <conditionalFormatting sqref="O242">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H209:O209 A201:F212 G210:O212 G201:O208">
-    <cfRule type="expression" dxfId="1" priority="3">
+  <conditionalFormatting sqref="E208">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P201:P206">
-    <cfRule type="expression" dxfId="0" priority="2">
+  <conditionalFormatting sqref="E202">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(), 2) = 0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20936,7 +22607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
@@ -21146,7 +22817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:H84"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>

</xml_diff>